<commit_message>
Added Hi, lo registers and control signals to excel file
</commit_message>
<xml_diff>
--- a/LAB8-11/DatapathComponents/ALU_mapping.xlsx
+++ b/LAB8-11/DatapathComponents/ALU_mapping.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dennis/Documents/2017FALL/ECE369A/lab369a/LAB8-11/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ryan\Documents\ECE369a\lab369a\LAB8-11\DatapathComponents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="880" yWindow="460" windowWidth="24720" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="1815" yWindow="465" windowWidth="24720" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="207">
   <si>
     <t>Type</t>
   </si>
@@ -597,13 +597,68 @@
   </si>
   <si>
     <t>STOPPED HERE</t>
+  </si>
+  <si>
+    <t>Control Signals:</t>
+  </si>
+  <si>
+    <t>ZeroExtend</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>ALUSrc</t>
+  </si>
+  <si>
+    <t>RegDst</t>
+  </si>
+  <si>
+    <t>ALUControl</t>
+  </si>
+  <si>
+    <t>MemWrite</t>
+  </si>
+  <si>
+    <t>MemRead</t>
+  </si>
+  <si>
+    <t>MemToReg</t>
+  </si>
+  <si>
+    <t>RegWrite</t>
+  </si>
+  <si>
+    <t>hi_read</t>
+  </si>
+  <si>
+    <t>hi_write</t>
+  </si>
+  <si>
+    <t>lo_read</t>
+  </si>
+  <si>
+    <t>lo_write</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Don't worry for this lab</t>
+  </si>
+  <si>
+    <t>DepRegWrite</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="00"/>
+    <numFmt numFmtId="166" formatCode="0000"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -612,22 +667,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -645,8 +689,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -689,8 +765,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -770,98 +858,163 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="9" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="9" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="8" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="9" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
+    <cellStyle name="20% - Accent3" xfId="9" builtinId="38"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -877,6 +1030,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1144,64 +1300,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AC55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="8"/>
+    <col min="2" max="2" width="32.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="11" style="8"/>
+    <col min="12" max="12" width="20.25" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="30"/>
+    <col min="14" max="14" width="6.875" style="33" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.875" style="44" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" style="33" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.125" style="33" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.625" style="33" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.75" style="33" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" style="33" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.625" style="33" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="4.875" style="33" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.875" style="33" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.375" style="41" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.875" style="33" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="16" t="s">
+    <row r="1" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="7" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="L1" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="N1" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="O1" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="P1" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q1" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="R1" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="S1" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="T1" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="U1" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="V1" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z1" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="AA1" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="AB1" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="12" t="s">
         <v>127</v>
       </c>
       <c r="E2" s="13" t="s">
@@ -1219,20 +1450,72 @@
       <c r="I2" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="L2" s="24"/>
-    </row>
-    <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="L2" s="16"/>
+      <c r="M2" s="31">
+        <v>0</v>
+      </c>
+      <c r="N2" s="34">
+        <v>0</v>
+      </c>
+      <c r="O2" s="43">
+        <v>1</v>
+      </c>
+      <c r="P2" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="38" t="str">
+        <f>K2</f>
+        <v>0000</v>
+      </c>
+      <c r="R2" s="34">
+        <v>0</v>
+      </c>
+      <c r="S2" s="34">
+        <v>0</v>
+      </c>
+      <c r="T2" s="34">
+        <v>0</v>
+      </c>
+      <c r="U2" s="34">
+        <v>1</v>
+      </c>
+      <c r="V2" s="34">
+        <v>0</v>
+      </c>
+      <c r="W2" s="34">
+        <v>0</v>
+      </c>
+      <c r="X2" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="34">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="13" t="s">
@@ -1244,29 +1527,81 @@
       <c r="F3" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="L3" s="24"/>
-    </row>
-    <row r="4" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+      <c r="L3" s="16"/>
+      <c r="M3" s="30">
+        <v>0</v>
+      </c>
+      <c r="N3" s="33">
+        <v>0</v>
+      </c>
+      <c r="O3" s="47">
+        <v>1</v>
+      </c>
+      <c r="P3" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="39" t="str">
+        <f t="shared" ref="Q3:Q54" si="0">K3</f>
+        <v>0000</v>
+      </c>
+      <c r="R3" s="33">
+        <v>0</v>
+      </c>
+      <c r="S3" s="33">
+        <v>0</v>
+      </c>
+      <c r="T3" s="33">
+        <v>0</v>
+      </c>
+      <c r="U3" s="33">
+        <v>1</v>
+      </c>
+      <c r="V3" s="33">
+        <v>0</v>
+      </c>
+      <c r="W3" s="33">
+        <v>0</v>
+      </c>
+      <c r="X3" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="33">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="33">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="13" t="s">
@@ -1287,20 +1622,72 @@
       <c r="I4" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="23" t="s">
+      <c r="K4" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="L4" s="24"/>
-    </row>
-    <row r="5" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2" t="s">
+      <c r="L4" s="16"/>
+      <c r="M4" s="31">
+        <v>0</v>
+      </c>
+      <c r="N4" s="34">
+        <v>0</v>
+      </c>
+      <c r="O4" s="43">
+        <v>1</v>
+      </c>
+      <c r="P4" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="R4" s="34">
+        <v>0</v>
+      </c>
+      <c r="S4" s="34">
+        <v>0</v>
+      </c>
+      <c r="T4" s="34">
+        <v>0</v>
+      </c>
+      <c r="U4" s="34">
+        <v>1</v>
+      </c>
+      <c r="V4" s="34">
+        <v>0</v>
+      </c>
+      <c r="W4" s="34">
+        <v>0</v>
+      </c>
+      <c r="X4" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="34">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="13" t="s">
@@ -1312,29 +1699,81 @@
       <c r="F5" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="L5" s="24"/>
-    </row>
-    <row r="6" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2" t="s">
+      <c r="L5" s="16"/>
+      <c r="M5" s="30">
+        <v>0</v>
+      </c>
+      <c r="N5" s="33">
+        <v>0</v>
+      </c>
+      <c r="O5" s="47">
+        <v>1</v>
+      </c>
+      <c r="P5" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q5" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0010</v>
+      </c>
+      <c r="R5" s="33">
+        <v>0</v>
+      </c>
+      <c r="S5" s="33">
+        <v>0</v>
+      </c>
+      <c r="T5" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="U5" s="33">
+        <v>0</v>
+      </c>
+      <c r="V5" s="33">
+        <v>0</v>
+      </c>
+      <c r="W5" s="33">
+        <v>0</v>
+      </c>
+      <c r="X5" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="33">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="33">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="13" t="s">
@@ -1355,22 +1794,74 @@
       <c r="I6" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="J6" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="K6" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="L6" s="24"/>
-    </row>
-    <row r="7" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="L6" s="16"/>
+      <c r="M6" s="31">
+        <v>0</v>
+      </c>
+      <c r="N6" s="34">
+        <v>0</v>
+      </c>
+      <c r="O6" s="43">
+        <v>1</v>
+      </c>
+      <c r="P6" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q6" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>0011</v>
+      </c>
+      <c r="R6" s="34">
+        <v>0</v>
+      </c>
+      <c r="S6" s="34">
+        <v>0</v>
+      </c>
+      <c r="T6" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="U6" s="34">
+        <v>0</v>
+      </c>
+      <c r="V6" s="34">
+        <v>0</v>
+      </c>
+      <c r="W6" s="34">
+        <v>0</v>
+      </c>
+      <c r="X6" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="34">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="34">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="19" t="s">
         <v>68</v>
       </c>
       <c r="D7" s="13" t="s">
@@ -1391,20 +1882,72 @@
       <c r="I7" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="J7" s="28" t="s">
+      <c r="J7" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="K7" s="23" t="s">
+      <c r="K7" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="L7" s="24"/>
-    </row>
-    <row r="8" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="7" t="s">
+      <c r="L7" s="16"/>
+      <c r="M7" s="30">
+        <v>0</v>
+      </c>
+      <c r="N7" s="33">
+        <v>0</v>
+      </c>
+      <c r="O7" s="47">
+        <v>1</v>
+      </c>
+      <c r="P7" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0110</v>
+      </c>
+      <c r="R7" s="33">
+        <v>0</v>
+      </c>
+      <c r="S7" s="33">
+        <v>0</v>
+      </c>
+      <c r="T7" s="33">
+        <v>0</v>
+      </c>
+      <c r="U7" s="33">
+        <v>1</v>
+      </c>
+      <c r="V7" s="33">
+        <v>0</v>
+      </c>
+      <c r="W7" s="33">
+        <v>0</v>
+      </c>
+      <c r="X7" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="33">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="33">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="19" t="s">
         <v>72</v>
       </c>
       <c r="D8" s="13" t="s">
@@ -1425,88 +1968,244 @@
       <c r="I8" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="J8" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="L8" s="24"/>
-    </row>
-    <row r="9" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="7" t="s">
+      <c r="L8" s="16"/>
+      <c r="M8" s="31">
+        <v>0</v>
+      </c>
+      <c r="N8" s="34">
+        <v>0</v>
+      </c>
+      <c r="O8" s="43">
+        <v>1</v>
+      </c>
+      <c r="P8" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>0111</v>
+      </c>
+      <c r="R8" s="34">
+        <v>0</v>
+      </c>
+      <c r="S8" s="34">
+        <v>0</v>
+      </c>
+      <c r="T8" s="34">
+        <v>0</v>
+      </c>
+      <c r="U8" s="34">
+        <v>1</v>
+      </c>
+      <c r="V8" s="34">
+        <v>0</v>
+      </c>
+      <c r="W8" s="34">
+        <v>0</v>
+      </c>
+      <c r="X8" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="34">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="L9" s="24"/>
-    </row>
-    <row r="10" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="7" t="s">
+      <c r="L9" s="16"/>
+      <c r="M9" s="30">
+        <v>0</v>
+      </c>
+      <c r="N9" s="33">
+        <v>0</v>
+      </c>
+      <c r="O9" s="47">
+        <v>1</v>
+      </c>
+      <c r="P9" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="R9" s="33">
+        <v>0</v>
+      </c>
+      <c r="S9" s="33">
+        <v>0</v>
+      </c>
+      <c r="T9" s="33">
+        <v>0</v>
+      </c>
+      <c r="U9" s="33">
+        <v>1</v>
+      </c>
+      <c r="V9" s="33">
+        <v>0</v>
+      </c>
+      <c r="W9" s="33">
+        <v>0</v>
+      </c>
+      <c r="X9" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="33">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="33">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="19" t="s">
         <v>74</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J10" s="28" t="s">
+      <c r="J10" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="23" t="s">
+      <c r="K10" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="L10" s="24"/>
-    </row>
-    <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="7" t="s">
+      <c r="L10" s="16"/>
+      <c r="M10" s="31">
+        <v>0</v>
+      </c>
+      <c r="N10" s="34">
+        <v>0</v>
+      </c>
+      <c r="O10" s="43">
+        <v>1</v>
+      </c>
+      <c r="P10" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>1001</v>
+      </c>
+      <c r="R10" s="34">
+        <v>0</v>
+      </c>
+      <c r="S10" s="34">
+        <v>0</v>
+      </c>
+      <c r="T10" s="34">
+        <v>0</v>
+      </c>
+      <c r="U10" s="34">
+        <v>1</v>
+      </c>
+      <c r="V10" s="34">
+        <v>0</v>
+      </c>
+      <c r="W10" s="34">
+        <v>0</v>
+      </c>
+      <c r="X10" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="34">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="19" t="s">
         <v>84</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -1518,29 +2217,81 @@
       <c r="F11" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="K11" s="23" t="s">
+      <c r="K11" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="L11" s="24"/>
-    </row>
-    <row r="12" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="7" t="s">
+      <c r="L11" s="16"/>
+      <c r="M11" s="30">
+        <v>1</v>
+      </c>
+      <c r="N11" s="48">
+        <v>0</v>
+      </c>
+      <c r="O11" s="47">
+        <v>1</v>
+      </c>
+      <c r="P11" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>1010</v>
+      </c>
+      <c r="R11" s="48">
+        <v>0</v>
+      </c>
+      <c r="S11" s="48">
+        <v>0</v>
+      </c>
+      <c r="T11" s="48">
+        <v>0</v>
+      </c>
+      <c r="U11" s="48">
+        <v>1</v>
+      </c>
+      <c r="V11" s="48">
+        <v>0</v>
+      </c>
+      <c r="W11" s="48">
+        <v>0</v>
+      </c>
+      <c r="X11" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="19" t="s">
         <v>88</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -1552,29 +2303,81 @@
       <c r="F12" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="J12" s="28" t="s">
+      <c r="J12" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="K12" s="23" t="s">
+      <c r="K12" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="L12" s="24"/>
-    </row>
-    <row r="13" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="7" t="s">
+      <c r="L12" s="16"/>
+      <c r="M12" s="31">
+        <v>0</v>
+      </c>
+      <c r="N12" s="34">
+        <v>0</v>
+      </c>
+      <c r="O12" s="43">
+        <v>1</v>
+      </c>
+      <c r="P12" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>1010</v>
+      </c>
+      <c r="R12" s="34">
+        <v>0</v>
+      </c>
+      <c r="S12" s="34">
+        <v>0</v>
+      </c>
+      <c r="T12" s="34">
+        <v>0</v>
+      </c>
+      <c r="U12" s="34">
+        <v>1</v>
+      </c>
+      <c r="V12" s="34">
+        <v>0</v>
+      </c>
+      <c r="W12" s="34">
+        <v>0</v>
+      </c>
+      <c r="X12" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="34">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="19" t="s">
         <v>86</v>
       </c>
       <c r="D13" s="13" t="s">
@@ -1586,32 +2389,84 @@
       <c r="F13" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="I13" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="J13" s="28" t="s">
+      <c r="J13" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="K13" s="23" t="s">
+      <c r="K13" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="L13" s="24"/>
-    </row>
-    <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="7" t="s">
+      <c r="L13" s="16"/>
+      <c r="M13" s="30">
+        <v>1</v>
+      </c>
+      <c r="N13" s="48">
+        <v>0</v>
+      </c>
+      <c r="O13" s="47">
+        <v>1</v>
+      </c>
+      <c r="P13" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>1011</v>
+      </c>
+      <c r="R13" s="48">
+        <v>0</v>
+      </c>
+      <c r="S13" s="48">
+        <v>0</v>
+      </c>
+      <c r="T13" s="48">
+        <v>0</v>
+      </c>
+      <c r="U13" s="48">
+        <v>1</v>
+      </c>
+      <c r="V13" s="48">
+        <v>0</v>
+      </c>
+      <c r="W13" s="48">
+        <v>0</v>
+      </c>
+      <c r="X13" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="13" t="s">
         <v>127</v>
       </c>
       <c r="E14" s="13" t="s">
@@ -1620,29 +2475,81 @@
       <c r="F14" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I14" s="21" t="s">
+      <c r="I14" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="J14" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="K14" s="23" t="s">
+      <c r="K14" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="L14" s="24"/>
-    </row>
-    <row r="15" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="7" t="s">
+      <c r="L14" s="16"/>
+      <c r="M14" s="32">
+        <v>0</v>
+      </c>
+      <c r="N14" s="34">
+        <v>0</v>
+      </c>
+      <c r="O14" s="43">
+        <v>1</v>
+      </c>
+      <c r="P14" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>1011</v>
+      </c>
+      <c r="R14" s="34">
+        <v>0</v>
+      </c>
+      <c r="S14" s="34">
+        <v>0</v>
+      </c>
+      <c r="T14" s="34">
+        <v>0</v>
+      </c>
+      <c r="U14" s="34">
+        <v>1</v>
+      </c>
+      <c r="V14" s="34">
+        <v>0</v>
+      </c>
+      <c r="W14" s="34">
+        <v>0</v>
+      </c>
+      <c r="X14" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="34">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="19" t="s">
         <v>104</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -1654,29 +2561,81 @@
       <c r="F15" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="I15" s="21" t="s">
+      <c r="I15" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="J15" s="28" t="s">
+      <c r="J15" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="K15" s="23" t="s">
+      <c r="K15" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="L15" s="24"/>
-    </row>
-    <row r="16" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="7" t="s">
+      <c r="L15" s="16"/>
+      <c r="M15" s="30">
+        <v>1</v>
+      </c>
+      <c r="N15" s="48">
+        <v>0</v>
+      </c>
+      <c r="O15" s="47">
+        <v>1</v>
+      </c>
+      <c r="P15" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="R15" s="48">
+        <v>0</v>
+      </c>
+      <c r="S15" s="48">
+        <v>0</v>
+      </c>
+      <c r="T15" s="48">
+        <v>0</v>
+      </c>
+      <c r="U15" s="48">
+        <v>1</v>
+      </c>
+      <c r="V15" s="48">
+        <v>0</v>
+      </c>
+      <c r="W15" s="48">
+        <v>0</v>
+      </c>
+      <c r="X15" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="19" t="s">
         <v>106</v>
       </c>
       <c r="D16" s="13" t="s">
@@ -1688,29 +2647,81 @@
       <c r="F16" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="J16" s="28" t="s">
+      <c r="J16" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="K16" s="23" t="s">
+      <c r="K16" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="L16" s="24"/>
-    </row>
-    <row r="17" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="7" t="s">
+      <c r="L16" s="16"/>
+      <c r="M16" s="32">
+        <v>0</v>
+      </c>
+      <c r="N16" s="34">
+        <v>0</v>
+      </c>
+      <c r="O16" s="43">
+        <v>1</v>
+      </c>
+      <c r="P16" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="R16" s="34">
+        <v>0</v>
+      </c>
+      <c r="S16" s="34">
+        <v>0</v>
+      </c>
+      <c r="T16" s="34">
+        <v>0</v>
+      </c>
+      <c r="U16" s="34">
+        <v>1</v>
+      </c>
+      <c r="V16" s="34">
+        <v>0</v>
+      </c>
+      <c r="W16" s="34">
+        <v>0</v>
+      </c>
+      <c r="X16" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="34">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="19" t="s">
         <v>102</v>
       </c>
       <c r="D17" s="13" t="s">
@@ -1722,29 +2733,81 @@
       <c r="F17" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="I17" s="21" t="s">
+      <c r="I17" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="J17" s="28" t="s">
+      <c r="J17" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="K17" s="23" t="s">
+      <c r="K17" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="L17" s="24"/>
-    </row>
-    <row r="18" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="7" t="s">
+      <c r="L17" s="16"/>
+      <c r="M17" s="30">
+        <v>1</v>
+      </c>
+      <c r="N17" s="48">
+        <v>0</v>
+      </c>
+      <c r="O17" s="47">
+        <v>1</v>
+      </c>
+      <c r="P17" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>1101</v>
+      </c>
+      <c r="R17" s="48">
+        <v>0</v>
+      </c>
+      <c r="S17" s="48">
+        <v>0</v>
+      </c>
+      <c r="T17" s="48">
+        <v>0</v>
+      </c>
+      <c r="U17" s="48">
+        <v>1</v>
+      </c>
+      <c r="V17" s="48">
+        <v>0</v>
+      </c>
+      <c r="W17" s="48">
+        <v>0</v>
+      </c>
+      <c r="X17" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="19" t="s">
         <v>100</v>
       </c>
       <c r="D18" s="13" t="s">
@@ -1756,29 +2819,81 @@
       <c r="F18" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="I18" s="21" t="s">
+      <c r="I18" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="J18" s="28" t="s">
+      <c r="J18" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="K18" s="23" t="s">
+      <c r="K18" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="L18" s="24"/>
-    </row>
-    <row r="19" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="7" t="s">
+      <c r="L18" s="16"/>
+      <c r="M18" s="32">
+        <v>0</v>
+      </c>
+      <c r="N18" s="34">
+        <v>0</v>
+      </c>
+      <c r="O18" s="43">
+        <v>1</v>
+      </c>
+      <c r="P18" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>1101</v>
+      </c>
+      <c r="R18" s="34">
+        <v>0</v>
+      </c>
+      <c r="S18" s="34">
+        <v>0</v>
+      </c>
+      <c r="T18" s="34">
+        <v>0</v>
+      </c>
+      <c r="U18" s="34">
+        <v>1</v>
+      </c>
+      <c r="V18" s="34">
+        <v>0</v>
+      </c>
+      <c r="W18" s="34">
+        <v>0</v>
+      </c>
+      <c r="X18" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="34">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="17"/>
+      <c r="B19" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="19" t="s">
         <v>92</v>
       </c>
       <c r="D19" s="13" t="s">
@@ -1790,29 +2905,81 @@
       <c r="F19" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="H19" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="I19" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="J19" s="28" t="s">
+      <c r="J19" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="K19" s="23" t="s">
+      <c r="K19" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="L19" s="24"/>
-    </row>
-    <row r="20" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="7" t="s">
+      <c r="L19" s="16"/>
+      <c r="M19" s="30">
+        <v>0</v>
+      </c>
+      <c r="N19" s="48">
+        <v>0</v>
+      </c>
+      <c r="O19" s="47">
+        <v>1</v>
+      </c>
+      <c r="P19" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>1110</v>
+      </c>
+      <c r="R19" s="48">
+        <v>0</v>
+      </c>
+      <c r="S19" s="48">
+        <v>0</v>
+      </c>
+      <c r="T19" s="48">
+        <v>0</v>
+      </c>
+      <c r="U19" s="48">
+        <v>1</v>
+      </c>
+      <c r="V19" s="48">
+        <v>0</v>
+      </c>
+      <c r="W19" s="48">
+        <v>0</v>
+      </c>
+      <c r="X19" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="48">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="17"/>
+      <c r="B20" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="19" t="s">
         <v>112</v>
       </c>
       <c r="D20" s="13" t="s">
@@ -1824,29 +2991,81 @@
       <c r="F20" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I20" s="21" t="s">
+      <c r="I20" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="J20" s="28" t="s">
+      <c r="J20" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="K20" s="23" t="s">
+      <c r="K20" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="L20" s="24"/>
-    </row>
-    <row r="21" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6" t="s">
+      <c r="L20" s="16"/>
+      <c r="M20" s="32">
+        <v>0</v>
+      </c>
+      <c r="N20" s="34">
+        <v>0</v>
+      </c>
+      <c r="O20" s="43">
+        <v>1</v>
+      </c>
+      <c r="P20" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>1110</v>
+      </c>
+      <c r="R20" s="34">
+        <v>0</v>
+      </c>
+      <c r="S20" s="34">
+        <v>0</v>
+      </c>
+      <c r="T20" s="34">
+        <v>0</v>
+      </c>
+      <c r="U20" s="34">
+        <v>1</v>
+      </c>
+      <c r="V20" s="34">
+        <v>0</v>
+      </c>
+      <c r="W20" s="34">
+        <v>0</v>
+      </c>
+      <c r="X20" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="34">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="22" t="s">
         <v>63</v>
       </c>
       <c r="D21" s="13" t="s">
@@ -1858,25 +3077,32 @@
       <c r="F21" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="I21" s="21" t="s">
+      <c r="I21" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="J21" s="28"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="24"/>
-    </row>
-    <row r="22" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="7" t="s">
+      <c r="J21" s="14"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="M21" s="30">
+        <v>0</v>
+      </c>
+      <c r="N21" s="48"/>
+      <c r="Q21" s="39"/>
+    </row>
+    <row r="22" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="17"/>
+      <c r="B22" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="19" t="s">
         <v>98</v>
       </c>
       <c r="D22" s="13" t="s">
@@ -1888,25 +3114,81 @@
       <c r="F22" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G22" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H22" s="21" t="s">
+      <c r="H22" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I22" s="21" t="s">
+      <c r="I22" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="J22" s="28"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="24"/>
-    </row>
-    <row r="23" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="7" t="s">
+      <c r="J22" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" s="49">
+        <v>0</v>
+      </c>
+      <c r="L22" s="16"/>
+      <c r="M22" s="32">
+        <v>0</v>
+      </c>
+      <c r="N22" s="35">
+        <v>0</v>
+      </c>
+      <c r="O22" s="45">
+        <v>10</v>
+      </c>
+      <c r="P22" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="50">
+        <f>K22</f>
+        <v>0</v>
+      </c>
+      <c r="R22" s="35">
+        <v>0</v>
+      </c>
+      <c r="S22" s="35">
+        <v>0</v>
+      </c>
+      <c r="T22" s="35">
+        <v>0</v>
+      </c>
+      <c r="U22" s="35">
+        <v>1</v>
+      </c>
+      <c r="V22" s="35">
+        <v>0</v>
+      </c>
+      <c r="W22" s="35">
+        <v>0</v>
+      </c>
+      <c r="X22" s="35">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="35">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="35">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="42">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="35">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="17"/>
+      <c r="B23" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="19" t="s">
         <v>96</v>
       </c>
       <c r="D23" s="13" t="s">
@@ -1918,25 +3200,81 @@
       <c r="F23" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G23" s="21" t="s">
+      <c r="G23" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H23" s="21" t="s">
+      <c r="H23" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I23" s="21" t="s">
+      <c r="I23" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="J23" s="28"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="24"/>
-    </row>
-    <row r="24" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4" t="s">
+      <c r="J23" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K23" s="49">
+        <v>0</v>
+      </c>
+      <c r="L23" s="16"/>
+      <c r="M23" s="30">
+        <v>0</v>
+      </c>
+      <c r="N23" s="33">
+        <v>0</v>
+      </c>
+      <c r="O23" s="44">
+        <v>10</v>
+      </c>
+      <c r="P23" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="51">
+        <f>K23</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="33">
+        <v>0</v>
+      </c>
+      <c r="S23" s="33">
+        <v>0</v>
+      </c>
+      <c r="T23" s="33">
+        <v>0</v>
+      </c>
+      <c r="U23" s="33">
+        <v>1</v>
+      </c>
+      <c r="V23" s="33">
+        <v>0</v>
+      </c>
+      <c r="W23" s="33">
+        <v>0</v>
+      </c>
+      <c r="X23" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="33">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="33">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="23"/>
+      <c r="B24" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="25" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="13" t="s">
@@ -1948,25 +3286,43 @@
       <c r="F24" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H24" s="21" t="s">
+      <c r="H24" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I24" s="21" t="s">
+      <c r="I24" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="J24" s="28"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="24"/>
-    </row>
-    <row r="25" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4" t="s">
+      <c r="J24" s="14"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="M24" s="32"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="40"/>
+      <c r="R24" s="35"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="35"/>
+      <c r="U24" s="35"/>
+      <c r="V24" s="35"/>
+      <c r="W24" s="35"/>
+      <c r="X24" s="35"/>
+      <c r="Y24" s="35"/>
+      <c r="Z24" s="35"/>
+      <c r="AA24" s="42"/>
+      <c r="AB24" s="35"/>
+    </row>
+    <row r="25" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="23"/>
+      <c r="B25" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="25" t="s">
         <v>38</v>
       </c>
       <c r="D25" s="13" t="s">
@@ -1978,25 +3334,28 @@
       <c r="F25" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G25" s="21" t="s">
+      <c r="G25" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="H25" s="21" t="s">
+      <c r="H25" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I25" s="21" t="s">
+      <c r="I25" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="J25" s="28"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="24"/>
-    </row>
-    <row r="26" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4" t="s">
+      <c r="J25" s="14"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q25" s="39"/>
+    </row>
+    <row r="26" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="23"/>
+      <c r="B26" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="25" t="s">
         <v>44</v>
       </c>
       <c r="D26" s="13" t="s">
@@ -2008,25 +3367,43 @@
       <c r="F26" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G26" s="21" t="s">
+      <c r="G26" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H26" s="21" t="s">
+      <c r="H26" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I26" s="21" t="s">
+      <c r="I26" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="J26" s="28"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="24"/>
-    </row>
-    <row r="27" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4" t="s">
+      <c r="J26" s="14"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="M26" s="32"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="46"/>
+      <c r="P26" s="35"/>
+      <c r="Q26" s="40"/>
+      <c r="R26" s="35"/>
+      <c r="S26" s="35"/>
+      <c r="T26" s="35"/>
+      <c r="U26" s="35"/>
+      <c r="V26" s="35"/>
+      <c r="W26" s="35"/>
+      <c r="X26" s="35"/>
+      <c r="Y26" s="35"/>
+      <c r="Z26" s="35"/>
+      <c r="AA26" s="42"/>
+      <c r="AB26" s="35"/>
+    </row>
+    <row r="27" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="23"/>
+      <c r="B27" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="25" t="s">
         <v>40</v>
       </c>
       <c r="D27" s="13" t="s">
@@ -2038,27 +3415,30 @@
       <c r="F27" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G27" s="21" t="s">
+      <c r="G27" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="H27" s="21" t="s">
+      <c r="H27" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I27" s="21" t="s">
+      <c r="I27" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="J27" s="28"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="24"/>
-    </row>
-    <row r="28" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="J27" s="14"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q27" s="39"/>
+    </row>
+    <row r="28" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="22" t="s">
         <v>49</v>
       </c>
       <c r="D28" s="13" t="s">
@@ -2070,109 +3450,161 @@
       <c r="F28" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="G28" s="25" t="s">
+      <c r="G28" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="28" t="s">
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K28" s="23" t="s">
+      <c r="K28" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="L28" s="24"/>
-    </row>
-    <row r="29" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6" t="s">
+      <c r="L28" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="M28" s="32"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="46"/>
+      <c r="P28" s="35"/>
+      <c r="Q28" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="R28" s="35"/>
+      <c r="S28" s="35"/>
+      <c r="T28" s="35"/>
+      <c r="U28" s="35"/>
+      <c r="V28" s="35"/>
+      <c r="W28" s="35"/>
+      <c r="X28" s="35"/>
+      <c r="Y28" s="35"/>
+      <c r="Z28" s="35"/>
+      <c r="AA28" s="42"/>
+      <c r="AB28" s="35"/>
+    </row>
+    <row r="29" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="20"/>
+      <c r="B29" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="22" t="s">
         <v>59</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="F29" s="21" t="s">
+      <c r="F29" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G29" s="25" t="s">
+      <c r="G29" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="28" t="s">
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K29" s="23" t="s">
+      <c r="K29" s="15" t="s">
         <v>175</v>
       </c>
       <c r="L29" s="27" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6" t="s">
+      <c r="Q29" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="20"/>
+      <c r="B30" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="22" t="s">
         <v>61</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="28" t="s">
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="K30" s="23" t="s">
+      <c r="K30" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="L30" s="24"/>
-    </row>
-    <row r="31" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6" t="s">
+      <c r="L30" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="M30" s="32"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="46"/>
+      <c r="P30" s="35"/>
+      <c r="Q30" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="R30" s="35"/>
+      <c r="S30" s="35"/>
+      <c r="T30" s="35"/>
+      <c r="U30" s="35"/>
+      <c r="V30" s="35"/>
+      <c r="W30" s="35"/>
+      <c r="X30" s="35"/>
+      <c r="Y30" s="35"/>
+      <c r="Z30" s="35"/>
+      <c r="AA30" s="42"/>
+      <c r="AB30" s="35"/>
+    </row>
+    <row r="31" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="20"/>
+      <c r="B31" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="22" t="s">
         <v>65</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="E31" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="28" t="s">
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="K31" s="23" t="s">
+      <c r="K31" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="L31" s="24"/>
-    </row>
-    <row r="32" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6" t="s">
+      <c r="L31" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q31" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="21"/>
+      <c r="B32" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="22" t="s">
         <v>51</v>
       </c>
       <c r="D32" s="13" t="s">
@@ -2184,25 +3616,46 @@
       <c r="F32" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G32" s="25" t="s">
+      <c r="G32" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="28" t="s">
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K32" s="23" t="s">
+      <c r="K32" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="L32" s="24"/>
-    </row>
-    <row r="33" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6" t="s">
+      <c r="L32" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="M32" s="32"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="46"/>
+      <c r="P32" s="35"/>
+      <c r="Q32" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="R32" s="35"/>
+      <c r="S32" s="35"/>
+      <c r="T32" s="35"/>
+      <c r="U32" s="35"/>
+      <c r="V32" s="35"/>
+      <c r="W32" s="35"/>
+      <c r="X32" s="35"/>
+      <c r="Y32" s="35"/>
+      <c r="Z32" s="35"/>
+      <c r="AA32" s="42"/>
+      <c r="AB32" s="35"/>
+    </row>
+    <row r="33" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="22" t="s">
         <v>53</v>
       </c>
       <c r="D33" s="13" t="s">
@@ -2214,25 +3667,31 @@
       <c r="F33" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G33" s="25" t="s">
+      <c r="G33" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="28" t="s">
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K33" s="23" t="s">
+      <c r="K33" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="L33" s="24"/>
-    </row>
-    <row r="34" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6" t="s">
+      <c r="L33" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q33" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="21"/>
+      <c r="B34" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="22" t="s">
         <v>57</v>
       </c>
       <c r="D34" s="13" t="s">
@@ -2244,85 +3703,164 @@
       <c r="F34" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G34" s="25" t="s">
+      <c r="G34" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="28" t="s">
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K34" s="23" t="s">
+      <c r="K34" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="L34" s="24"/>
-    </row>
-    <row r="35" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6" t="s">
+      <c r="L34" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="M34" s="32"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="46"/>
+      <c r="P34" s="35"/>
+      <c r="Q34" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="R34" s="35"/>
+      <c r="S34" s="35"/>
+      <c r="T34" s="35"/>
+      <c r="U34" s="35"/>
+      <c r="V34" s="35"/>
+      <c r="W34" s="35"/>
+      <c r="X34" s="35"/>
+      <c r="Y34" s="35"/>
+      <c r="Z34" s="35"/>
+      <c r="AA34" s="42"/>
+      <c r="AB34" s="35"/>
+    </row>
+    <row r="35" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="21"/>
+      <c r="B35" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="22" t="s">
         <v>55</v>
       </c>
       <c r="D35" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="E35" s="21" t="s">
+      <c r="E35" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="F35" s="21" t="s">
+      <c r="F35" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G35" s="25" t="s">
+      <c r="G35" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="28" t="s">
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K35" s="23" t="s">
+      <c r="K35" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="L35" s="24"/>
-    </row>
-    <row r="36" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2" t="s">
+      <c r="L35" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q35" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D36" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E36" s="21" t="s">
+      <c r="E36" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="F36" s="21" t="s">
+      <c r="F36" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G36" s="25" t="s">
+      <c r="G36" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="28" t="s">
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K36" s="23" t="s">
+      <c r="K36" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="L36" s="24"/>
-    </row>
-    <row r="37" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2" t="s">
+      <c r="L36" s="16"/>
+      <c r="M36" s="32">
+        <v>0</v>
+      </c>
+      <c r="N36" s="35">
+        <v>0</v>
+      </c>
+      <c r="O36" s="46">
+        <v>0</v>
+      </c>
+      <c r="P36" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="R36" s="35">
+        <v>0</v>
+      </c>
+      <c r="S36" s="35">
+        <v>0</v>
+      </c>
+      <c r="T36" s="35">
+        <v>0</v>
+      </c>
+      <c r="U36" s="35">
+        <v>1</v>
+      </c>
+      <c r="V36" s="35">
+        <v>0</v>
+      </c>
+      <c r="W36" s="35">
+        <v>0</v>
+      </c>
+      <c r="X36" s="35">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="35">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="35">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="42">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="35">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D37" s="13" t="s">
@@ -2334,25 +3872,77 @@
       <c r="F37" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G37" s="25" t="s">
+      <c r="G37" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="28" t="s">
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K37" s="23" t="s">
+      <c r="K37" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="L37" s="24"/>
-    </row>
-    <row r="38" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7" t="s">
+      <c r="L37" s="16"/>
+      <c r="M37" s="30">
+        <v>1</v>
+      </c>
+      <c r="N37" s="33">
+        <v>0</v>
+      </c>
+      <c r="O37" s="44">
+        <v>0</v>
+      </c>
+      <c r="P37" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="R37" s="33">
+        <v>0</v>
+      </c>
+      <c r="S37" s="33">
+        <v>0</v>
+      </c>
+      <c r="T37" s="33">
+        <v>0</v>
+      </c>
+      <c r="U37" s="33">
+        <v>1</v>
+      </c>
+      <c r="V37" s="33">
+        <v>0</v>
+      </c>
+      <c r="W37" s="33">
+        <v>0</v>
+      </c>
+      <c r="X37" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="33">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="33">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="19" t="s">
         <v>94</v>
       </c>
       <c r="D38" s="13" t="s">
@@ -2364,25 +3954,77 @@
       <c r="F38" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G38" s="25" t="s">
+      <c r="G38" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="28" t="s">
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="K38" s="23" t="s">
+      <c r="K38" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="L38" s="24"/>
-    </row>
-    <row r="39" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7" t="s">
+      <c r="L38" s="16"/>
+      <c r="M38" s="32">
+        <v>0</v>
+      </c>
+      <c r="N38" s="35">
+        <v>0</v>
+      </c>
+      <c r="O38" s="46">
+        <v>0</v>
+      </c>
+      <c r="P38" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>1110</v>
+      </c>
+      <c r="R38" s="35">
+        <v>0</v>
+      </c>
+      <c r="S38" s="35">
+        <v>0</v>
+      </c>
+      <c r="T38" s="35">
+        <v>0</v>
+      </c>
+      <c r="U38" s="35">
+        <v>1</v>
+      </c>
+      <c r="V38" s="35">
+        <v>0</v>
+      </c>
+      <c r="W38" s="35">
+        <v>0</v>
+      </c>
+      <c r="X38" s="35">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="35">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="35">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="42">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="35">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="18"/>
+      <c r="B39" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="19" t="s">
         <v>110</v>
       </c>
       <c r="D39" s="13" t="s">
@@ -2394,25 +4036,77 @@
       <c r="F39" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G39" s="25" t="s">
+      <c r="G39" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="28" t="s">
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="K39" s="23" t="s">
+      <c r="K39" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="L39" s="24"/>
-    </row>
-    <row r="40" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7" t="s">
+      <c r="L39" s="16"/>
+      <c r="M39" s="30">
+        <v>1</v>
+      </c>
+      <c r="N39" s="33">
+        <v>0</v>
+      </c>
+      <c r="O39" s="44">
+        <v>0</v>
+      </c>
+      <c r="P39" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>1110</v>
+      </c>
+      <c r="R39" s="33">
+        <v>0</v>
+      </c>
+      <c r="S39" s="33">
+        <v>0</v>
+      </c>
+      <c r="T39" s="33">
+        <v>0</v>
+      </c>
+      <c r="U39" s="33">
+        <v>1</v>
+      </c>
+      <c r="V39" s="33">
+        <v>0</v>
+      </c>
+      <c r="W39" s="33">
+        <v>0</v>
+      </c>
+      <c r="X39" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="33">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="33">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="19" t="s">
         <v>70</v>
       </c>
       <c r="D40" s="13" t="s">
@@ -2424,25 +4118,46 @@
       <c r="F40" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G40" s="25" t="s">
+      <c r="G40" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="28" t="s">
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="K40" s="23" t="s">
+      <c r="K40" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="L40" s="24"/>
-    </row>
-    <row r="41" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7" t="s">
+      <c r="L40" s="16"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="46">
+        <v>0</v>
+      </c>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>0110</v>
+      </c>
+      <c r="R40" s="35"/>
+      <c r="S40" s="35"/>
+      <c r="T40" s="35"/>
+      <c r="U40" s="35"/>
+      <c r="V40" s="35"/>
+      <c r="W40" s="35"/>
+      <c r="X40" s="35"/>
+      <c r="Y40" s="35"/>
+      <c r="Z40" s="35"/>
+      <c r="AA40" s="42"/>
+      <c r="AB40" s="35"/>
+    </row>
+    <row r="41" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="19" t="s">
         <v>78</v>
       </c>
       <c r="D41" s="13" t="s">
@@ -2454,25 +4169,32 @@
       <c r="F41" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G41" s="25" t="s">
+      <c r="G41" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="28" t="s">
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K41" s="23" t="s">
+      <c r="K41" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="L41" s="24"/>
-    </row>
-    <row r="42" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7" t="s">
+      <c r="L41" s="16"/>
+      <c r="O41" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="19" t="s">
         <v>80</v>
       </c>
       <c r="D42" s="13" t="s">
@@ -2484,25 +4206,46 @@
       <c r="F42" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G42" s="25" t="s">
+      <c r="G42" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="28" t="s">
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="K42" s="23" t="s">
+      <c r="K42" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="L42" s="24"/>
-    </row>
-    <row r="43" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4" t="s">
+      <c r="L42" s="16"/>
+      <c r="M42" s="32"/>
+      <c r="N42" s="35"/>
+      <c r="O42" s="46">
+        <v>0</v>
+      </c>
+      <c r="P42" s="35"/>
+      <c r="Q42" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="R42" s="35"/>
+      <c r="S42" s="35"/>
+      <c r="T42" s="35"/>
+      <c r="U42" s="35"/>
+      <c r="V42" s="35"/>
+      <c r="W42" s="35"/>
+      <c r="X42" s="35"/>
+      <c r="Y42" s="35"/>
+      <c r="Z42" s="35"/>
+      <c r="AA42" s="42"/>
+      <c r="AB42" s="35"/>
+    </row>
+    <row r="43" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="24"/>
+      <c r="B43" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="25" t="s">
         <v>46</v>
       </c>
       <c r="D43" s="13" t="s">
@@ -2514,25 +4257,31 @@
       <c r="F43" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G43" s="25" t="s">
+      <c r="G43" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="28" t="s">
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="K43" s="23" t="s">
+      <c r="K43" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="L43" s="24"/>
-    </row>
-    <row r="44" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2" t="s">
+      <c r="L43" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q43" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="10"/>
+      <c r="B44" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D44" s="13" t="s">
@@ -2544,29 +4293,50 @@
       <c r="F44" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G44" s="21" t="s">
+      <c r="G44" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H44" s="21" t="s">
+      <c r="H44" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I44" s="21" t="s">
+      <c r="I44" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="J44" s="28" t="s">
+      <c r="J44" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="K44" s="23" t="s">
+      <c r="K44" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="L44" s="24"/>
-    </row>
-    <row r="45" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2" t="s">
+      <c r="L44" s="16"/>
+      <c r="M44" s="32"/>
+      <c r="N44" s="35"/>
+      <c r="O44" s="46">
+        <v>1</v>
+      </c>
+      <c r="P44" s="35"/>
+      <c r="Q44" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>0010</v>
+      </c>
+      <c r="R44" s="35"/>
+      <c r="S44" s="35"/>
+      <c r="T44" s="35"/>
+      <c r="U44" s="35"/>
+      <c r="V44" s="35"/>
+      <c r="W44" s="35"/>
+      <c r="X44" s="35"/>
+      <c r="Y44" s="35"/>
+      <c r="Z44" s="35"/>
+      <c r="AA44" s="42"/>
+      <c r="AB44" s="35"/>
+    </row>
+    <row r="45" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="10"/>
+      <c r="B45" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D45" s="13" t="s">
@@ -2578,29 +4348,36 @@
       <c r="F45" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G45" s="21" t="s">
+      <c r="G45" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="H45" s="21" t="s">
+      <c r="H45" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I45" s="21" t="s">
+      <c r="I45" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="J45" s="28" t="s">
+      <c r="J45" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="K45" s="23" t="s">
+      <c r="K45" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="L45" s="24"/>
-    </row>
-    <row r="46" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2" t="s">
+      <c r="L45" s="16"/>
+      <c r="O45" s="44">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="10"/>
+      <c r="B46" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D46" s="13" t="s">
@@ -2612,29 +4389,50 @@
       <c r="F46" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G46" s="21" t="s">
+      <c r="G46" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I46" s="21" t="s">
+      <c r="I46" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="J46" s="28" t="s">
+      <c r="J46" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="K46" s="23" t="s">
+      <c r="K46" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="L46" s="24"/>
-    </row>
-    <row r="47" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7" t="s">
+      <c r="L46" s="16"/>
+      <c r="M46" s="32"/>
+      <c r="N46" s="35"/>
+      <c r="O46" s="46">
+        <v>1</v>
+      </c>
+      <c r="P46" s="35"/>
+      <c r="Q46" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>0101</v>
+      </c>
+      <c r="R46" s="35"/>
+      <c r="S46" s="35"/>
+      <c r="T46" s="35"/>
+      <c r="U46" s="35"/>
+      <c r="V46" s="35"/>
+      <c r="W46" s="35"/>
+      <c r="X46" s="35"/>
+      <c r="Y46" s="35"/>
+      <c r="Z46" s="35"/>
+      <c r="AA46" s="42"/>
+      <c r="AB46" s="35"/>
+    </row>
+    <row r="47" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="18"/>
+      <c r="B47" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="19" t="s">
         <v>82</v>
       </c>
       <c r="D47" s="13" t="s">
@@ -2646,29 +4444,36 @@
       <c r="F47" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="G47" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H47" s="21" t="s">
+      <c r="H47" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="I47" s="21" t="s">
+      <c r="I47" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="J47" s="28" t="s">
+      <c r="J47" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="K47" s="23" t="s">
+      <c r="K47" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="L47" s="24"/>
-    </row>
-    <row r="48" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7" t="s">
+      <c r="L47" s="16"/>
+      <c r="O47" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="19" t="s">
         <v>108</v>
       </c>
       <c r="D48" s="13" t="s">
@@ -2680,27 +4485,48 @@
       <c r="F48" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G48" s="21" t="s">
+      <c r="G48" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H48" s="21" t="s">
+      <c r="H48" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="I48" s="21" t="s">
+      <c r="I48" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="J48" s="28"/>
-      <c r="K48" s="23" t="s">
+      <c r="J48" s="14"/>
+      <c r="K48" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="L48" s="24"/>
-    </row>
-    <row r="49" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4" t="s">
+      <c r="L48" s="16"/>
+      <c r="M48" s="32"/>
+      <c r="N48" s="35"/>
+      <c r="O48" s="46">
+        <v>0</v>
+      </c>
+      <c r="P48" s="35"/>
+      <c r="Q48" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="R48" s="35"/>
+      <c r="S48" s="35"/>
+      <c r="T48" s="35"/>
+      <c r="U48" s="35"/>
+      <c r="V48" s="35"/>
+      <c r="W48" s="35"/>
+      <c r="X48" s="35"/>
+      <c r="Y48" s="35"/>
+      <c r="Z48" s="35"/>
+      <c r="AA48" s="42"/>
+      <c r="AB48" s="35"/>
+    </row>
+    <row r="49" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="24"/>
+      <c r="B49" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="25" t="s">
         <v>34</v>
       </c>
       <c r="D49" s="13" t="s">
@@ -2712,25 +4538,31 @@
       <c r="F49" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G49" s="25" t="s">
+      <c r="G49" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="28" t="s">
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K49" s="23" t="s">
+      <c r="K49" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="L49" s="24"/>
-    </row>
-    <row r="50" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4" t="s">
+      <c r="L49" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q49" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="24"/>
+      <c r="B50" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="25" t="s">
         <v>32</v>
       </c>
       <c r="D50" s="13" t="s">
@@ -2742,27 +4574,48 @@
       <c r="F50" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G50" s="25" t="s">
+      <c r="G50" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="H50" s="25"/>
-      <c r="I50" s="25"/>
-      <c r="J50" s="28" t="s">
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K50" s="23" t="s">
+      <c r="K50" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="L50" s="24"/>
-    </row>
-    <row r="51" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="L50" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="M50" s="32"/>
+      <c r="N50" s="35"/>
+      <c r="O50" s="46"/>
+      <c r="P50" s="35"/>
+      <c r="Q50" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="R50" s="35"/>
+      <c r="S50" s="35"/>
+      <c r="T50" s="35"/>
+      <c r="U50" s="35"/>
+      <c r="V50" s="35"/>
+      <c r="W50" s="35"/>
+      <c r="X50" s="35"/>
+      <c r="Y50" s="35"/>
+      <c r="Z50" s="35"/>
+      <c r="AA50" s="42"/>
+      <c r="AB50" s="35"/>
+    </row>
+    <row r="51" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="25" t="s">
         <v>26</v>
       </c>
       <c r="D51" s="13" t="s">
@@ -2774,25 +4627,31 @@
       <c r="F51" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G51" s="25" t="s">
+      <c r="G51" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="H51" s="25"/>
-      <c r="I51" s="25"/>
-      <c r="J51" s="28" t="s">
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K51" s="23" t="s">
+      <c r="K51" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="L51" s="24"/>
-    </row>
-    <row r="52" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4" t="s">
+      <c r="L51" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q51" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="24"/>
+      <c r="B52" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="25" t="s">
         <v>30</v>
       </c>
       <c r="D52" s="13" t="s">
@@ -2804,25 +4663,46 @@
       <c r="F52" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G52" s="25" t="s">
+      <c r="G52" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="H52" s="25"/>
-      <c r="I52" s="25"/>
-      <c r="J52" s="28" t="s">
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K52" s="23" t="s">
+      <c r="K52" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="L52" s="24"/>
-    </row>
-    <row r="53" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4" t="s">
+      <c r="L52" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="M52" s="32"/>
+      <c r="N52" s="35"/>
+      <c r="O52" s="46"/>
+      <c r="P52" s="35"/>
+      <c r="Q52" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="R52" s="35"/>
+      <c r="S52" s="35"/>
+      <c r="T52" s="35"/>
+      <c r="U52" s="35"/>
+      <c r="V52" s="35"/>
+      <c r="W52" s="35"/>
+      <c r="X52" s="35"/>
+      <c r="Y52" s="35"/>
+      <c r="Z52" s="35"/>
+      <c r="AA52" s="42"/>
+      <c r="AB52" s="35"/>
+    </row>
+    <row r="53" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="24"/>
+      <c r="B53" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C53" s="25" t="s">
         <v>36</v>
       </c>
       <c r="D53" s="13" t="s">
@@ -2834,25 +4714,31 @@
       <c r="F53" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G53" s="25" t="s">
+      <c r="G53" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="28" t="s">
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K53" s="23" t="s">
+      <c r="K53" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="L53" s="24"/>
-    </row>
-    <row r="54" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4" t="s">
+      <c r="L53" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q53" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="24"/>
+      <c r="B54" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="25" t="s">
         <v>28</v>
       </c>
       <c r="D54" s="13" t="s">
@@ -2864,26 +4750,47 @@
       <c r="F54" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G54" s="25" t="s">
+      <c r="G54" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="28" t="s">
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K54" s="23" t="s">
+      <c r="K54" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="L54" s="24"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
+      <c r="L54" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="M54" s="32"/>
+      <c r="N54" s="35"/>
+      <c r="O54" s="46"/>
+      <c r="P54" s="35"/>
+      <c r="Q54" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="R54" s="35"/>
+      <c r="S54" s="35"/>
+      <c r="T54" s="35"/>
+      <c r="U54" s="35"/>
+      <c r="V54" s="35"/>
+      <c r="W54" s="35"/>
+      <c r="X54" s="35"/>
+      <c r="Y54" s="35"/>
+      <c r="Z54" s="35"/>
+      <c r="AA54" s="42"/>
+      <c r="AB54" s="35"/>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="28"/>
+      <c r="I55" s="28"/>
     </row>
   </sheetData>
   <sortState ref="A2:K54">
@@ -2891,18 +4798,6 @@
     <sortCondition ref="K2:K54"/>
     <sortCondition ref="I2:I54"/>
   </sortState>
-  <conditionalFormatting sqref="K2:K54">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L2:L54">
     <cfRule type="colorScale" priority="1">
       <colorScale>
@@ -2914,5 +4809,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished lab 8-14 control signals in spreadsheet
</commit_message>
<xml_diff>
--- a/LAB8-11/DatapathComponents/ALU_mapping.xlsx
+++ b/LAB8-11/DatapathComponents/ALU_mapping.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ryan\Documents\ECE369a\lab369a\LAB8-11\DatapathComponents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanjsims\lab369a\LAB8-11\DatapathComponents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="465" windowWidth="24720" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1815" yWindow="465" windowWidth="24720" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="206">
   <si>
     <t>Type</t>
   </si>
@@ -594,9 +594,6 @@
   </si>
   <si>
     <t>1100</t>
-  </si>
-  <si>
-    <t>STOPPED HERE</t>
   </si>
   <si>
     <t>Control Signals:</t>
@@ -653,10 +650,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="00"/>
-    <numFmt numFmtId="166" formatCode="0000"/>
+    <numFmt numFmtId="164" formatCode="00"/>
+    <numFmt numFmtId="165" formatCode="0000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -722,7 +719,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -761,12 +758,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
@@ -778,7 +769,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -878,6 +869,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -889,9 +889,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -963,53 +963,58 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="9" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="9" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="9" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="9" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="8" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="7" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="9" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1300,13 +1305,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="M40" sqref="M40"/>
+      <selection pane="bottomLeft" activeCell="AD48" sqref="AD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1315,21 +1320,21 @@
     <col min="2" max="2" width="32.125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="11" width="11" style="8"/>
     <col min="12" max="12" width="20.25" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" style="30"/>
-    <col min="14" max="14" width="6.875" style="33" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.875" style="44" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7" style="33" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.375" style="33" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.125" style="33" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.625" style="33" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.75" style="33" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9" style="33" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.625" style="33" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="4.875" style="33" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.375" style="33" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.875" style="33" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.375" style="41" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.875" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="29"/>
+    <col min="14" max="14" width="6.875" style="32" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.875" style="43" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" style="32" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.375" style="32" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.125" style="32" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.625" style="32" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.75" style="32" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" style="32" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.625" style="32" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="4.875" style="32" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.375" style="32" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.875" style="32" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.375" style="40" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.875" style="32" bestFit="1" customWidth="1"/>
     <col min="29" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
@@ -1368,58 +1373,58 @@
         <v>120</v>
       </c>
       <c r="L1" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="M1" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="N1" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="O1" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="O1" s="44" t="s">
+      <c r="P1" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="Q1" s="32" t="s">
         <v>194</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="R1" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="S1" s="32" t="s">
         <v>196</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="T1" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="U1" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="U1" s="33" t="s">
+      <c r="V1" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="V1" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="W1" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="X1" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y1" s="33" t="s">
+      <c r="Z1" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="Z1" s="33" t="s">
+      <c r="AA1" s="40" t="s">
         <v>201</v>
       </c>
-      <c r="AA1" s="41" t="s">
+      <c r="AB1" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="AB1" s="33" t="s">
-        <v>203</v>
-      </c>
       <c r="AC1" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1457,53 +1462,53 @@
         <v>174</v>
       </c>
       <c r="L2" s="16"/>
-      <c r="M2" s="31">
-        <v>0</v>
-      </c>
-      <c r="N2" s="34">
-        <v>0</v>
-      </c>
-      <c r="O2" s="43">
-        <v>1</v>
-      </c>
-      <c r="P2" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="38" t="str">
+      <c r="M2" s="30">
+        <v>0</v>
+      </c>
+      <c r="N2" s="33">
+        <v>0</v>
+      </c>
+      <c r="O2" s="42">
+        <v>1</v>
+      </c>
+      <c r="P2" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="37" t="str">
         <f>K2</f>
         <v>0000</v>
       </c>
-      <c r="R2" s="34">
-        <v>0</v>
-      </c>
-      <c r="S2" s="34">
-        <v>0</v>
-      </c>
-      <c r="T2" s="34">
-        <v>0</v>
-      </c>
-      <c r="U2" s="34">
-        <v>1</v>
-      </c>
-      <c r="V2" s="34">
-        <v>0</v>
-      </c>
-      <c r="W2" s="34">
-        <v>0</v>
-      </c>
-      <c r="X2" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="34">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="34">
+      <c r="R2" s="33">
+        <v>0</v>
+      </c>
+      <c r="S2" s="33">
+        <v>0</v>
+      </c>
+      <c r="T2" s="33">
+        <v>0</v>
+      </c>
+      <c r="U2" s="33">
+        <v>1</v>
+      </c>
+      <c r="V2" s="33">
+        <v>0</v>
+      </c>
+      <c r="W2" s="33">
+        <v>0</v>
+      </c>
+      <c r="X2" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="33">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="33">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="33">
         <v>0</v>
       </c>
       <c r="AC2" s="8">
@@ -1543,53 +1548,53 @@
         <v>174</v>
       </c>
       <c r="L3" s="16"/>
-      <c r="M3" s="30">
-        <v>0</v>
-      </c>
-      <c r="N3" s="33">
-        <v>0</v>
-      </c>
-      <c r="O3" s="47">
-        <v>1</v>
-      </c>
-      <c r="P3" s="33">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="39" t="str">
+      <c r="M3" s="29">
+        <v>0</v>
+      </c>
+      <c r="N3" s="32">
+        <v>0</v>
+      </c>
+      <c r="O3" s="46">
+        <v>1</v>
+      </c>
+      <c r="P3" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="38" t="str">
         <f t="shared" ref="Q3:Q54" si="0">K3</f>
         <v>0000</v>
       </c>
-      <c r="R3" s="33">
-        <v>0</v>
-      </c>
-      <c r="S3" s="33">
-        <v>0</v>
-      </c>
-      <c r="T3" s="33">
-        <v>0</v>
-      </c>
-      <c r="U3" s="33">
-        <v>1</v>
-      </c>
-      <c r="V3" s="33">
-        <v>0</v>
-      </c>
-      <c r="W3" s="33">
-        <v>0</v>
-      </c>
-      <c r="X3" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="33">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="33">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="41">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="33">
+      <c r="R3" s="32">
+        <v>0</v>
+      </c>
+      <c r="S3" s="32">
+        <v>0</v>
+      </c>
+      <c r="T3" s="32">
+        <v>0</v>
+      </c>
+      <c r="U3" s="32">
+        <v>1</v>
+      </c>
+      <c r="V3" s="32">
+        <v>0</v>
+      </c>
+      <c r="W3" s="32">
+        <v>0</v>
+      </c>
+      <c r="X3" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="32">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="32">
         <v>0</v>
       </c>
       <c r="AC3" s="8">
@@ -1629,53 +1634,53 @@
         <v>175</v>
       </c>
       <c r="L4" s="16"/>
-      <c r="M4" s="31">
-        <v>0</v>
-      </c>
-      <c r="N4" s="34">
-        <v>0</v>
-      </c>
-      <c r="O4" s="43">
-        <v>1</v>
-      </c>
-      <c r="P4" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="38" t="str">
+      <c r="M4" s="30">
+        <v>0</v>
+      </c>
+      <c r="N4" s="33">
+        <v>0</v>
+      </c>
+      <c r="O4" s="42">
+        <v>1</v>
+      </c>
+      <c r="P4" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="37" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
-      <c r="R4" s="34">
-        <v>0</v>
-      </c>
-      <c r="S4" s="34">
-        <v>0</v>
-      </c>
-      <c r="T4" s="34">
-        <v>0</v>
-      </c>
-      <c r="U4" s="34">
-        <v>1</v>
-      </c>
-      <c r="V4" s="34">
-        <v>0</v>
-      </c>
-      <c r="W4" s="34">
-        <v>0</v>
-      </c>
-      <c r="X4" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="34">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="34">
+      <c r="R4" s="33">
+        <v>0</v>
+      </c>
+      <c r="S4" s="33">
+        <v>0</v>
+      </c>
+      <c r="T4" s="33">
+        <v>0</v>
+      </c>
+      <c r="U4" s="33">
+        <v>1</v>
+      </c>
+      <c r="V4" s="33">
+        <v>0</v>
+      </c>
+      <c r="W4" s="33">
+        <v>0</v>
+      </c>
+      <c r="X4" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="33">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="33">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="33">
         <v>0</v>
       </c>
       <c r="AC4" s="8">
@@ -1715,53 +1720,53 @@
         <v>176</v>
       </c>
       <c r="L5" s="16"/>
-      <c r="M5" s="30">
-        <v>0</v>
-      </c>
-      <c r="N5" s="33">
-        <v>0</v>
-      </c>
-      <c r="O5" s="47">
-        <v>1</v>
-      </c>
-      <c r="P5" s="36" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q5" s="39" t="str">
+      <c r="M5" s="29">
+        <v>0</v>
+      </c>
+      <c r="N5" s="32">
+        <v>0</v>
+      </c>
+      <c r="O5" s="46">
+        <v>1</v>
+      </c>
+      <c r="P5" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q5" s="38" t="str">
         <f t="shared" si="0"/>
         <v>0010</v>
       </c>
-      <c r="R5" s="33">
-        <v>0</v>
-      </c>
-      <c r="S5" s="33">
-        <v>0</v>
-      </c>
-      <c r="T5" s="36" t="s">
-        <v>204</v>
-      </c>
-      <c r="U5" s="33">
-        <v>0</v>
-      </c>
-      <c r="V5" s="33">
-        <v>0</v>
-      </c>
-      <c r="W5" s="33">
-        <v>0</v>
-      </c>
-      <c r="X5" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="33">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="33">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="41">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="33">
+      <c r="R5" s="32">
+        <v>0</v>
+      </c>
+      <c r="S5" s="32">
+        <v>0</v>
+      </c>
+      <c r="T5" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="U5" s="32">
+        <v>0</v>
+      </c>
+      <c r="V5" s="32">
+        <v>0</v>
+      </c>
+      <c r="W5" s="32">
+        <v>0</v>
+      </c>
+      <c r="X5" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="32">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="32">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="32">
         <v>1</v>
       </c>
       <c r="AC5" s="8">
@@ -1801,53 +1806,53 @@
         <v>177</v>
       </c>
       <c r="L6" s="16"/>
-      <c r="M6" s="31">
-        <v>0</v>
-      </c>
-      <c r="N6" s="34">
-        <v>0</v>
-      </c>
-      <c r="O6" s="43">
-        <v>1</v>
-      </c>
-      <c r="P6" s="37" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q6" s="38" t="str">
+      <c r="M6" s="30">
+        <v>0</v>
+      </c>
+      <c r="N6" s="33">
+        <v>0</v>
+      </c>
+      <c r="O6" s="42">
+        <v>1</v>
+      </c>
+      <c r="P6" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q6" s="37" t="str">
         <f t="shared" si="0"/>
         <v>0011</v>
       </c>
-      <c r="R6" s="34">
-        <v>0</v>
-      </c>
-      <c r="S6" s="34">
-        <v>0</v>
-      </c>
-      <c r="T6" s="37" t="s">
-        <v>204</v>
-      </c>
-      <c r="U6" s="34">
-        <v>0</v>
-      </c>
-      <c r="V6" s="34">
-        <v>0</v>
-      </c>
-      <c r="W6" s="34">
-        <v>0</v>
-      </c>
-      <c r="X6" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="34">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="34">
+      <c r="R6" s="33">
+        <v>0</v>
+      </c>
+      <c r="S6" s="33">
+        <v>0</v>
+      </c>
+      <c r="T6" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="U6" s="33">
+        <v>0</v>
+      </c>
+      <c r="V6" s="33">
+        <v>0</v>
+      </c>
+      <c r="W6" s="33">
+        <v>0</v>
+      </c>
+      <c r="X6" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="33">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="33">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="33">
         <v>1</v>
       </c>
       <c r="AC6" s="8">
@@ -1889,53 +1894,53 @@
         <v>180</v>
       </c>
       <c r="L7" s="16"/>
-      <c r="M7" s="30">
-        <v>0</v>
-      </c>
-      <c r="N7" s="33">
-        <v>0</v>
-      </c>
-      <c r="O7" s="47">
-        <v>1</v>
-      </c>
-      <c r="P7" s="33">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="39" t="str">
+      <c r="M7" s="29">
+        <v>0</v>
+      </c>
+      <c r="N7" s="32">
+        <v>0</v>
+      </c>
+      <c r="O7" s="46">
+        <v>1</v>
+      </c>
+      <c r="P7" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="38" t="str">
         <f t="shared" si="0"/>
         <v>0110</v>
       </c>
-      <c r="R7" s="33">
-        <v>0</v>
-      </c>
-      <c r="S7" s="33">
-        <v>0</v>
-      </c>
-      <c r="T7" s="33">
-        <v>0</v>
-      </c>
-      <c r="U7" s="33">
-        <v>1</v>
-      </c>
-      <c r="V7" s="33">
-        <v>0</v>
-      </c>
-      <c r="W7" s="33">
-        <v>0</v>
-      </c>
-      <c r="X7" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="33">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="33">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="41">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="33">
+      <c r="R7" s="32">
+        <v>0</v>
+      </c>
+      <c r="S7" s="32">
+        <v>0</v>
+      </c>
+      <c r="T7" s="32">
+        <v>0</v>
+      </c>
+      <c r="U7" s="32">
+        <v>1</v>
+      </c>
+      <c r="V7" s="32">
+        <v>0</v>
+      </c>
+      <c r="W7" s="32">
+        <v>0</v>
+      </c>
+      <c r="X7" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="32">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="32">
         <v>0</v>
       </c>
       <c r="AC7" s="8">
@@ -1975,53 +1980,53 @@
         <v>181</v>
       </c>
       <c r="L8" s="16"/>
-      <c r="M8" s="31">
-        <v>0</v>
-      </c>
-      <c r="N8" s="34">
-        <v>0</v>
-      </c>
-      <c r="O8" s="43">
-        <v>1</v>
-      </c>
-      <c r="P8" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="38" t="str">
+      <c r="M8" s="30">
+        <v>0</v>
+      </c>
+      <c r="N8" s="33">
+        <v>0</v>
+      </c>
+      <c r="O8" s="42">
+        <v>1</v>
+      </c>
+      <c r="P8" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="37" t="str">
         <f t="shared" si="0"/>
         <v>0111</v>
       </c>
-      <c r="R8" s="34">
-        <v>0</v>
-      </c>
-      <c r="S8" s="34">
-        <v>0</v>
-      </c>
-      <c r="T8" s="34">
-        <v>0</v>
-      </c>
-      <c r="U8" s="34">
-        <v>1</v>
-      </c>
-      <c r="V8" s="34">
-        <v>0</v>
-      </c>
-      <c r="W8" s="34">
-        <v>0</v>
-      </c>
-      <c r="X8" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="34">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="34">
+      <c r="R8" s="33">
+        <v>0</v>
+      </c>
+      <c r="S8" s="33">
+        <v>0</v>
+      </c>
+      <c r="T8" s="33">
+        <v>0</v>
+      </c>
+      <c r="U8" s="33">
+        <v>1</v>
+      </c>
+      <c r="V8" s="33">
+        <v>0</v>
+      </c>
+      <c r="W8" s="33">
+        <v>0</v>
+      </c>
+      <c r="X8" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="33">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="33">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="33">
         <v>0</v>
       </c>
       <c r="AC8" s="8">
@@ -2061,53 +2066,53 @@
         <v>183</v>
       </c>
       <c r="L9" s="16"/>
-      <c r="M9" s="30">
-        <v>0</v>
-      </c>
-      <c r="N9" s="33">
-        <v>0</v>
-      </c>
-      <c r="O9" s="47">
-        <v>1</v>
-      </c>
-      <c r="P9" s="33">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="39" t="str">
+      <c r="M9" s="29">
+        <v>0</v>
+      </c>
+      <c r="N9" s="32">
+        <v>0</v>
+      </c>
+      <c r="O9" s="46">
+        <v>1</v>
+      </c>
+      <c r="P9" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="38" t="str">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="R9" s="33">
-        <v>0</v>
-      </c>
-      <c r="S9" s="33">
-        <v>0</v>
-      </c>
-      <c r="T9" s="33">
-        <v>0</v>
-      </c>
-      <c r="U9" s="33">
-        <v>1</v>
-      </c>
-      <c r="V9" s="33">
-        <v>0</v>
-      </c>
-      <c r="W9" s="33">
-        <v>0</v>
-      </c>
-      <c r="X9" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="33">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="33">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="41">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="33">
+      <c r="R9" s="32">
+        <v>0</v>
+      </c>
+      <c r="S9" s="32">
+        <v>0</v>
+      </c>
+      <c r="T9" s="32">
+        <v>0</v>
+      </c>
+      <c r="U9" s="32">
+        <v>1</v>
+      </c>
+      <c r="V9" s="32">
+        <v>0</v>
+      </c>
+      <c r="W9" s="32">
+        <v>0</v>
+      </c>
+      <c r="X9" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="32">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="32">
         <v>0</v>
       </c>
       <c r="AC9" s="8">
@@ -2147,53 +2152,53 @@
         <v>182</v>
       </c>
       <c r="L10" s="16"/>
-      <c r="M10" s="31">
-        <v>0</v>
-      </c>
-      <c r="N10" s="34">
-        <v>0</v>
-      </c>
-      <c r="O10" s="43">
-        <v>1</v>
-      </c>
-      <c r="P10" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="38" t="str">
+      <c r="M10" s="30">
+        <v>0</v>
+      </c>
+      <c r="N10" s="33">
+        <v>0</v>
+      </c>
+      <c r="O10" s="42">
+        <v>1</v>
+      </c>
+      <c r="P10" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="37" t="str">
         <f t="shared" si="0"/>
         <v>1001</v>
       </c>
-      <c r="R10" s="34">
-        <v>0</v>
-      </c>
-      <c r="S10" s="34">
-        <v>0</v>
-      </c>
-      <c r="T10" s="34">
-        <v>0</v>
-      </c>
-      <c r="U10" s="34">
-        <v>1</v>
-      </c>
-      <c r="V10" s="34">
-        <v>0</v>
-      </c>
-      <c r="W10" s="34">
-        <v>0</v>
-      </c>
-      <c r="X10" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="34">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="34">
+      <c r="R10" s="33">
+        <v>0</v>
+      </c>
+      <c r="S10" s="33">
+        <v>0</v>
+      </c>
+      <c r="T10" s="33">
+        <v>0</v>
+      </c>
+      <c r="U10" s="33">
+        <v>1</v>
+      </c>
+      <c r="V10" s="33">
+        <v>0</v>
+      </c>
+      <c r="W10" s="33">
+        <v>0</v>
+      </c>
+      <c r="X10" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="33">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="33">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="33">
         <v>0</v>
       </c>
       <c r="AC10" s="8">
@@ -2233,53 +2238,53 @@
         <v>184</v>
       </c>
       <c r="L11" s="16"/>
-      <c r="M11" s="30">
-        <v>1</v>
-      </c>
-      <c r="N11" s="48">
-        <v>0</v>
-      </c>
-      <c r="O11" s="47">
-        <v>1</v>
-      </c>
-      <c r="P11" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="39" t="str">
+      <c r="M11" s="29">
+        <v>1</v>
+      </c>
+      <c r="N11" s="47">
+        <v>0</v>
+      </c>
+      <c r="O11" s="46">
+        <v>1</v>
+      </c>
+      <c r="P11" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="38" t="str">
         <f t="shared" si="0"/>
         <v>1010</v>
       </c>
-      <c r="R11" s="48">
-        <v>0</v>
-      </c>
-      <c r="S11" s="48">
-        <v>0</v>
-      </c>
-      <c r="T11" s="48">
-        <v>0</v>
-      </c>
-      <c r="U11" s="48">
-        <v>1</v>
-      </c>
-      <c r="V11" s="48">
-        <v>0</v>
-      </c>
-      <c r="W11" s="48">
-        <v>0</v>
-      </c>
-      <c r="X11" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="48">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="48">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="48">
+      <c r="R11" s="47">
+        <v>0</v>
+      </c>
+      <c r="S11" s="47">
+        <v>0</v>
+      </c>
+      <c r="T11" s="47">
+        <v>0</v>
+      </c>
+      <c r="U11" s="47">
+        <v>1</v>
+      </c>
+      <c r="V11" s="47">
+        <v>0</v>
+      </c>
+      <c r="W11" s="47">
+        <v>0</v>
+      </c>
+      <c r="X11" s="47">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="47">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="47">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="47">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="47">
         <v>0</v>
       </c>
       <c r="AC11" s="8">
@@ -2319,53 +2324,53 @@
         <v>184</v>
       </c>
       <c r="L12" s="16"/>
-      <c r="M12" s="31">
-        <v>0</v>
-      </c>
-      <c r="N12" s="34">
-        <v>0</v>
-      </c>
-      <c r="O12" s="43">
-        <v>1</v>
-      </c>
-      <c r="P12" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="38" t="str">
+      <c r="M12" s="30">
+        <v>0</v>
+      </c>
+      <c r="N12" s="33">
+        <v>0</v>
+      </c>
+      <c r="O12" s="42">
+        <v>1</v>
+      </c>
+      <c r="P12" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="37" t="str">
         <f t="shared" si="0"/>
         <v>1010</v>
       </c>
-      <c r="R12" s="34">
-        <v>0</v>
-      </c>
-      <c r="S12" s="34">
-        <v>0</v>
-      </c>
-      <c r="T12" s="34">
-        <v>0</v>
-      </c>
-      <c r="U12" s="34">
-        <v>1</v>
-      </c>
-      <c r="V12" s="34">
-        <v>0</v>
-      </c>
-      <c r="W12" s="34">
-        <v>0</v>
-      </c>
-      <c r="X12" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="34">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="34">
+      <c r="R12" s="33">
+        <v>0</v>
+      </c>
+      <c r="S12" s="33">
+        <v>0</v>
+      </c>
+      <c r="T12" s="33">
+        <v>0</v>
+      </c>
+      <c r="U12" s="33">
+        <v>1</v>
+      </c>
+      <c r="V12" s="33">
+        <v>0</v>
+      </c>
+      <c r="W12" s="33">
+        <v>0</v>
+      </c>
+      <c r="X12" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="33">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="33">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="33">
         <v>0</v>
       </c>
       <c r="AC12" s="8">
@@ -2405,53 +2410,53 @@
         <v>185</v>
       </c>
       <c r="L13" s="16"/>
-      <c r="M13" s="30">
-        <v>1</v>
-      </c>
-      <c r="N13" s="48">
-        <v>0</v>
-      </c>
-      <c r="O13" s="47">
-        <v>1</v>
-      </c>
-      <c r="P13" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="39" t="str">
+      <c r="M13" s="29">
+        <v>1</v>
+      </c>
+      <c r="N13" s="47">
+        <v>0</v>
+      </c>
+      <c r="O13" s="46">
+        <v>1</v>
+      </c>
+      <c r="P13" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="38" t="str">
         <f t="shared" si="0"/>
         <v>1011</v>
       </c>
-      <c r="R13" s="48">
-        <v>0</v>
-      </c>
-      <c r="S13" s="48">
-        <v>0</v>
-      </c>
-      <c r="T13" s="48">
-        <v>0</v>
-      </c>
-      <c r="U13" s="48">
-        <v>1</v>
-      </c>
-      <c r="V13" s="48">
-        <v>0</v>
-      </c>
-      <c r="W13" s="48">
-        <v>0</v>
-      </c>
-      <c r="X13" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="48">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="48">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="48">
+      <c r="R13" s="47">
+        <v>0</v>
+      </c>
+      <c r="S13" s="47">
+        <v>0</v>
+      </c>
+      <c r="T13" s="47">
+        <v>0</v>
+      </c>
+      <c r="U13" s="47">
+        <v>1</v>
+      </c>
+      <c r="V13" s="47">
+        <v>0</v>
+      </c>
+      <c r="W13" s="47">
+        <v>0</v>
+      </c>
+      <c r="X13" s="47">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="47">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="47">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="47">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="47">
         <v>0</v>
       </c>
       <c r="AC13" s="8">
@@ -2491,53 +2496,53 @@
         <v>185</v>
       </c>
       <c r="L14" s="16"/>
-      <c r="M14" s="32">
-        <v>0</v>
-      </c>
-      <c r="N14" s="34">
-        <v>0</v>
-      </c>
-      <c r="O14" s="43">
-        <v>1</v>
-      </c>
-      <c r="P14" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="40" t="str">
+      <c r="M14" s="31">
+        <v>0</v>
+      </c>
+      <c r="N14" s="33">
+        <v>0</v>
+      </c>
+      <c r="O14" s="42">
+        <v>1</v>
+      </c>
+      <c r="P14" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="39" t="str">
         <f t="shared" si="0"/>
         <v>1011</v>
       </c>
-      <c r="R14" s="34">
-        <v>0</v>
-      </c>
-      <c r="S14" s="34">
-        <v>0</v>
-      </c>
-      <c r="T14" s="34">
-        <v>0</v>
-      </c>
-      <c r="U14" s="34">
-        <v>1</v>
-      </c>
-      <c r="V14" s="34">
-        <v>0</v>
-      </c>
-      <c r="W14" s="34">
-        <v>0</v>
-      </c>
-      <c r="X14" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="34">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="34">
+      <c r="R14" s="33">
+        <v>0</v>
+      </c>
+      <c r="S14" s="33">
+        <v>0</v>
+      </c>
+      <c r="T14" s="33">
+        <v>0</v>
+      </c>
+      <c r="U14" s="33">
+        <v>1</v>
+      </c>
+      <c r="V14" s="33">
+        <v>0</v>
+      </c>
+      <c r="W14" s="33">
+        <v>0</v>
+      </c>
+      <c r="X14" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="33">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="33">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="33">
         <v>0</v>
       </c>
       <c r="AC14" s="8">
@@ -2577,53 +2582,53 @@
         <v>188</v>
       </c>
       <c r="L15" s="16"/>
-      <c r="M15" s="30">
-        <v>1</v>
-      </c>
-      <c r="N15" s="48">
-        <v>0</v>
-      </c>
-      <c r="O15" s="47">
-        <v>1</v>
-      </c>
-      <c r="P15" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="39" t="str">
+      <c r="M15" s="29">
+        <v>1</v>
+      </c>
+      <c r="N15" s="47">
+        <v>0</v>
+      </c>
+      <c r="O15" s="46">
+        <v>1</v>
+      </c>
+      <c r="P15" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="38" t="str">
         <f t="shared" si="0"/>
         <v>1100</v>
       </c>
-      <c r="R15" s="48">
-        <v>0</v>
-      </c>
-      <c r="S15" s="48">
-        <v>0</v>
-      </c>
-      <c r="T15" s="48">
-        <v>0</v>
-      </c>
-      <c r="U15" s="48">
-        <v>1</v>
-      </c>
-      <c r="V15" s="48">
-        <v>0</v>
-      </c>
-      <c r="W15" s="48">
-        <v>0</v>
-      </c>
-      <c r="X15" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="48">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="48">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="48">
+      <c r="R15" s="47">
+        <v>0</v>
+      </c>
+      <c r="S15" s="47">
+        <v>0</v>
+      </c>
+      <c r="T15" s="47">
+        <v>0</v>
+      </c>
+      <c r="U15" s="47">
+        <v>1</v>
+      </c>
+      <c r="V15" s="47">
+        <v>0</v>
+      </c>
+      <c r="W15" s="47">
+        <v>0</v>
+      </c>
+      <c r="X15" s="47">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="47">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="47">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="47">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="47">
         <v>0</v>
       </c>
       <c r="AC15" s="8">
@@ -2663,53 +2668,53 @@
         <v>188</v>
       </c>
       <c r="L16" s="16"/>
-      <c r="M16" s="32">
-        <v>0</v>
-      </c>
-      <c r="N16" s="34">
-        <v>0</v>
-      </c>
-      <c r="O16" s="43">
-        <v>1</v>
-      </c>
-      <c r="P16" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="40" t="str">
+      <c r="M16" s="31">
+        <v>0</v>
+      </c>
+      <c r="N16" s="33">
+        <v>0</v>
+      </c>
+      <c r="O16" s="42">
+        <v>1</v>
+      </c>
+      <c r="P16" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="39" t="str">
         <f t="shared" si="0"/>
         <v>1100</v>
       </c>
-      <c r="R16" s="34">
-        <v>0</v>
-      </c>
-      <c r="S16" s="34">
-        <v>0</v>
-      </c>
-      <c r="T16" s="34">
-        <v>0</v>
-      </c>
-      <c r="U16" s="34">
-        <v>1</v>
-      </c>
-      <c r="V16" s="34">
-        <v>0</v>
-      </c>
-      <c r="W16" s="34">
-        <v>0</v>
-      </c>
-      <c r="X16" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="34">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="34">
+      <c r="R16" s="33">
+        <v>0</v>
+      </c>
+      <c r="S16" s="33">
+        <v>0</v>
+      </c>
+      <c r="T16" s="33">
+        <v>0</v>
+      </c>
+      <c r="U16" s="33">
+        <v>1</v>
+      </c>
+      <c r="V16" s="33">
+        <v>0</v>
+      </c>
+      <c r="W16" s="33">
+        <v>0</v>
+      </c>
+      <c r="X16" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="33">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="33">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="33">
         <v>0</v>
       </c>
       <c r="AC16" s="8">
@@ -2749,53 +2754,53 @@
         <v>187</v>
       </c>
       <c r="L17" s="16"/>
-      <c r="M17" s="30">
-        <v>1</v>
-      </c>
-      <c r="N17" s="48">
-        <v>0</v>
-      </c>
-      <c r="O17" s="47">
-        <v>1</v>
-      </c>
-      <c r="P17" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="39" t="str">
+      <c r="M17" s="29">
+        <v>1</v>
+      </c>
+      <c r="N17" s="47">
+        <v>0</v>
+      </c>
+      <c r="O17" s="46">
+        <v>1</v>
+      </c>
+      <c r="P17" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="38" t="str">
         <f t="shared" si="0"/>
         <v>1101</v>
       </c>
-      <c r="R17" s="48">
-        <v>0</v>
-      </c>
-      <c r="S17" s="48">
-        <v>0</v>
-      </c>
-      <c r="T17" s="48">
-        <v>0</v>
-      </c>
-      <c r="U17" s="48">
-        <v>1</v>
-      </c>
-      <c r="V17" s="48">
-        <v>0</v>
-      </c>
-      <c r="W17" s="48">
-        <v>0</v>
-      </c>
-      <c r="X17" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="48">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="48">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="48">
+      <c r="R17" s="47">
+        <v>0</v>
+      </c>
+      <c r="S17" s="47">
+        <v>0</v>
+      </c>
+      <c r="T17" s="47">
+        <v>0</v>
+      </c>
+      <c r="U17" s="47">
+        <v>1</v>
+      </c>
+      <c r="V17" s="47">
+        <v>0</v>
+      </c>
+      <c r="W17" s="47">
+        <v>0</v>
+      </c>
+      <c r="X17" s="47">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="47">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="47">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="47">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="47">
         <v>0</v>
       </c>
       <c r="AC17" s="8">
@@ -2835,53 +2840,53 @@
         <v>187</v>
       </c>
       <c r="L18" s="16"/>
-      <c r="M18" s="32">
-        <v>0</v>
-      </c>
-      <c r="N18" s="34">
-        <v>0</v>
-      </c>
-      <c r="O18" s="43">
-        <v>1</v>
-      </c>
-      <c r="P18" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="40" t="str">
+      <c r="M18" s="31">
+        <v>0</v>
+      </c>
+      <c r="N18" s="33">
+        <v>0</v>
+      </c>
+      <c r="O18" s="42">
+        <v>1</v>
+      </c>
+      <c r="P18" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="39" t="str">
         <f t="shared" si="0"/>
         <v>1101</v>
       </c>
-      <c r="R18" s="34">
-        <v>0</v>
-      </c>
-      <c r="S18" s="34">
-        <v>0</v>
-      </c>
-      <c r="T18" s="34">
-        <v>0</v>
-      </c>
-      <c r="U18" s="34">
-        <v>1</v>
-      </c>
-      <c r="V18" s="34">
-        <v>0</v>
-      </c>
-      <c r="W18" s="34">
-        <v>0</v>
-      </c>
-      <c r="X18" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="34">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="34">
+      <c r="R18" s="33">
+        <v>0</v>
+      </c>
+      <c r="S18" s="33">
+        <v>0</v>
+      </c>
+      <c r="T18" s="33">
+        <v>0</v>
+      </c>
+      <c r="U18" s="33">
+        <v>1</v>
+      </c>
+      <c r="V18" s="33">
+        <v>0</v>
+      </c>
+      <c r="W18" s="33">
+        <v>0</v>
+      </c>
+      <c r="X18" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="33">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="33">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="33">
         <v>0</v>
       </c>
       <c r="AC18" s="8">
@@ -2921,53 +2926,53 @@
         <v>186</v>
       </c>
       <c r="L19" s="16"/>
-      <c r="M19" s="30">
-        <v>0</v>
-      </c>
-      <c r="N19" s="48">
-        <v>0</v>
-      </c>
-      <c r="O19" s="47">
-        <v>1</v>
-      </c>
-      <c r="P19" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="39" t="str">
+      <c r="M19" s="29">
+        <v>0</v>
+      </c>
+      <c r="N19" s="47">
+        <v>0</v>
+      </c>
+      <c r="O19" s="46">
+        <v>1</v>
+      </c>
+      <c r="P19" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="38" t="str">
         <f t="shared" si="0"/>
         <v>1110</v>
       </c>
-      <c r="R19" s="48">
-        <v>0</v>
-      </c>
-      <c r="S19" s="48">
-        <v>0</v>
-      </c>
-      <c r="T19" s="48">
-        <v>0</v>
-      </c>
-      <c r="U19" s="48">
-        <v>1</v>
-      </c>
-      <c r="V19" s="48">
-        <v>0</v>
-      </c>
-      <c r="W19" s="48">
-        <v>0</v>
-      </c>
-      <c r="X19" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="48">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="48">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="48">
+      <c r="R19" s="47">
+        <v>0</v>
+      </c>
+      <c r="S19" s="47">
+        <v>0</v>
+      </c>
+      <c r="T19" s="47">
+        <v>0</v>
+      </c>
+      <c r="U19" s="47">
+        <v>1</v>
+      </c>
+      <c r="V19" s="47">
+        <v>0</v>
+      </c>
+      <c r="W19" s="47">
+        <v>0</v>
+      </c>
+      <c r="X19" s="47">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="47">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="47">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="47">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="47">
         <v>0</v>
       </c>
       <c r="AC19" s="8">
@@ -3007,53 +3012,53 @@
         <v>186</v>
       </c>
       <c r="L20" s="16"/>
-      <c r="M20" s="32">
-        <v>0</v>
-      </c>
-      <c r="N20" s="34">
-        <v>0</v>
-      </c>
-      <c r="O20" s="43">
-        <v>1</v>
-      </c>
-      <c r="P20" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="40" t="str">
+      <c r="M20" s="31">
+        <v>0</v>
+      </c>
+      <c r="N20" s="33">
+        <v>0</v>
+      </c>
+      <c r="O20" s="42">
+        <v>1</v>
+      </c>
+      <c r="P20" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="39" t="str">
         <f t="shared" si="0"/>
         <v>1110</v>
       </c>
-      <c r="R20" s="34">
-        <v>0</v>
-      </c>
-      <c r="S20" s="34">
-        <v>0</v>
-      </c>
-      <c r="T20" s="34">
-        <v>0</v>
-      </c>
-      <c r="U20" s="34">
-        <v>1</v>
-      </c>
-      <c r="V20" s="34">
-        <v>0</v>
-      </c>
-      <c r="W20" s="34">
-        <v>0</v>
-      </c>
-      <c r="X20" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="34">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="34">
+      <c r="R20" s="33">
+        <v>0</v>
+      </c>
+      <c r="S20" s="33">
+        <v>0</v>
+      </c>
+      <c r="T20" s="33">
+        <v>0</v>
+      </c>
+      <c r="U20" s="33">
+        <v>1</v>
+      </c>
+      <c r="V20" s="33">
+        <v>0</v>
+      </c>
+      <c r="W20" s="33">
+        <v>0</v>
+      </c>
+      <c r="X20" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="33">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="33">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="33">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="33">
         <v>0</v>
       </c>
       <c r="AC20" s="8">
@@ -3089,13 +3094,13 @@
       <c r="J21" s="14"/>
       <c r="K21" s="15"/>
       <c r="L21" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="M21" s="30">
-        <v>0</v>
-      </c>
-      <c r="N21" s="48"/>
-      <c r="Q21" s="39"/>
+        <v>204</v>
+      </c>
+      <c r="M21" s="29">
+        <v>0</v>
+      </c>
+      <c r="N21" s="47"/>
+      <c r="Q21" s="38"/>
     </row>
     <row r="22" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17"/>
@@ -3126,60 +3131,60 @@
       <c r="J22" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K22" s="49">
+      <c r="K22" s="48">
         <v>0</v>
       </c>
       <c r="L22" s="16"/>
-      <c r="M22" s="32">
-        <v>0</v>
-      </c>
-      <c r="N22" s="35">
-        <v>0</v>
-      </c>
-      <c r="O22" s="45">
+      <c r="M22" s="31">
+        <v>0</v>
+      </c>
+      <c r="N22" s="34">
+        <v>0</v>
+      </c>
+      <c r="O22" s="44">
         <v>10</v>
       </c>
-      <c r="P22" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="50">
+      <c r="P22" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="49">
         <f>K22</f>
         <v>0</v>
       </c>
-      <c r="R22" s="35">
-        <v>0</v>
-      </c>
-      <c r="S22" s="35">
-        <v>0</v>
-      </c>
-      <c r="T22" s="35">
-        <v>0</v>
-      </c>
-      <c r="U22" s="35">
-        <v>1</v>
-      </c>
-      <c r="V22" s="35">
-        <v>0</v>
-      </c>
-      <c r="W22" s="35">
-        <v>0</v>
-      </c>
-      <c r="X22" s="35">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="35">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="42">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="35">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="29">
+      <c r="R22" s="34">
+        <v>0</v>
+      </c>
+      <c r="S22" s="34">
+        <v>0</v>
+      </c>
+      <c r="T22" s="34">
+        <v>0</v>
+      </c>
+      <c r="U22" s="34">
+        <v>1</v>
+      </c>
+      <c r="V22" s="34">
+        <v>0</v>
+      </c>
+      <c r="W22" s="34">
+        <v>0</v>
+      </c>
+      <c r="X22" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="34">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="28">
         <v>1</v>
       </c>
     </row>
@@ -3212,57 +3217,57 @@
       <c r="J23" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K23" s="49">
+      <c r="K23" s="48">
         <v>0</v>
       </c>
       <c r="L23" s="16"/>
-      <c r="M23" s="30">
-        <v>0</v>
-      </c>
-      <c r="N23" s="33">
-        <v>0</v>
-      </c>
-      <c r="O23" s="44">
+      <c r="M23" s="29">
+        <v>0</v>
+      </c>
+      <c r="N23" s="32">
+        <v>0</v>
+      </c>
+      <c r="O23" s="43">
         <v>10</v>
       </c>
-      <c r="P23" s="33">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="51">
+      <c r="P23" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="50">
         <f>K23</f>
         <v>0</v>
       </c>
-      <c r="R23" s="33">
-        <v>0</v>
-      </c>
-      <c r="S23" s="33">
-        <v>0</v>
-      </c>
-      <c r="T23" s="33">
-        <v>0</v>
-      </c>
-      <c r="U23" s="33">
-        <v>1</v>
-      </c>
-      <c r="V23" s="33">
-        <v>0</v>
-      </c>
-      <c r="W23" s="33">
-        <v>0</v>
-      </c>
-      <c r="X23" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="33">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="33">
-        <v>0</v>
-      </c>
-      <c r="AA23" s="41">
-        <v>0</v>
-      </c>
-      <c r="AB23" s="33">
+      <c r="R23" s="32">
+        <v>0</v>
+      </c>
+      <c r="S23" s="32">
+        <v>0</v>
+      </c>
+      <c r="T23" s="32">
+        <v>0</v>
+      </c>
+      <c r="U23" s="32">
+        <v>1</v>
+      </c>
+      <c r="V23" s="32">
+        <v>0</v>
+      </c>
+      <c r="W23" s="32">
+        <v>0</v>
+      </c>
+      <c r="X23" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="32">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="32">
         <v>0</v>
       </c>
       <c r="AC23" s="8">
@@ -3298,24 +3303,24 @@
       <c r="J24" s="14"/>
       <c r="K24" s="15"/>
       <c r="L24" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="M24" s="32"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="46"/>
-      <c r="P24" s="35"/>
-      <c r="Q24" s="40"/>
-      <c r="R24" s="35"/>
-      <c r="S24" s="35"/>
-      <c r="T24" s="35"/>
-      <c r="U24" s="35"/>
-      <c r="V24" s="35"/>
-      <c r="W24" s="35"/>
-      <c r="X24" s="35"/>
-      <c r="Y24" s="35"/>
-      <c r="Z24" s="35"/>
-      <c r="AA24" s="42"/>
-      <c r="AB24" s="35"/>
+        <v>204</v>
+      </c>
+      <c r="M24" s="31"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="45"/>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="39"/>
+      <c r="R24" s="34"/>
+      <c r="S24" s="34"/>
+      <c r="T24" s="34"/>
+      <c r="U24" s="34"/>
+      <c r="V24" s="34"/>
+      <c r="W24" s="34"/>
+      <c r="X24" s="34"/>
+      <c r="Y24" s="34"/>
+      <c r="Z24" s="34"/>
+      <c r="AA24" s="41"/>
+      <c r="AB24" s="34"/>
     </row>
     <row r="25" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="23"/>
@@ -3346,9 +3351,9 @@
       <c r="J25" s="14"/>
       <c r="K25" s="15"/>
       <c r="L25" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q25" s="39"/>
+        <v>204</v>
+      </c>
+      <c r="Q25" s="38"/>
     </row>
     <row r="26" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="23"/>
@@ -3379,24 +3384,24 @@
       <c r="J26" s="14"/>
       <c r="K26" s="15"/>
       <c r="L26" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="M26" s="32"/>
-      <c r="N26" s="35"/>
-      <c r="O26" s="46"/>
-      <c r="P26" s="35"/>
-      <c r="Q26" s="40"/>
-      <c r="R26" s="35"/>
-      <c r="S26" s="35"/>
-      <c r="T26" s="35"/>
-      <c r="U26" s="35"/>
-      <c r="V26" s="35"/>
-      <c r="W26" s="35"/>
-      <c r="X26" s="35"/>
-      <c r="Y26" s="35"/>
-      <c r="Z26" s="35"/>
-      <c r="AA26" s="42"/>
-      <c r="AB26" s="35"/>
+        <v>204</v>
+      </c>
+      <c r="M26" s="31"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="45"/>
+      <c r="P26" s="34"/>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="34"/>
+      <c r="S26" s="34"/>
+      <c r="T26" s="34"/>
+      <c r="U26" s="34"/>
+      <c r="V26" s="34"/>
+      <c r="W26" s="34"/>
+      <c r="X26" s="34"/>
+      <c r="Y26" s="34"/>
+      <c r="Z26" s="34"/>
+      <c r="AA26" s="41"/>
+      <c r="AB26" s="34"/>
     </row>
     <row r="27" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="23"/>
@@ -3427,9 +3432,9 @@
       <c r="J27" s="14"/>
       <c r="K27" s="15"/>
       <c r="L27" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q27" s="39"/>
+        <v>204</v>
+      </c>
+      <c r="Q27" s="38"/>
     </row>
     <row r="28" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
@@ -3462,27 +3467,27 @@
         <v>175</v>
       </c>
       <c r="L28" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="M28" s="32"/>
-      <c r="N28" s="35"/>
-      <c r="O28" s="46"/>
-      <c r="P28" s="35"/>
-      <c r="Q28" s="40" t="str">
+        <v>204</v>
+      </c>
+      <c r="M28" s="31"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="45"/>
+      <c r="P28" s="34"/>
+      <c r="Q28" s="39" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
-      <c r="R28" s="35"/>
-      <c r="S28" s="35"/>
-      <c r="T28" s="35"/>
-      <c r="U28" s="35"/>
-      <c r="V28" s="35"/>
-      <c r="W28" s="35"/>
-      <c r="X28" s="35"/>
-      <c r="Y28" s="35"/>
-      <c r="Z28" s="35"/>
-      <c r="AA28" s="42"/>
-      <c r="AB28" s="35"/>
+      <c r="R28" s="34"/>
+      <c r="S28" s="34"/>
+      <c r="T28" s="34"/>
+      <c r="U28" s="34"/>
+      <c r="V28" s="34"/>
+      <c r="W28" s="34"/>
+      <c r="X28" s="34"/>
+      <c r="Y28" s="34"/>
+      <c r="Z28" s="34"/>
+      <c r="AA28" s="41"/>
+      <c r="AB28" s="34"/>
     </row>
     <row r="29" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20"/>
@@ -3512,10 +3517,10 @@
       <c r="K29" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="L29" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q29" s="39" t="str">
+      <c r="L29" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q29" s="38" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
@@ -3545,27 +3550,27 @@
         <v>122</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="M30" s="32"/>
-      <c r="N30" s="35"/>
-      <c r="O30" s="46"/>
-      <c r="P30" s="35"/>
-      <c r="Q30" s="40" t="str">
+        <v>204</v>
+      </c>
+      <c r="M30" s="31"/>
+      <c r="N30" s="34"/>
+      <c r="O30" s="45"/>
+      <c r="P30" s="34"/>
+      <c r="Q30" s="39" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="R30" s="35"/>
-      <c r="S30" s="35"/>
-      <c r="T30" s="35"/>
-      <c r="U30" s="35"/>
-      <c r="V30" s="35"/>
-      <c r="W30" s="35"/>
-      <c r="X30" s="35"/>
-      <c r="Y30" s="35"/>
-      <c r="Z30" s="35"/>
-      <c r="AA30" s="42"/>
-      <c r="AB30" s="35"/>
+      <c r="R30" s="34"/>
+      <c r="S30" s="34"/>
+      <c r="T30" s="34"/>
+      <c r="U30" s="34"/>
+      <c r="V30" s="34"/>
+      <c r="W30" s="34"/>
+      <c r="X30" s="34"/>
+      <c r="Y30" s="34"/>
+      <c r="Z30" s="34"/>
+      <c r="AA30" s="41"/>
+      <c r="AB30" s="34"/>
     </row>
     <row r="31" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20"/>
@@ -3592,9 +3597,9 @@
         <v>122</v>
       </c>
       <c r="L31" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q31" s="39" t="str">
+        <v>204</v>
+      </c>
+      <c r="Q31" s="38" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
@@ -3628,27 +3633,27 @@
         <v>175</v>
       </c>
       <c r="L32" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="M32" s="32"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="46"/>
-      <c r="P32" s="35"/>
-      <c r="Q32" s="40" t="str">
+        <v>204</v>
+      </c>
+      <c r="M32" s="31"/>
+      <c r="N32" s="34"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="34"/>
+      <c r="Q32" s="39" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
-      <c r="R32" s="35"/>
-      <c r="S32" s="35"/>
-      <c r="T32" s="35"/>
-      <c r="U32" s="35"/>
-      <c r="V32" s="35"/>
-      <c r="W32" s="35"/>
-      <c r="X32" s="35"/>
-      <c r="Y32" s="35"/>
-      <c r="Z32" s="35"/>
-      <c r="AA32" s="42"/>
-      <c r="AB32" s="35"/>
+      <c r="R32" s="34"/>
+      <c r="S32" s="34"/>
+      <c r="T32" s="34"/>
+      <c r="U32" s="34"/>
+      <c r="V32" s="34"/>
+      <c r="W32" s="34"/>
+      <c r="X32" s="34"/>
+      <c r="Y32" s="34"/>
+      <c r="Z32" s="34"/>
+      <c r="AA32" s="41"/>
+      <c r="AB32" s="34"/>
     </row>
     <row r="33" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="21"/>
@@ -3679,9 +3684,9 @@
         <v>175</v>
       </c>
       <c r="L33" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q33" s="39" t="str">
+        <v>204</v>
+      </c>
+      <c r="Q33" s="38" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
@@ -3715,27 +3720,27 @@
         <v>175</v>
       </c>
       <c r="L34" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="M34" s="32"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="46"/>
-      <c r="P34" s="35"/>
-      <c r="Q34" s="40" t="str">
+        <v>204</v>
+      </c>
+      <c r="M34" s="31"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="34"/>
+      <c r="Q34" s="39" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
-      <c r="R34" s="35"/>
-      <c r="S34" s="35"/>
-      <c r="T34" s="35"/>
-      <c r="U34" s="35"/>
-      <c r="V34" s="35"/>
-      <c r="W34" s="35"/>
-      <c r="X34" s="35"/>
-      <c r="Y34" s="35"/>
-      <c r="Z34" s="35"/>
-      <c r="AA34" s="42"/>
-      <c r="AB34" s="35"/>
+      <c r="R34" s="34"/>
+      <c r="S34" s="34"/>
+      <c r="T34" s="34"/>
+      <c r="U34" s="34"/>
+      <c r="V34" s="34"/>
+      <c r="W34" s="34"/>
+      <c r="X34" s="34"/>
+      <c r="Y34" s="34"/>
+      <c r="Z34" s="34"/>
+      <c r="AA34" s="41"/>
+      <c r="AB34" s="34"/>
     </row>
     <row r="35" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21"/>
@@ -3766,9 +3771,9 @@
         <v>175</v>
       </c>
       <c r="L35" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q35" s="39" t="str">
+        <v>204</v>
+      </c>
+      <c r="Q35" s="38" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
@@ -3802,53 +3807,53 @@
         <v>174</v>
       </c>
       <c r="L36" s="16"/>
-      <c r="M36" s="32">
-        <v>0</v>
-      </c>
-      <c r="N36" s="35">
-        <v>0</v>
-      </c>
-      <c r="O36" s="46">
-        <v>0</v>
-      </c>
-      <c r="P36" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="40" t="str">
+      <c r="M36" s="31">
+        <v>0</v>
+      </c>
+      <c r="N36" s="34">
+        <v>0</v>
+      </c>
+      <c r="O36" s="45">
+        <v>0</v>
+      </c>
+      <c r="P36" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="39" t="str">
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R36" s="35">
-        <v>0</v>
-      </c>
-      <c r="S36" s="35">
-        <v>0</v>
-      </c>
-      <c r="T36" s="35">
-        <v>0</v>
-      </c>
-      <c r="U36" s="35">
-        <v>1</v>
-      </c>
-      <c r="V36" s="35">
-        <v>0</v>
-      </c>
-      <c r="W36" s="35">
-        <v>0</v>
-      </c>
-      <c r="X36" s="35">
-        <v>0</v>
-      </c>
-      <c r="Y36" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z36" s="35">
-        <v>0</v>
-      </c>
-      <c r="AA36" s="42">
-        <v>0</v>
-      </c>
-      <c r="AB36" s="35">
+      <c r="R36" s="34">
+        <v>0</v>
+      </c>
+      <c r="S36" s="34">
+        <v>0</v>
+      </c>
+      <c r="T36" s="34">
+        <v>0</v>
+      </c>
+      <c r="U36" s="34">
+        <v>1</v>
+      </c>
+      <c r="V36" s="34">
+        <v>0</v>
+      </c>
+      <c r="W36" s="34">
+        <v>0</v>
+      </c>
+      <c r="X36" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="34">
         <v>0</v>
       </c>
       <c r="AC36" s="8">
@@ -3884,53 +3889,53 @@
         <v>174</v>
       </c>
       <c r="L37" s="16"/>
-      <c r="M37" s="30">
-        <v>1</v>
-      </c>
-      <c r="N37" s="33">
-        <v>0</v>
-      </c>
-      <c r="O37" s="44">
-        <v>0</v>
-      </c>
-      <c r="P37" s="33">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="39" t="str">
+      <c r="M37" s="29">
+        <v>1</v>
+      </c>
+      <c r="N37" s="32">
+        <v>0</v>
+      </c>
+      <c r="O37" s="43">
+        <v>0</v>
+      </c>
+      <c r="P37" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="38" t="str">
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R37" s="33">
-        <v>0</v>
-      </c>
-      <c r="S37" s="33">
-        <v>0</v>
-      </c>
-      <c r="T37" s="33">
-        <v>0</v>
-      </c>
-      <c r="U37" s="33">
-        <v>1</v>
-      </c>
-      <c r="V37" s="33">
-        <v>0</v>
-      </c>
-      <c r="W37" s="33">
-        <v>0</v>
-      </c>
-      <c r="X37" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y37" s="33">
-        <v>0</v>
-      </c>
-      <c r="Z37" s="33">
-        <v>0</v>
-      </c>
-      <c r="AA37" s="41">
-        <v>0</v>
-      </c>
-      <c r="AB37" s="33">
+      <c r="R37" s="32">
+        <v>0</v>
+      </c>
+      <c r="S37" s="32">
+        <v>0</v>
+      </c>
+      <c r="T37" s="32">
+        <v>0</v>
+      </c>
+      <c r="U37" s="32">
+        <v>1</v>
+      </c>
+      <c r="V37" s="32">
+        <v>0</v>
+      </c>
+      <c r="W37" s="32">
+        <v>0</v>
+      </c>
+      <c r="X37" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="32">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="32">
         <v>0</v>
       </c>
       <c r="AC37" s="8">
@@ -3966,53 +3971,53 @@
         <v>186</v>
       </c>
       <c r="L38" s="16"/>
-      <c r="M38" s="32">
-        <v>0</v>
-      </c>
-      <c r="N38" s="35">
-        <v>0</v>
-      </c>
-      <c r="O38" s="46">
-        <v>0</v>
-      </c>
-      <c r="P38" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="40" t="str">
+      <c r="M38" s="31">
+        <v>0</v>
+      </c>
+      <c r="N38" s="34">
+        <v>0</v>
+      </c>
+      <c r="O38" s="45">
+        <v>0</v>
+      </c>
+      <c r="P38" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="39" t="str">
         <f t="shared" si="0"/>
         <v>1110</v>
       </c>
-      <c r="R38" s="35">
-        <v>0</v>
-      </c>
-      <c r="S38" s="35">
-        <v>0</v>
-      </c>
-      <c r="T38" s="35">
-        <v>0</v>
-      </c>
-      <c r="U38" s="35">
-        <v>1</v>
-      </c>
-      <c r="V38" s="35">
-        <v>0</v>
-      </c>
-      <c r="W38" s="35">
-        <v>0</v>
-      </c>
-      <c r="X38" s="35">
-        <v>0</v>
-      </c>
-      <c r="Y38" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z38" s="35">
-        <v>0</v>
-      </c>
-      <c r="AA38" s="42">
-        <v>0</v>
-      </c>
-      <c r="AB38" s="35">
+      <c r="R38" s="34">
+        <v>0</v>
+      </c>
+      <c r="S38" s="34">
+        <v>0</v>
+      </c>
+      <c r="T38" s="34">
+        <v>0</v>
+      </c>
+      <c r="U38" s="34">
+        <v>1</v>
+      </c>
+      <c r="V38" s="34">
+        <v>0</v>
+      </c>
+      <c r="W38" s="34">
+        <v>0</v>
+      </c>
+      <c r="X38" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="34">
         <v>0</v>
       </c>
       <c r="AC38" s="8">
@@ -4048,53 +4053,53 @@
         <v>186</v>
       </c>
       <c r="L39" s="16"/>
-      <c r="M39" s="30">
-        <v>1</v>
-      </c>
-      <c r="N39" s="33">
-        <v>0</v>
-      </c>
-      <c r="O39" s="44">
-        <v>0</v>
-      </c>
-      <c r="P39" s="33">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="39" t="str">
+      <c r="M39" s="29">
+        <v>1</v>
+      </c>
+      <c r="N39" s="32">
+        <v>0</v>
+      </c>
+      <c r="O39" s="43">
+        <v>0</v>
+      </c>
+      <c r="P39" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="38" t="str">
         <f t="shared" si="0"/>
         <v>1110</v>
       </c>
-      <c r="R39" s="33">
-        <v>0</v>
-      </c>
-      <c r="S39" s="33">
-        <v>0</v>
-      </c>
-      <c r="T39" s="33">
-        <v>0</v>
-      </c>
-      <c r="U39" s="33">
-        <v>1</v>
-      </c>
-      <c r="V39" s="33">
-        <v>0</v>
-      </c>
-      <c r="W39" s="33">
-        <v>0</v>
-      </c>
-      <c r="X39" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y39" s="33">
-        <v>0</v>
-      </c>
-      <c r="Z39" s="33">
-        <v>0</v>
-      </c>
-      <c r="AA39" s="41">
-        <v>0</v>
-      </c>
-      <c r="AB39" s="33">
+      <c r="R39" s="32">
+        <v>0</v>
+      </c>
+      <c r="S39" s="32">
+        <v>0</v>
+      </c>
+      <c r="T39" s="32">
+        <v>0</v>
+      </c>
+      <c r="U39" s="32">
+        <v>1</v>
+      </c>
+      <c r="V39" s="32">
+        <v>0</v>
+      </c>
+      <c r="W39" s="32">
+        <v>0</v>
+      </c>
+      <c r="X39" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="32">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="32">
         <v>0</v>
       </c>
       <c r="AC39" s="8">
@@ -4130,27 +4135,58 @@
         <v>180</v>
       </c>
       <c r="L40" s="16"/>
-      <c r="M40" s="32"/>
-      <c r="N40" s="35"/>
-      <c r="O40" s="46">
-        <v>0</v>
-      </c>
-      <c r="P40" s="35"/>
-      <c r="Q40" s="40" t="str">
+      <c r="M40" s="31">
+        <v>0</v>
+      </c>
+      <c r="N40" s="34">
+        <v>0</v>
+      </c>
+      <c r="O40" s="45">
+        <v>0</v>
+      </c>
+      <c r="P40" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="39" t="str">
         <f t="shared" si="0"/>
         <v>0110</v>
       </c>
-      <c r="R40" s="35"/>
-      <c r="S40" s="35"/>
-      <c r="T40" s="35"/>
-      <c r="U40" s="35"/>
-      <c r="V40" s="35"/>
-      <c r="W40" s="35"/>
-      <c r="X40" s="35"/>
-      <c r="Y40" s="35"/>
-      <c r="Z40" s="35"/>
-      <c r="AA40" s="42"/>
-      <c r="AB40" s="35"/>
+      <c r="R40" s="34">
+        <v>0</v>
+      </c>
+      <c r="S40" s="34">
+        <v>0</v>
+      </c>
+      <c r="T40" s="34">
+        <v>0</v>
+      </c>
+      <c r="U40" s="34">
+        <v>1</v>
+      </c>
+      <c r="V40" s="34">
+        <v>0</v>
+      </c>
+      <c r="W40" s="34">
+        <v>0</v>
+      </c>
+      <c r="X40" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA40" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="34">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="41">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
@@ -4181,12 +4217,57 @@
         <v>181</v>
       </c>
       <c r="L41" s="16"/>
-      <c r="O41" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="39" t="str">
+      <c r="M41" s="29">
+        <v>0</v>
+      </c>
+      <c r="N41" s="32">
+        <v>0</v>
+      </c>
+      <c r="O41" s="43">
+        <v>0</v>
+      </c>
+      <c r="P41" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="38" t="str">
         <f t="shared" si="0"/>
         <v>0111</v>
+      </c>
+      <c r="R41" s="32">
+        <v>0</v>
+      </c>
+      <c r="S41" s="32">
+        <v>0</v>
+      </c>
+      <c r="T41" s="32">
+        <v>0</v>
+      </c>
+      <c r="U41" s="32">
+        <v>1</v>
+      </c>
+      <c r="V41" s="32">
+        <v>0</v>
+      </c>
+      <c r="W41" s="32">
+        <v>0</v>
+      </c>
+      <c r="X41" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="32">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA41" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="32">
+        <v>0</v>
+      </c>
+      <c r="AC41" s="51">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4218,27 +4299,58 @@
         <v>183</v>
       </c>
       <c r="L42" s="16"/>
-      <c r="M42" s="32"/>
-      <c r="N42" s="35"/>
-      <c r="O42" s="46">
-        <v>0</v>
-      </c>
-      <c r="P42" s="35"/>
-      <c r="Q42" s="40" t="str">
+      <c r="M42" s="31">
+        <v>0</v>
+      </c>
+      <c r="N42" s="34">
+        <v>0</v>
+      </c>
+      <c r="O42" s="45">
+        <v>0</v>
+      </c>
+      <c r="P42" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="39" t="str">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="R42" s="35"/>
-      <c r="S42" s="35"/>
-      <c r="T42" s="35"/>
-      <c r="U42" s="35"/>
-      <c r="V42" s="35"/>
-      <c r="W42" s="35"/>
-      <c r="X42" s="35"/>
-      <c r="Y42" s="35"/>
-      <c r="Z42" s="35"/>
-      <c r="AA42" s="42"/>
-      <c r="AB42" s="35"/>
+      <c r="R42" s="34">
+        <v>0</v>
+      </c>
+      <c r="S42" s="34">
+        <v>0</v>
+      </c>
+      <c r="T42" s="34">
+        <v>0</v>
+      </c>
+      <c r="U42" s="34">
+        <v>1</v>
+      </c>
+      <c r="V42" s="34">
+        <v>0</v>
+      </c>
+      <c r="W42" s="34">
+        <v>0</v>
+      </c>
+      <c r="X42" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA42" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB42" s="34">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="52">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="24"/>
@@ -4269,9 +4381,9 @@
         <v>122</v>
       </c>
       <c r="L43" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q43" s="39" t="str">
+        <v>204</v>
+      </c>
+      <c r="Q43" s="38" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
@@ -4309,27 +4421,58 @@
         <v>176</v>
       </c>
       <c r="L44" s="16"/>
-      <c r="M44" s="32"/>
-      <c r="N44" s="35"/>
-      <c r="O44" s="46">
-        <v>1</v>
-      </c>
-      <c r="P44" s="35"/>
-      <c r="Q44" s="40" t="str">
+      <c r="M44" s="31">
+        <v>0</v>
+      </c>
+      <c r="N44" s="34">
+        <v>0</v>
+      </c>
+      <c r="O44" s="45">
+        <v>1</v>
+      </c>
+      <c r="P44" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="39" t="str">
         <f t="shared" si="0"/>
         <v>0010</v>
       </c>
-      <c r="R44" s="35"/>
-      <c r="S44" s="35"/>
-      <c r="T44" s="35"/>
-      <c r="U44" s="35"/>
-      <c r="V44" s="35"/>
-      <c r="W44" s="35"/>
-      <c r="X44" s="35"/>
-      <c r="Y44" s="35"/>
-      <c r="Z44" s="35"/>
-      <c r="AA44" s="42"/>
-      <c r="AB44" s="35"/>
+      <c r="R44" s="34">
+        <v>0</v>
+      </c>
+      <c r="S44" s="34">
+        <v>0</v>
+      </c>
+      <c r="T44" s="34">
+        <v>0</v>
+      </c>
+      <c r="U44" s="34">
+        <v>1</v>
+      </c>
+      <c r="V44" s="34">
+        <v>0</v>
+      </c>
+      <c r="W44" s="34">
+        <v>0</v>
+      </c>
+      <c r="X44" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="34">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="41">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="10"/>
@@ -4364,12 +4507,57 @@
         <v>178</v>
       </c>
       <c r="L45" s="16"/>
-      <c r="O45" s="44">
-        <v>1</v>
-      </c>
-      <c r="Q45" s="39" t="str">
+      <c r="M45" s="29">
+        <v>0</v>
+      </c>
+      <c r="N45" s="32">
+        <v>0</v>
+      </c>
+      <c r="O45" s="43">
+        <v>1</v>
+      </c>
+      <c r="P45" s="53" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q45" s="38" t="str">
         <f t="shared" si="0"/>
         <v>0100</v>
+      </c>
+      <c r="R45" s="32">
+        <v>0</v>
+      </c>
+      <c r="S45" s="32">
+        <v>0</v>
+      </c>
+      <c r="T45" s="32">
+        <v>0</v>
+      </c>
+      <c r="U45" s="32">
+        <v>0</v>
+      </c>
+      <c r="V45" s="32">
+        <v>0</v>
+      </c>
+      <c r="W45" s="32">
+        <v>0</v>
+      </c>
+      <c r="X45" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="32">
+        <v>1</v>
+      </c>
+      <c r="Z45" s="32">
+        <v>1</v>
+      </c>
+      <c r="AA45" s="40">
+        <v>1</v>
+      </c>
+      <c r="AB45" s="32">
+        <v>1</v>
+      </c>
+      <c r="AC45" s="51">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4405,27 +4593,58 @@
         <v>179</v>
       </c>
       <c r="L46" s="16"/>
-      <c r="M46" s="32"/>
-      <c r="N46" s="35"/>
-      <c r="O46" s="46">
-        <v>1</v>
-      </c>
-      <c r="P46" s="35"/>
-      <c r="Q46" s="40" t="str">
+      <c r="M46" s="31">
+        <v>0</v>
+      </c>
+      <c r="N46" s="34">
+        <v>0</v>
+      </c>
+      <c r="O46" s="45">
+        <v>1</v>
+      </c>
+      <c r="P46" s="54" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q46" s="39" t="str">
         <f t="shared" si="0"/>
         <v>0101</v>
       </c>
-      <c r="R46" s="35"/>
-      <c r="S46" s="35"/>
-      <c r="T46" s="35"/>
-      <c r="U46" s="35"/>
-      <c r="V46" s="35"/>
-      <c r="W46" s="35"/>
-      <c r="X46" s="35"/>
-      <c r="Y46" s="35"/>
-      <c r="Z46" s="35"/>
-      <c r="AA46" s="42"/>
-      <c r="AB46" s="35"/>
+      <c r="R46" s="34">
+        <v>0</v>
+      </c>
+      <c r="S46" s="34">
+        <v>0</v>
+      </c>
+      <c r="T46" s="34">
+        <v>0</v>
+      </c>
+      <c r="U46" s="34">
+        <v>0</v>
+      </c>
+      <c r="V46" s="34">
+        <v>0</v>
+      </c>
+      <c r="W46" s="34">
+        <v>0</v>
+      </c>
+      <c r="X46" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="34">
+        <v>1</v>
+      </c>
+      <c r="Z46" s="34">
+        <v>1</v>
+      </c>
+      <c r="AA46" s="41">
+        <v>1</v>
+      </c>
+      <c r="AB46" s="34">
+        <v>1</v>
+      </c>
+      <c r="AC46" s="52">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18"/>
@@ -4460,12 +4679,57 @@
         <v>122</v>
       </c>
       <c r="L47" s="16"/>
-      <c r="O47" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q47" s="39" t="str">
+      <c r="M47" s="29">
+        <v>0</v>
+      </c>
+      <c r="N47" s="32">
+        <v>0</v>
+      </c>
+      <c r="O47" s="43">
+        <v>0</v>
+      </c>
+      <c r="P47" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="38" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
+      </c>
+      <c r="R47" s="32">
+        <v>0</v>
+      </c>
+      <c r="S47" s="32">
+        <v>0</v>
+      </c>
+      <c r="T47" s="32">
+        <v>0</v>
+      </c>
+      <c r="U47" s="32">
+        <v>1</v>
+      </c>
+      <c r="V47" s="32">
+        <v>0</v>
+      </c>
+      <c r="W47" s="32">
+        <v>0</v>
+      </c>
+      <c r="X47" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="32">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="32">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="52">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4499,27 +4763,58 @@
         <v>122</v>
       </c>
       <c r="L48" s="16"/>
-      <c r="M48" s="32"/>
-      <c r="N48" s="35"/>
-      <c r="O48" s="46">
-        <v>0</v>
-      </c>
-      <c r="P48" s="35"/>
-      <c r="Q48" s="40" t="str">
+      <c r="M48" s="31">
+        <v>0</v>
+      </c>
+      <c r="N48" s="34">
+        <v>0</v>
+      </c>
+      <c r="O48" s="45">
+        <v>0</v>
+      </c>
+      <c r="P48" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="39" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="R48" s="35"/>
-      <c r="S48" s="35"/>
-      <c r="T48" s="35"/>
-      <c r="U48" s="35"/>
-      <c r="V48" s="35"/>
-      <c r="W48" s="35"/>
-      <c r="X48" s="35"/>
-      <c r="Y48" s="35"/>
-      <c r="Z48" s="35"/>
-      <c r="AA48" s="42"/>
-      <c r="AB48" s="35"/>
+      <c r="R48" s="34">
+        <v>0</v>
+      </c>
+      <c r="S48" s="34">
+        <v>0</v>
+      </c>
+      <c r="T48" s="34">
+        <v>0</v>
+      </c>
+      <c r="U48" s="34">
+        <v>1</v>
+      </c>
+      <c r="V48" s="34">
+        <v>0</v>
+      </c>
+      <c r="W48" s="34">
+        <v>0</v>
+      </c>
+      <c r="X48" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y48" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB48" s="34">
+        <v>0</v>
+      </c>
+      <c r="AC48" s="52">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="24"/>
@@ -4550,9 +4845,9 @@
         <v>174</v>
       </c>
       <c r="L49" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q49" s="39" t="str">
+        <v>204</v>
+      </c>
+      <c r="Q49" s="38" t="str">
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
@@ -4586,27 +4881,27 @@
         <v>174</v>
       </c>
       <c r="L50" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="M50" s="32"/>
-      <c r="N50" s="35"/>
-      <c r="O50" s="46"/>
-      <c r="P50" s="35"/>
-      <c r="Q50" s="40" t="str">
+        <v>204</v>
+      </c>
+      <c r="M50" s="31"/>
+      <c r="N50" s="34"/>
+      <c r="O50" s="45"/>
+      <c r="P50" s="34"/>
+      <c r="Q50" s="39" t="str">
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R50" s="35"/>
-      <c r="S50" s="35"/>
-      <c r="T50" s="35"/>
-      <c r="U50" s="35"/>
-      <c r="V50" s="35"/>
-      <c r="W50" s="35"/>
-      <c r="X50" s="35"/>
-      <c r="Y50" s="35"/>
-      <c r="Z50" s="35"/>
-      <c r="AA50" s="42"/>
-      <c r="AB50" s="35"/>
+      <c r="R50" s="34"/>
+      <c r="S50" s="34"/>
+      <c r="T50" s="34"/>
+      <c r="U50" s="34"/>
+      <c r="V50" s="34"/>
+      <c r="W50" s="34"/>
+      <c r="X50" s="34"/>
+      <c r="Y50" s="34"/>
+      <c r="Z50" s="34"/>
+      <c r="AA50" s="41"/>
+      <c r="AB50" s="34"/>
     </row>
     <row r="51" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="24" t="s">
@@ -4639,9 +4934,9 @@
         <v>174</v>
       </c>
       <c r="L51" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q51" s="39" t="str">
+        <v>204</v>
+      </c>
+      <c r="Q51" s="38" t="str">
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
@@ -4675,27 +4970,27 @@
         <v>174</v>
       </c>
       <c r="L52" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="M52" s="32"/>
-      <c r="N52" s="35"/>
-      <c r="O52" s="46"/>
-      <c r="P52" s="35"/>
-      <c r="Q52" s="40" t="str">
+        <v>204</v>
+      </c>
+      <c r="M52" s="31"/>
+      <c r="N52" s="34"/>
+      <c r="O52" s="45"/>
+      <c r="P52" s="34"/>
+      <c r="Q52" s="39" t="str">
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R52" s="35"/>
-      <c r="S52" s="35"/>
-      <c r="T52" s="35"/>
-      <c r="U52" s="35"/>
-      <c r="V52" s="35"/>
-      <c r="W52" s="35"/>
-      <c r="X52" s="35"/>
-      <c r="Y52" s="35"/>
-      <c r="Z52" s="35"/>
-      <c r="AA52" s="42"/>
-      <c r="AB52" s="35"/>
+      <c r="R52" s="34"/>
+      <c r="S52" s="34"/>
+      <c r="T52" s="34"/>
+      <c r="U52" s="34"/>
+      <c r="V52" s="34"/>
+      <c r="W52" s="34"/>
+      <c r="X52" s="34"/>
+      <c r="Y52" s="34"/>
+      <c r="Z52" s="34"/>
+      <c r="AA52" s="41"/>
+      <c r="AB52" s="34"/>
     </row>
     <row r="53" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="24"/>
@@ -4726,9 +5021,9 @@
         <v>174</v>
       </c>
       <c r="L53" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q53" s="39" t="str">
+        <v>204</v>
+      </c>
+      <c r="Q53" s="38" t="str">
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
@@ -4762,35 +5057,35 @@
         <v>174</v>
       </c>
       <c r="L54" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="M54" s="32"/>
-      <c r="N54" s="35"/>
-      <c r="O54" s="46"/>
-      <c r="P54" s="35"/>
-      <c r="Q54" s="40" t="str">
+        <v>204</v>
+      </c>
+      <c r="M54" s="31"/>
+      <c r="N54" s="34"/>
+      <c r="O54" s="45"/>
+      <c r="P54" s="34"/>
+      <c r="Q54" s="39" t="str">
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R54" s="35"/>
-      <c r="S54" s="35"/>
-      <c r="T54" s="35"/>
-      <c r="U54" s="35"/>
-      <c r="V54" s="35"/>
-      <c r="W54" s="35"/>
-      <c r="X54" s="35"/>
-      <c r="Y54" s="35"/>
-      <c r="Z54" s="35"/>
-      <c r="AA54" s="42"/>
-      <c r="AB54" s="35"/>
+      <c r="R54" s="34"/>
+      <c r="S54" s="34"/>
+      <c r="T54" s="34"/>
+      <c r="U54" s="34"/>
+      <c r="V54" s="34"/>
+      <c r="W54" s="34"/>
+      <c r="X54" s="34"/>
+      <c r="Y54" s="34"/>
+      <c r="Z54" s="34"/>
+      <c r="AA54" s="41"/>
+      <c r="AB54" s="34"/>
     </row>
     <row r="55" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="28"/>
-      <c r="G55" s="28"/>
-      <c r="H55" s="28"/>
-      <c r="I55" s="28"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="27"/>
     </row>
   </sheetData>
   <sortState ref="A2:K54">

</xml_diff>

<commit_message>
Added Load and stores and jump register
</commit_message>
<xml_diff>
--- a/LAB8-11/DatapathComponents/ALU_mapping.xlsx
+++ b/LAB8-11/DatapathComponents/ALU_mapping.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="215">
   <si>
     <t>Type</t>
   </si>
@@ -654,6 +654,24 @@
   </si>
   <si>
     <t>SE</t>
+  </si>
+  <si>
+    <t>UseByte</t>
+  </si>
+  <si>
+    <t>UseHalf</t>
+  </si>
+  <si>
+    <t>LUI</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>XXXX</t>
+  </si>
+  <si>
+    <t>Jump</t>
   </si>
 </sst>
 </file>
@@ -893,7 +911,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1015,6 +1033,25 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1306,13 +1343,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF55"/>
+  <dimension ref="A1:AJ55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R49" sqref="R49"/>
+      <selection pane="bottomRight" activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1339,7 +1376,7 @@
     <col min="29" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1436,8 +1473,20 @@
       <c r="AF1" s="8" t="s">
         <v>208</v>
       </c>
+      <c r="AG1" s="54" t="s">
+        <v>209</v>
+      </c>
+      <c r="AH1" s="54" t="s">
+        <v>210</v>
+      </c>
+      <c r="AI1" s="54" t="s">
+        <v>211</v>
+      </c>
+      <c r="AJ1" s="54" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="2" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
@@ -1533,8 +1582,20 @@
       <c r="AF2" s="8">
         <v>0</v>
       </c>
+      <c r="AG2" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
         <v>8</v>
@@ -1628,8 +1689,20 @@
       <c r="AF3" s="8">
         <v>0</v>
       </c>
+      <c r="AG3" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
         <v>12</v>
@@ -1723,8 +1796,20 @@
       <c r="AF4" s="8">
         <v>0</v>
       </c>
+      <c r="AG4" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
         <v>16</v>
@@ -1818,8 +1903,20 @@
       <c r="AF5" s="8">
         <v>0</v>
       </c>
+      <c r="AG5" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" s="13" t="s">
         <v>18</v>
@@ -1913,8 +2010,20 @@
       <c r="AF6" s="8">
         <v>0</v>
       </c>
+      <c r="AG6" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="28" t="s">
         <v>66</v>
       </c>
@@ -2010,8 +2119,20 @@
       <c r="AF7" s="8">
         <v>0</v>
       </c>
+      <c r="AG7" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
       <c r="B8" s="29" t="s">
         <v>71</v>
@@ -2105,8 +2226,20 @@
       <c r="AF8" s="8">
         <v>0</v>
       </c>
+      <c r="AG8" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28"/>
       <c r="B9" s="29" t="s">
         <v>75</v>
@@ -2200,8 +2333,20 @@
       <c r="AF9" s="8">
         <v>0</v>
       </c>
+      <c r="AG9" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="28"/>
       <c r="B10" s="29" t="s">
         <v>73</v>
@@ -2295,8 +2440,20 @@
       <c r="AF10" s="8">
         <v>0</v>
       </c>
+      <c r="AG10" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="28"/>
       <c r="B11" s="29" t="s">
         <v>83</v>
@@ -2390,8 +2547,20 @@
       <c r="AF11" s="8">
         <v>0</v>
       </c>
+      <c r="AG11" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="28"/>
       <c r="B12" s="29" t="s">
         <v>87</v>
@@ -2485,8 +2654,20 @@
       <c r="AF12" s="8">
         <v>0</v>
       </c>
+      <c r="AG12" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="28"/>
       <c r="B13" s="29" t="s">
         <v>85</v>
@@ -2580,8 +2761,20 @@
       <c r="AF13" s="8">
         <v>0</v>
       </c>
+      <c r="AG13" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:32" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="28"/>
       <c r="B14" s="29" t="s">
         <v>89</v>
@@ -2675,8 +2868,20 @@
       <c r="AF14" s="8">
         <v>0</v>
       </c>
+      <c r="AG14" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28"/>
       <c r="B15" s="29" t="s">
         <v>103</v>
@@ -2770,8 +2975,20 @@
       <c r="AF15" s="8">
         <v>0</v>
       </c>
+      <c r="AG15" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28"/>
       <c r="B16" s="29" t="s">
         <v>105</v>
@@ -2865,8 +3082,20 @@
       <c r="AF16" s="8">
         <v>0</v>
       </c>
+      <c r="AG16" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28"/>
       <c r="B17" s="29" t="s">
         <v>101</v>
@@ -2960,8 +3189,20 @@
       <c r="AF17" s="8">
         <v>0</v>
       </c>
+      <c r="AG17" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="28"/>
       <c r="B18" s="29" t="s">
         <v>99</v>
@@ -3055,8 +3296,20 @@
       <c r="AF18" s="8">
         <v>0</v>
       </c>
+      <c r="AG18" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="28"/>
       <c r="B19" s="29" t="s">
         <v>91</v>
@@ -3150,8 +3403,20 @@
       <c r="AF19" s="8">
         <v>0</v>
       </c>
+      <c r="AG19" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28"/>
       <c r="B20" s="29" t="s">
         <v>111</v>
@@ -3245,8 +3510,20 @@
       <c r="AF20" s="8">
         <v>0</v>
       </c>
+      <c r="AG20" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI20" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="34"/>
       <c r="B21" s="35" t="s">
         <v>62</v>
@@ -3274,16 +3551,81 @@
       </c>
       <c r="J21" s="17"/>
       <c r="K21" s="18"/>
-      <c r="L21" s="19" t="s">
-        <v>204</v>
-      </c>
+      <c r="L21" s="19"/>
       <c r="M21" s="9">
         <v>0</v>
       </c>
-      <c r="N21" s="31"/>
-      <c r="Q21" s="25"/>
+      <c r="N21" s="31">
+        <v>0</v>
+      </c>
+      <c r="O21" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="P21" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q21" s="60" t="s">
+        <v>213</v>
+      </c>
+      <c r="R21" s="26">
+        <v>0</v>
+      </c>
+      <c r="S21" s="10">
+        <v>0</v>
+      </c>
+      <c r="T21" s="10">
+        <v>0</v>
+      </c>
+      <c r="U21" s="10">
+        <v>0</v>
+      </c>
+      <c r="V21" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="W21" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="X21" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="Y21" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="Z21" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA21" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="AB21" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC21" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="AD21" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE21" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="AF21" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="AG21" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="AH21" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="AI21" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="AJ21" s="54">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="28"/>
       <c r="B22" s="29" t="s">
         <v>97</v>
@@ -3377,8 +3719,20 @@
       <c r="AF22" s="8">
         <v>0</v>
       </c>
+      <c r="AG22" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI22" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="28"/>
       <c r="B23" s="29" t="s">
         <v>95</v>
@@ -3472,8 +3826,20 @@
       <c r="AF23" s="8">
         <v>0</v>
       </c>
+      <c r="AG23" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="43"/>
       <c r="B24" s="44" t="s">
         <v>41</v>
@@ -3562,8 +3928,20 @@
       <c r="AF24" s="8">
         <v>0</v>
       </c>
+      <c r="AG24" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI24" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="43"/>
       <c r="B25" s="44" t="s">
         <v>37</v>
@@ -3652,8 +4030,20 @@
       <c r="AF25" s="8">
         <v>0</v>
       </c>
+      <c r="AG25" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI25" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="43"/>
       <c r="B26" s="44" t="s">
         <v>43</v>
@@ -3742,8 +4132,20 @@
       <c r="AF26" s="8">
         <v>0</v>
       </c>
+      <c r="AG26" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="43"/>
       <c r="B27" s="44" t="s">
         <v>39</v>
@@ -3832,8 +4234,20 @@
       <c r="AF27" s="8">
         <v>0</v>
       </c>
+      <c r="AG27" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI27" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="34" t="s">
         <v>47</v>
       </c>
@@ -3885,8 +4299,20 @@
       <c r="Z28" s="38"/>
       <c r="AA28" s="38"/>
       <c r="AB28" s="38"/>
+      <c r="AG28" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH28" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI28" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="34"/>
       <c r="B29" s="35" t="s">
         <v>58</v>
@@ -3921,8 +4347,20 @@
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
+      <c r="AG29" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH29" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI29" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ29" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="34"/>
       <c r="B30" s="35" t="s">
         <v>60</v>
@@ -3968,8 +4406,20 @@
       <c r="Z30" s="38"/>
       <c r="AA30" s="38"/>
       <c r="AB30" s="38"/>
+      <c r="AG30" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH30" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI30" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ30" s="54">
+        <v>1</v>
+      </c>
     </row>
-    <row r="31" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="34"/>
       <c r="B31" s="35" t="s">
         <v>64</v>
@@ -4000,8 +4450,20 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
+      <c r="AG31" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH31" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI31" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ31" s="54">
+        <v>1</v>
+      </c>
     </row>
-    <row r="32" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="35"/>
       <c r="B32" s="35" t="s">
         <v>50</v>
@@ -4051,8 +4513,20 @@
       <c r="Z32" s="38"/>
       <c r="AA32" s="38"/>
       <c r="AB32" s="38"/>
+      <c r="AG32" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH32" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI32" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ32" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="35"/>
       <c r="B33" s="35" t="s">
         <v>52</v>
@@ -4087,8 +4561,20 @@
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
+      <c r="AG33" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH33" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI33" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ33" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="35"/>
       <c r="B34" s="35" t="s">
         <v>56</v>
@@ -4138,8 +4624,20 @@
       <c r="Z34" s="38"/>
       <c r="AA34" s="38"/>
       <c r="AB34" s="38"/>
+      <c r="AG34" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI34" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ34" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="35"/>
       <c r="B35" s="35" t="s">
         <v>54</v>
@@ -4174,8 +4672,20 @@
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
+      <c r="AG35" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH35" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI35" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ35" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="13" t="s">
         <v>10</v>
@@ -4265,8 +4775,20 @@
       <c r="AF36" s="8">
         <v>0</v>
       </c>
+      <c r="AG36" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH36" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI36" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ36" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="13" t="s">
         <v>6</v>
@@ -4356,8 +4878,20 @@
       <c r="AF37" s="8">
         <v>0</v>
       </c>
+      <c r="AG37" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH37" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI37" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ37" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="29"/>
       <c r="B38" s="29" t="s">
         <v>93</v>
@@ -4447,8 +4981,20 @@
       <c r="AF38" s="8">
         <v>0</v>
       </c>
+      <c r="AG38" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH38" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI38" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ38" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:32" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:36" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="29"/>
       <c r="B39" s="29" t="s">
         <v>109</v>
@@ -4538,8 +5084,20 @@
       <c r="AF39" s="8">
         <v>0</v>
       </c>
+      <c r="AG39" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH39" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI39" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ39" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="29"/>
       <c r="B40" s="29" t="s">
         <v>69</v>
@@ -4629,8 +5187,20 @@
       <c r="AF40" s="8">
         <v>0</v>
       </c>
+      <c r="AG40" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH40" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI40" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ40" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="29"/>
       <c r="B41" s="29" t="s">
         <v>77</v>
@@ -4720,8 +5290,20 @@
       <c r="AF41" s="8">
         <v>0</v>
       </c>
+      <c r="AG41" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH41" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI41" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ41" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="29"/>
       <c r="B42" s="29" t="s">
         <v>79</v>
@@ -4811,8 +5393,20 @@
       <c r="AF42" s="8">
         <v>0</v>
       </c>
+      <c r="AG42" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH42" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI42" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ42" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="44"/>
       <c r="B43" s="44" t="s">
         <v>45</v>
@@ -4834,21 +5428,87 @@
       </c>
       <c r="H43" s="47"/>
       <c r="I43" s="47"/>
-      <c r="J43" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="K43" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="L43" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q43" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="J43" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="K43" s="37">
+        <v>10</v>
+      </c>
+      <c r="L43" s="19"/>
+      <c r="M43" s="9">
+        <v>1</v>
+      </c>
+      <c r="N43" s="10">
+        <v>0</v>
+      </c>
+      <c r="O43" s="11">
+        <v>0</v>
+      </c>
+      <c r="P43" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="52">
+        <v>10</v>
+      </c>
+      <c r="R43" s="10">
+        <v>0</v>
+      </c>
+      <c r="S43" s="10">
+        <v>0</v>
+      </c>
+      <c r="T43" s="10">
+        <v>0</v>
+      </c>
+      <c r="U43" s="10">
+        <v>1</v>
+      </c>
+      <c r="V43" s="10">
+        <v>0</v>
+      </c>
+      <c r="W43" s="10">
+        <v>0</v>
+      </c>
+      <c r="X43" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC43" s="53">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="53">
+        <v>0</v>
+      </c>
+      <c r="AE43" s="53">
+        <v>0</v>
+      </c>
+      <c r="AF43" s="53">
+        <v>0</v>
+      </c>
+      <c r="AG43" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH43" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI43" s="54">
+        <v>1</v>
+      </c>
+      <c r="AJ43" s="54">
+        <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13"/>
       <c r="B44" s="13" t="s">
         <v>14</v>
@@ -4942,8 +5602,20 @@
       <c r="AF44" s="8">
         <v>0</v>
       </c>
+      <c r="AG44" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH44" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI44" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ44" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13"/>
       <c r="B45" s="13" t="s">
         <v>20</v>
@@ -5037,8 +5709,20 @@
       <c r="AF45" s="8">
         <v>0</v>
       </c>
+      <c r="AG45" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH45" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI45" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ45" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13"/>
       <c r="B46" s="13" t="s">
         <v>22</v>
@@ -5132,8 +5816,20 @@
       <c r="AF46" s="8">
         <v>0</v>
       </c>
+      <c r="AG46" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH46" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI46" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ46" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="29"/>
       <c r="B47" s="29" t="s">
         <v>81</v>
@@ -5227,8 +5923,20 @@
       <c r="AF47" s="8">
         <v>1</v>
       </c>
+      <c r="AG47" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH47" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI47" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ47" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="29"/>
       <c r="B48" s="29" t="s">
         <v>107</v>
@@ -5320,8 +6028,20 @@
       <c r="AF48" s="8">
         <v>1</v>
       </c>
+      <c r="AG48" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH48" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI48" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ48" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="44"/>
       <c r="B49" s="44" t="s">
         <v>33</v>
@@ -5349,9 +6069,7 @@
       <c r="K49" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="L49" s="19" t="s">
-        <v>204</v>
-      </c>
+      <c r="L49" s="19"/>
       <c r="M49" s="9">
         <v>0</v>
       </c>
@@ -5368,8 +6086,65 @@
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
+      <c r="R49" s="10">
+        <v>0</v>
+      </c>
+      <c r="S49" s="10">
+        <v>1</v>
+      </c>
+      <c r="T49" s="10">
+        <v>1</v>
+      </c>
+      <c r="U49" s="10">
+        <v>1</v>
+      </c>
+      <c r="V49" s="10">
+        <v>0</v>
+      </c>
+      <c r="W49" s="10">
+        <v>0</v>
+      </c>
+      <c r="X49" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y49" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z49" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA49" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB49" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC49" s="53">
+        <v>0</v>
+      </c>
+      <c r="AD49" s="53">
+        <v>0</v>
+      </c>
+      <c r="AE49" s="53">
+        <v>0</v>
+      </c>
+      <c r="AF49" s="53">
+        <v>0</v>
+      </c>
+      <c r="AG49" s="53">
+        <v>1</v>
+      </c>
+      <c r="AH49" s="53">
+        <v>0</v>
+      </c>
+      <c r="AI49" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ49" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="44"/>
       <c r="B50" s="44" t="s">
         <v>31</v>
@@ -5397,30 +6172,82 @@
       <c r="K50" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="L50" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="M50" s="32"/>
-      <c r="N50" s="38"/>
-      <c r="O50" s="46"/>
-      <c r="P50" s="38"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="32">
+        <v>0</v>
+      </c>
+      <c r="N50" s="38">
+        <v>0</v>
+      </c>
+      <c r="O50" s="46">
+        <v>0</v>
+      </c>
+      <c r="P50" s="38">
+        <v>1</v>
+      </c>
       <c r="Q50" s="33" t="str">
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R50" s="38"/>
-      <c r="S50" s="38"/>
-      <c r="T50" s="38"/>
-      <c r="U50" s="38"/>
-      <c r="V50" s="38"/>
-      <c r="W50" s="38"/>
-      <c r="X50" s="38"/>
-      <c r="Y50" s="38"/>
-      <c r="Z50" s="38"/>
-      <c r="AA50" s="38"/>
-      <c r="AB50" s="38"/>
+      <c r="R50" s="38">
+        <v>0</v>
+      </c>
+      <c r="S50" s="38">
+        <v>1</v>
+      </c>
+      <c r="T50" s="38">
+        <v>1</v>
+      </c>
+      <c r="U50" s="38">
+        <v>1</v>
+      </c>
+      <c r="V50" s="38">
+        <v>0</v>
+      </c>
+      <c r="W50" s="38">
+        <v>0</v>
+      </c>
+      <c r="X50" s="38">
+        <v>0</v>
+      </c>
+      <c r="Y50" s="38">
+        <v>0</v>
+      </c>
+      <c r="Z50" s="38">
+        <v>0</v>
+      </c>
+      <c r="AA50" s="38">
+        <v>0</v>
+      </c>
+      <c r="AB50" s="38">
+        <v>0</v>
+      </c>
+      <c r="AC50" s="53">
+        <v>0</v>
+      </c>
+      <c r="AD50" s="55">
+        <v>0</v>
+      </c>
+      <c r="AE50" s="55">
+        <v>0</v>
+      </c>
+      <c r="AF50" s="55">
+        <v>0</v>
+      </c>
+      <c r="AG50" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH50" s="54">
+        <v>1</v>
+      </c>
+      <c r="AI50" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ50" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="44" t="s">
         <v>24</v>
       </c>
@@ -5450,15 +6277,82 @@
       <c r="K51" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="L51" s="19" t="s">
-        <v>204</v>
+      <c r="L51" s="19"/>
+      <c r="M51" s="9">
+        <v>0</v>
+      </c>
+      <c r="N51" s="10">
+        <v>0</v>
+      </c>
+      <c r="O51" s="11">
+        <v>0</v>
+      </c>
+      <c r="P51" s="10">
+        <v>1</v>
       </c>
       <c r="Q51" s="25" t="str">
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
+      <c r="R51" s="10">
+        <v>0</v>
+      </c>
+      <c r="S51" s="10">
+        <v>1</v>
+      </c>
+      <c r="T51" s="10">
+        <v>1</v>
+      </c>
+      <c r="U51" s="10">
+        <v>1</v>
+      </c>
+      <c r="V51" s="10">
+        <v>0</v>
+      </c>
+      <c r="W51" s="10">
+        <v>0</v>
+      </c>
+      <c r="X51" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y51" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z51" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA51" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB51" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC51" s="53">
+        <v>0</v>
+      </c>
+      <c r="AD51" s="53">
+        <v>0</v>
+      </c>
+      <c r="AE51" s="53">
+        <v>0</v>
+      </c>
+      <c r="AF51" s="53">
+        <v>0</v>
+      </c>
+      <c r="AG51" s="54">
+        <v>0</v>
+      </c>
+      <c r="AH51" s="54">
+        <v>0</v>
+      </c>
+      <c r="AI51" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ51" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="44"/>
       <c r="B52" s="44" t="s">
         <v>29</v>
@@ -5486,30 +6380,82 @@
       <c r="K52" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="L52" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="M52" s="32"/>
-      <c r="N52" s="38"/>
-      <c r="O52" s="46"/>
-      <c r="P52" s="38"/>
+      <c r="L52" s="19"/>
+      <c r="M52" s="32">
+        <v>0</v>
+      </c>
+      <c r="N52" s="38">
+        <v>0</v>
+      </c>
+      <c r="O52" s="46">
+        <v>0</v>
+      </c>
+      <c r="P52" s="56" t="s">
+        <v>203</v>
+      </c>
       <c r="Q52" s="33" t="str">
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R52" s="38"/>
-      <c r="S52" s="38"/>
-      <c r="T52" s="38"/>
-      <c r="U52" s="38"/>
-      <c r="V52" s="38"/>
-      <c r="W52" s="38"/>
-      <c r="X52" s="38"/>
-      <c r="Y52" s="38"/>
-      <c r="Z52" s="38"/>
-      <c r="AA52" s="38"/>
-      <c r="AB52" s="38"/>
+      <c r="R52" s="38">
+        <v>1</v>
+      </c>
+      <c r="S52" s="38">
+        <v>0</v>
+      </c>
+      <c r="T52" s="38">
+        <v>0</v>
+      </c>
+      <c r="U52" s="38">
+        <v>0</v>
+      </c>
+      <c r="V52" s="38">
+        <v>0</v>
+      </c>
+      <c r="W52" s="38">
+        <v>0</v>
+      </c>
+      <c r="X52" s="38">
+        <v>0</v>
+      </c>
+      <c r="Y52" s="38">
+        <v>0</v>
+      </c>
+      <c r="Z52" s="38">
+        <v>0</v>
+      </c>
+      <c r="AA52" s="38">
+        <v>0</v>
+      </c>
+      <c r="AB52" s="38">
+        <v>0</v>
+      </c>
+      <c r="AC52" s="53">
+        <v>0</v>
+      </c>
+      <c r="AD52" s="55">
+        <v>0</v>
+      </c>
+      <c r="AE52" s="55">
+        <v>0</v>
+      </c>
+      <c r="AF52" s="55">
+        <v>0</v>
+      </c>
+      <c r="AG52" s="55">
+        <v>1</v>
+      </c>
+      <c r="AH52" s="55">
+        <v>0</v>
+      </c>
+      <c r="AI52" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ52" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="44"/>
       <c r="B53" s="44" t="s">
         <v>35</v>
@@ -5537,15 +6483,82 @@
       <c r="K53" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="L53" s="19" t="s">
-        <v>204</v>
+      <c r="L53" s="19"/>
+      <c r="M53" s="9">
+        <v>0</v>
+      </c>
+      <c r="N53" s="10">
+        <v>0</v>
+      </c>
+      <c r="O53" s="11">
+        <v>0</v>
+      </c>
+      <c r="P53" s="57" t="s">
+        <v>203</v>
       </c>
       <c r="Q53" s="25" t="str">
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
+      <c r="R53" s="10">
+        <v>1</v>
+      </c>
+      <c r="S53" s="10">
+        <v>0</v>
+      </c>
+      <c r="T53" s="10">
+        <v>0</v>
+      </c>
+      <c r="U53" s="10">
+        <v>0</v>
+      </c>
+      <c r="V53" s="10">
+        <v>0</v>
+      </c>
+      <c r="W53" s="10">
+        <v>0</v>
+      </c>
+      <c r="X53" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y53" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z53" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA53" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB53" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC53" s="53">
+        <v>0</v>
+      </c>
+      <c r="AD53" s="53">
+        <v>0</v>
+      </c>
+      <c r="AE53" s="53">
+        <v>0</v>
+      </c>
+      <c r="AF53" s="53">
+        <v>0</v>
+      </c>
+      <c r="AG53" s="53">
+        <v>0</v>
+      </c>
+      <c r="AH53" s="53">
+        <v>1</v>
+      </c>
+      <c r="AI53" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ53" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="44"/>
       <c r="B54" s="44" t="s">
         <v>27</v>
@@ -5573,30 +6586,82 @@
       <c r="K54" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="L54" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="M54" s="32"/>
-      <c r="N54" s="38"/>
-      <c r="O54" s="46"/>
-      <c r="P54" s="38"/>
+      <c r="L54" s="19"/>
+      <c r="M54" s="32">
+        <v>0</v>
+      </c>
+      <c r="N54" s="38">
+        <v>0</v>
+      </c>
+      <c r="O54" s="46">
+        <v>0</v>
+      </c>
+      <c r="P54" s="56" t="s">
+        <v>203</v>
+      </c>
       <c r="Q54" s="33" t="str">
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R54" s="38"/>
-      <c r="S54" s="38"/>
-      <c r="T54" s="38"/>
-      <c r="U54" s="38"/>
-      <c r="V54" s="38"/>
-      <c r="W54" s="38"/>
-      <c r="X54" s="38"/>
-      <c r="Y54" s="38"/>
-      <c r="Z54" s="38"/>
-      <c r="AA54" s="38"/>
-      <c r="AB54" s="38"/>
+      <c r="R54" s="38">
+        <v>1</v>
+      </c>
+      <c r="S54" s="38">
+        <v>0</v>
+      </c>
+      <c r="T54" s="38">
+        <v>0</v>
+      </c>
+      <c r="U54" s="38">
+        <v>0</v>
+      </c>
+      <c r="V54" s="38">
+        <v>0</v>
+      </c>
+      <c r="W54" s="38">
+        <v>0</v>
+      </c>
+      <c r="X54" s="38">
+        <v>0</v>
+      </c>
+      <c r="Y54" s="38">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="38">
+        <v>0</v>
+      </c>
+      <c r="AA54" s="38">
+        <v>0</v>
+      </c>
+      <c r="AB54" s="38">
+        <v>0</v>
+      </c>
+      <c r="AC54" s="53">
+        <v>0</v>
+      </c>
+      <c r="AD54" s="55">
+        <v>0</v>
+      </c>
+      <c r="AE54" s="55">
+        <v>0</v>
+      </c>
+      <c r="AF54" s="55">
+        <v>0</v>
+      </c>
+      <c r="AG54" s="55">
+        <v>0</v>
+      </c>
+      <c r="AH54" s="55">
+        <v>0</v>
+      </c>
+      <c r="AI54" s="54">
+        <v>0</v>
+      </c>
+      <c r="AJ54" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="D55" s="51"/>
       <c r="E55" s="51"/>
       <c r="F55" s="51"/>

</xml_diff>

<commit_message>
And the excel file...
</commit_message>
<xml_diff>
--- a/LAB8-11/DatapathComponents/ALU_mapping.xlsx
+++ b/LAB8-11/DatapathComponents/ALU_mapping.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="214">
   <si>
     <t>Type</t>
   </si>
@@ -639,9 +639,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>Don't worry for this lab</t>
   </si>
   <si>
     <t>DepRegWrite</t>
@@ -911,7 +908,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1052,6 +1049,21 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1345,11 +1357,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1462,28 +1474,28 @@
         <v>202</v>
       </c>
       <c r="AC1" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="AD1" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AF1" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AG1" s="54" t="s">
         <v>208</v>
       </c>
-      <c r="AG1" s="54" t="s">
+      <c r="AH1" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="AH1" s="54" t="s">
+      <c r="AI1" s="54" t="s">
         <v>210</v>
       </c>
-      <c r="AI1" s="54" t="s">
-        <v>211</v>
-      </c>
       <c r="AJ1" s="54" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3559,13 +3571,13 @@
         <v>0</v>
       </c>
       <c r="O21" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="P21" s="57">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="60" t="s">
         <v>212</v>
-      </c>
-      <c r="P21" s="57" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q21" s="60" t="s">
-        <v>213</v>
       </c>
       <c r="R21" s="26">
         <v>0</v>
@@ -4277,9 +4289,7 @@
       <c r="K28" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="L28" s="19" t="s">
-        <v>204</v>
-      </c>
+      <c r="L28" s="19"/>
       <c r="M28" s="32"/>
       <c r="N28" s="38"/>
       <c r="O28" s="46"/>
@@ -4340,9 +4350,7 @@
       <c r="K29" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="L29" s="19" t="s">
-        <v>204</v>
-      </c>
+      <c r="L29" s="19"/>
       <c r="Q29" s="25" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>
@@ -4384,36 +4392,90 @@
       <c r="K30" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="L30" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="M30" s="32"/>
-      <c r="N30" s="38"/>
-      <c r="O30" s="46"/>
-      <c r="P30" s="38"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="63">
+        <f t="shared" ref="M30:N30" si="1">M21</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O30" s="62" t="str">
+        <f>O21</f>
+        <v>XX</v>
+      </c>
+      <c r="P30" s="38">
+        <v>0</v>
+      </c>
       <c r="Q30" s="33" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="R30" s="38"/>
-      <c r="S30" s="38"/>
-      <c r="T30" s="38"/>
-      <c r="U30" s="38"/>
-      <c r="V30" s="38"/>
-      <c r="W30" s="38"/>
-      <c r="X30" s="38"/>
-      <c r="Y30" s="38"/>
-      <c r="Z30" s="38"/>
-      <c r="AA30" s="38"/>
-      <c r="AB30" s="38"/>
-      <c r="AG30" s="54">
-        <v>0</v>
-      </c>
-      <c r="AH30" s="54">
-        <v>0</v>
-      </c>
-      <c r="AI30" s="54">
-        <v>0</v>
+      <c r="R30" s="50">
+        <f t="shared" ref="R30:AA30" si="2">R21</f>
+        <v>0</v>
+      </c>
+      <c r="S30" s="50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T30" s="50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U30" s="50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V30" s="50" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="W30" s="50" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="X30" s="50" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="Y30" s="50" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="Z30" s="50" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="AA30" s="50" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="AB30" s="50" t="str">
+        <f>AB21</f>
+        <v>X</v>
+      </c>
+      <c r="AC30" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="AD30" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE30" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="AF30" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="AG30" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="AH30" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="AI30" s="61" t="s">
+        <v>203</v>
       </c>
       <c r="AJ30" s="54">
         <v>1</v>
@@ -4443,21 +4505,77 @@
       <c r="K31" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="L31" s="19" t="s">
-        <v>204</v>
+      <c r="L31" s="19"/>
+      <c r="M31" s="9">
+        <v>0</v>
+      </c>
+      <c r="N31" s="10">
+        <v>0</v>
+      </c>
+      <c r="O31" s="66" t="str">
+        <f>O30</f>
+        <v>XX</v>
+      </c>
+      <c r="P31" s="10">
+        <v>0</v>
       </c>
       <c r="Q31" s="25" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="AG31" s="54">
-        <v>0</v>
-      </c>
-      <c r="AH31" s="54">
-        <v>0</v>
-      </c>
-      <c r="AI31" s="54">
-        <v>0</v>
+      <c r="R31" s="10">
+        <v>0</v>
+      </c>
+      <c r="S31" s="10">
+        <v>0</v>
+      </c>
+      <c r="T31" s="10">
+        <v>0</v>
+      </c>
+      <c r="U31" s="10">
+        <v>1</v>
+      </c>
+      <c r="V31" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="W31" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="X31" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="Y31" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="Z31" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA31" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="AB31" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC31" s="64" t="s">
+        <v>203</v>
+      </c>
+      <c r="AD31" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE31" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="AF31" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="AG31" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="AH31" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="AI31" s="65" t="s">
+        <v>203</v>
       </c>
       <c r="AJ31" s="54">
         <v>1</v>
@@ -4491,9 +4609,7 @@
       <c r="K32" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="L32" s="19" t="s">
-        <v>204</v>
-      </c>
+      <c r="L32" s="19"/>
       <c r="M32" s="32"/>
       <c r="N32" s="38"/>
       <c r="O32" s="46"/>
@@ -4554,9 +4670,7 @@
       <c r="K33" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="L33" s="19" t="s">
-        <v>204</v>
-      </c>
+      <c r="L33" s="19"/>
       <c r="Q33" s="25" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>
@@ -4602,9 +4716,7 @@
       <c r="K34" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="L34" s="19" t="s">
-        <v>204</v>
-      </c>
+      <c r="L34" s="19"/>
       <c r="M34" s="32"/>
       <c r="N34" s="38"/>
       <c r="O34" s="46"/>
@@ -4665,9 +4777,7 @@
       <c r="K35" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="L35" s="19" t="s">
-        <v>204</v>
-      </c>
+      <c r="L35" s="19"/>
       <c r="Q35" s="25" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>

</xml_diff>

<commit_message>
Implemented the rest of the instructions. Synthesizes and implements
</commit_message>
<xml_diff>
--- a/LAB8-11/DatapathComponents/ALU_mapping.xlsx
+++ b/LAB8-11/DatapathComponents/ALU_mapping.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="215">
   <si>
     <t>Type</t>
   </si>
@@ -669,15 +669,19 @@
   </si>
   <si>
     <t>Jump</t>
+  </si>
+  <si>
+    <t>Branch Ctrl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="00"/>
     <numFmt numFmtId="165" formatCode="0000"/>
+    <numFmt numFmtId="166" formatCode="000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -908,7 +912,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1066,6 +1070,15 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent3" xfId="9" builtinId="38"/>
@@ -1355,13 +1368,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ55"/>
+  <dimension ref="A1:AK55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1375,20 +1388,21 @@
     <col min="15" max="15" width="6.875" style="11" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7" style="10" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.375" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.125" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.75" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="4.875" style="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.375" style="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.875" style="10" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.375" style="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.875" style="10" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="11" style="8"/>
+    <col min="18" max="18" width="10.375" style="10" customWidth="1"/>
+    <col min="19" max="19" width="10.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9" style="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="4.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1440,65 +1454,68 @@
       <c r="Q1" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="67" t="s">
+        <v>214</v>
+      </c>
+      <c r="S1" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="U1" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="V1" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="W1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="X1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="Y1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Z1" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AB1" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="AB1" s="10" t="s">
+      <c r="AC1" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AF1" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AG1" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="AG1" s="54" t="s">
+      <c r="AH1" s="54" t="s">
         <v>208</v>
       </c>
-      <c r="AH1" s="54" t="s">
+      <c r="AI1" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="AI1" s="54" t="s">
+      <c r="AJ1" s="54" t="s">
         <v>210</v>
       </c>
-      <c r="AJ1" s="54" t="s">
+      <c r="AK1" s="54" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
@@ -1549,7 +1566,7 @@
         <f>K2</f>
         <v>0000</v>
       </c>
-      <c r="R2" s="21">
+      <c r="R2" s="69">
         <v>0</v>
       </c>
       <c r="S2" s="21">
@@ -1559,10 +1576,10 @@
         <v>0</v>
       </c>
       <c r="U2" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W2" s="21">
         <v>0</v>
@@ -1582,7 +1599,7 @@
       <c r="AB2" s="21">
         <v>0</v>
       </c>
-      <c r="AC2" s="8">
+      <c r="AC2" s="21">
         <v>0</v>
       </c>
       <c r="AD2" s="8">
@@ -1594,7 +1611,7 @@
       <c r="AF2" s="8">
         <v>0</v>
       </c>
-      <c r="AG2" s="54">
+      <c r="AG2" s="8">
         <v>0</v>
       </c>
       <c r="AH2" s="54">
@@ -1606,8 +1623,11 @@
       <c r="AJ2" s="54">
         <v>0</v>
       </c>
+      <c r="AK2" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
         <v>8</v>
@@ -1656,7 +1676,7 @@
         <f t="shared" ref="Q3:Q54" si="0">K3</f>
         <v>0000</v>
       </c>
-      <c r="R3" s="10">
+      <c r="R3" s="68">
         <v>0</v>
       </c>
       <c r="S3" s="10">
@@ -1666,10 +1686,10 @@
         <v>0</v>
       </c>
       <c r="U3" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3" s="10">
         <v>0</v>
@@ -1689,7 +1709,7 @@
       <c r="AB3" s="10">
         <v>0</v>
       </c>
-      <c r="AC3" s="8">
+      <c r="AC3" s="10">
         <v>0</v>
       </c>
       <c r="AD3" s="8">
@@ -1701,7 +1721,7 @@
       <c r="AF3" s="8">
         <v>0</v>
       </c>
-      <c r="AG3" s="54">
+      <c r="AG3" s="8">
         <v>0</v>
       </c>
       <c r="AH3" s="54">
@@ -1713,8 +1733,11 @@
       <c r="AJ3" s="54">
         <v>0</v>
       </c>
+      <c r="AK3" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
         <v>12</v>
@@ -1763,7 +1786,7 @@
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
-      <c r="R4" s="21">
+      <c r="R4" s="69">
         <v>0</v>
       </c>
       <c r="S4" s="21">
@@ -1773,10 +1796,10 @@
         <v>0</v>
       </c>
       <c r="U4" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4" s="21">
         <v>0</v>
@@ -1796,7 +1819,7 @@
       <c r="AB4" s="21">
         <v>0</v>
       </c>
-      <c r="AC4" s="8">
+      <c r="AC4" s="21">
         <v>0</v>
       </c>
       <c r="AD4" s="8">
@@ -1808,7 +1831,7 @@
       <c r="AF4" s="8">
         <v>0</v>
       </c>
-      <c r="AG4" s="54">
+      <c r="AG4" s="8">
         <v>0</v>
       </c>
       <c r="AH4" s="54">
@@ -1820,8 +1843,11 @@
       <c r="AJ4" s="54">
         <v>0</v>
       </c>
+      <c r="AK4" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
         <v>16</v>
@@ -1870,18 +1896,18 @@
         <f t="shared" si="0"/>
         <v>0010</v>
       </c>
-      <c r="R5" s="10">
+      <c r="R5" s="68">
         <v>0</v>
       </c>
       <c r="S5" s="10">
         <v>0</v>
       </c>
-      <c r="T5" s="26" t="s">
+      <c r="T5" s="10">
+        <v>0</v>
+      </c>
+      <c r="U5" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="U5" s="10">
-        <v>0</v>
-      </c>
       <c r="V5" s="10">
         <v>0</v>
       </c>
@@ -1895,16 +1921,16 @@
         <v>0</v>
       </c>
       <c r="Z5" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA5" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB5" s="10">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="8">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AC5" s="10">
+        <v>1</v>
       </c>
       <c r="AD5" s="8">
         <v>0</v>
@@ -1915,7 +1941,7 @@
       <c r="AF5" s="8">
         <v>0</v>
       </c>
-      <c r="AG5" s="54">
+      <c r="AG5" s="8">
         <v>0</v>
       </c>
       <c r="AH5" s="54">
@@ -1927,8 +1953,11 @@
       <c r="AJ5" s="54">
         <v>0</v>
       </c>
+      <c r="AK5" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" s="13" t="s">
         <v>18</v>
@@ -1977,18 +2006,18 @@
         <f t="shared" si="0"/>
         <v>0011</v>
       </c>
-      <c r="R6" s="21">
+      <c r="R6" s="69">
         <v>0</v>
       </c>
       <c r="S6" s="21">
         <v>0</v>
       </c>
-      <c r="T6" s="27" t="s">
+      <c r="T6" s="21">
+        <v>0</v>
+      </c>
+      <c r="U6" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="U6" s="21">
-        <v>0</v>
-      </c>
       <c r="V6" s="21">
         <v>0</v>
       </c>
@@ -2002,16 +2031,16 @@
         <v>0</v>
       </c>
       <c r="Z6" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB6" s="21">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="8">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="21">
+        <v>1</v>
       </c>
       <c r="AD6" s="8">
         <v>0</v>
@@ -2022,7 +2051,7 @@
       <c r="AF6" s="8">
         <v>0</v>
       </c>
-      <c r="AG6" s="54">
+      <c r="AG6" s="8">
         <v>0</v>
       </c>
       <c r="AH6" s="54">
@@ -2034,8 +2063,11 @@
       <c r="AJ6" s="54">
         <v>0</v>
       </c>
+      <c r="AK6" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="28" t="s">
         <v>66</v>
       </c>
@@ -2086,7 +2118,7 @@
         <f t="shared" si="0"/>
         <v>0110</v>
       </c>
-      <c r="R7" s="10">
+      <c r="R7" s="68">
         <v>0</v>
       </c>
       <c r="S7" s="10">
@@ -2096,10 +2128,10 @@
         <v>0</v>
       </c>
       <c r="U7" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V7" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" s="10">
         <v>0</v>
@@ -2119,7 +2151,7 @@
       <c r="AB7" s="10">
         <v>0</v>
       </c>
-      <c r="AC7" s="8">
+      <c r="AC7" s="10">
         <v>0</v>
       </c>
       <c r="AD7" s="8">
@@ -2131,7 +2163,7 @@
       <c r="AF7" s="8">
         <v>0</v>
       </c>
-      <c r="AG7" s="54">
+      <c r="AG7" s="8">
         <v>0</v>
       </c>
       <c r="AH7" s="54">
@@ -2143,8 +2175,11 @@
       <c r="AJ7" s="54">
         <v>0</v>
       </c>
+      <c r="AK7" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
       <c r="B8" s="29" t="s">
         <v>71</v>
@@ -2193,7 +2228,7 @@
         <f t="shared" si="0"/>
         <v>0111</v>
       </c>
-      <c r="R8" s="21">
+      <c r="R8" s="69">
         <v>0</v>
       </c>
       <c r="S8" s="21">
@@ -2203,10 +2238,10 @@
         <v>0</v>
       </c>
       <c r="U8" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8" s="21">
         <v>0</v>
@@ -2226,7 +2261,7 @@
       <c r="AB8" s="21">
         <v>0</v>
       </c>
-      <c r="AC8" s="8">
+      <c r="AC8" s="21">
         <v>0</v>
       </c>
       <c r="AD8" s="8">
@@ -2238,7 +2273,7 @@
       <c r="AF8" s="8">
         <v>0</v>
       </c>
-      <c r="AG8" s="54">
+      <c r="AG8" s="8">
         <v>0</v>
       </c>
       <c r="AH8" s="54">
@@ -2250,8 +2285,11 @@
       <c r="AJ8" s="54">
         <v>0</v>
       </c>
+      <c r="AK8" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28"/>
       <c r="B9" s="29" t="s">
         <v>75</v>
@@ -2300,7 +2338,7 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="R9" s="10">
+      <c r="R9" s="68">
         <v>0</v>
       </c>
       <c r="S9" s="10">
@@ -2310,10 +2348,10 @@
         <v>0</v>
       </c>
       <c r="U9" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V9" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W9" s="10">
         <v>0</v>
@@ -2333,7 +2371,7 @@
       <c r="AB9" s="10">
         <v>0</v>
       </c>
-      <c r="AC9" s="8">
+      <c r="AC9" s="10">
         <v>0</v>
       </c>
       <c r="AD9" s="8">
@@ -2345,7 +2383,7 @@
       <c r="AF9" s="8">
         <v>0</v>
       </c>
-      <c r="AG9" s="54">
+      <c r="AG9" s="8">
         <v>0</v>
       </c>
       <c r="AH9" s="54">
@@ -2357,8 +2395,11 @@
       <c r="AJ9" s="54">
         <v>0</v>
       </c>
+      <c r="AK9" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="28"/>
       <c r="B10" s="29" t="s">
         <v>73</v>
@@ -2407,7 +2448,7 @@
         <f t="shared" si="0"/>
         <v>1001</v>
       </c>
-      <c r="R10" s="21">
+      <c r="R10" s="69">
         <v>0</v>
       </c>
       <c r="S10" s="21">
@@ -2417,10 +2458,10 @@
         <v>0</v>
       </c>
       <c r="U10" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V10" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10" s="21">
         <v>0</v>
@@ -2440,7 +2481,7 @@
       <c r="AB10" s="21">
         <v>0</v>
       </c>
-      <c r="AC10" s="8">
+      <c r="AC10" s="21">
         <v>0</v>
       </c>
       <c r="AD10" s="8">
@@ -2452,7 +2493,7 @@
       <c r="AF10" s="8">
         <v>0</v>
       </c>
-      <c r="AG10" s="54">
+      <c r="AG10" s="8">
         <v>0</v>
       </c>
       <c r="AH10" s="54">
@@ -2464,8 +2505,11 @@
       <c r="AJ10" s="54">
         <v>0</v>
       </c>
+      <c r="AK10" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="28"/>
       <c r="B11" s="29" t="s">
         <v>83</v>
@@ -2514,7 +2558,7 @@
         <f t="shared" si="0"/>
         <v>1010</v>
       </c>
-      <c r="R11" s="31">
+      <c r="R11" s="68">
         <v>0</v>
       </c>
       <c r="S11" s="31">
@@ -2524,10 +2568,10 @@
         <v>0</v>
       </c>
       <c r="U11" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V11" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W11" s="31">
         <v>0</v>
@@ -2547,19 +2591,19 @@
       <c r="AB11" s="31">
         <v>0</v>
       </c>
-      <c r="AC11" s="8">
+      <c r="AC11" s="31">
         <v>0</v>
       </c>
       <c r="AD11" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE11" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF11" s="8">
         <v>0</v>
       </c>
-      <c r="AG11" s="54">
+      <c r="AG11" s="8">
         <v>0</v>
       </c>
       <c r="AH11" s="54">
@@ -2571,8 +2615,11 @@
       <c r="AJ11" s="54">
         <v>0</v>
       </c>
+      <c r="AK11" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="28"/>
       <c r="B12" s="29" t="s">
         <v>87</v>
@@ -2621,7 +2668,7 @@
         <f t="shared" si="0"/>
         <v>1010</v>
       </c>
-      <c r="R12" s="21">
+      <c r="R12" s="69">
         <v>0</v>
       </c>
       <c r="S12" s="21">
@@ -2631,10 +2678,10 @@
         <v>0</v>
       </c>
       <c r="U12" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V12" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W12" s="21">
         <v>0</v>
@@ -2654,19 +2701,19 @@
       <c r="AB12" s="21">
         <v>0</v>
       </c>
-      <c r="AC12" s="8">
+      <c r="AC12" s="21">
         <v>0</v>
       </c>
       <c r="AD12" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE12" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF12" s="8">
         <v>0</v>
       </c>
-      <c r="AG12" s="54">
+      <c r="AG12" s="8">
         <v>0</v>
       </c>
       <c r="AH12" s="54">
@@ -2678,8 +2725,11 @@
       <c r="AJ12" s="54">
         <v>0</v>
       </c>
+      <c r="AK12" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="28"/>
       <c r="B13" s="29" t="s">
         <v>85</v>
@@ -2728,7 +2778,7 @@
         <f t="shared" si="0"/>
         <v>1011</v>
       </c>
-      <c r="R13" s="31">
+      <c r="R13" s="68">
         <v>0</v>
       </c>
       <c r="S13" s="31">
@@ -2738,10 +2788,10 @@
         <v>0</v>
       </c>
       <c r="U13" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V13" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W13" s="31">
         <v>0</v>
@@ -2761,19 +2811,19 @@
       <c r="AB13" s="31">
         <v>0</v>
       </c>
-      <c r="AC13" s="8">
+      <c r="AC13" s="31">
         <v>0</v>
       </c>
       <c r="AD13" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE13" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF13" s="8">
         <v>0</v>
       </c>
-      <c r="AG13" s="54">
+      <c r="AG13" s="8">
         <v>0</v>
       </c>
       <c r="AH13" s="54">
@@ -2785,8 +2835,11 @@
       <c r="AJ13" s="54">
         <v>0</v>
       </c>
+      <c r="AK13" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:36" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="28"/>
       <c r="B14" s="29" t="s">
         <v>89</v>
@@ -2835,7 +2888,7 @@
         <f t="shared" si="0"/>
         <v>1011</v>
       </c>
-      <c r="R14" s="21">
+      <c r="R14" s="69">
         <v>0</v>
       </c>
       <c r="S14" s="21">
@@ -2845,10 +2898,10 @@
         <v>0</v>
       </c>
       <c r="U14" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V14" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W14" s="21">
         <v>0</v>
@@ -2868,19 +2921,19 @@
       <c r="AB14" s="21">
         <v>0</v>
       </c>
-      <c r="AC14" s="8">
+      <c r="AC14" s="21">
         <v>0</v>
       </c>
       <c r="AD14" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE14" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF14" s="8">
         <v>0</v>
       </c>
-      <c r="AG14" s="54">
+      <c r="AG14" s="8">
         <v>0</v>
       </c>
       <c r="AH14" s="54">
@@ -2892,8 +2945,11 @@
       <c r="AJ14" s="54">
         <v>0</v>
       </c>
+      <c r="AK14" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28"/>
       <c r="B15" s="29" t="s">
         <v>103</v>
@@ -2942,7 +2998,7 @@
         <f t="shared" si="0"/>
         <v>1100</v>
       </c>
-      <c r="R15" s="31">
+      <c r="R15" s="68">
         <v>0</v>
       </c>
       <c r="S15" s="31">
@@ -2952,10 +3008,10 @@
         <v>0</v>
       </c>
       <c r="U15" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V15" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W15" s="31">
         <v>0</v>
@@ -2975,19 +3031,19 @@
       <c r="AB15" s="31">
         <v>0</v>
       </c>
-      <c r="AC15" s="8">
+      <c r="AC15" s="31">
         <v>0</v>
       </c>
       <c r="AD15" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE15" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF15" s="8">
         <v>0</v>
       </c>
-      <c r="AG15" s="54">
+      <c r="AG15" s="8">
         <v>0</v>
       </c>
       <c r="AH15" s="54">
@@ -2999,8 +3055,11 @@
       <c r="AJ15" s="54">
         <v>0</v>
       </c>
+      <c r="AK15" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28"/>
       <c r="B16" s="29" t="s">
         <v>105</v>
@@ -3049,7 +3108,7 @@
         <f t="shared" si="0"/>
         <v>1100</v>
       </c>
-      <c r="R16" s="21">
+      <c r="R16" s="69">
         <v>0</v>
       </c>
       <c r="S16" s="21">
@@ -3059,10 +3118,10 @@
         <v>0</v>
       </c>
       <c r="U16" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V16" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W16" s="21">
         <v>0</v>
@@ -3082,19 +3141,19 @@
       <c r="AB16" s="21">
         <v>0</v>
       </c>
-      <c r="AC16" s="8">
+      <c r="AC16" s="21">
         <v>0</v>
       </c>
       <c r="AD16" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE16" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF16" s="8">
         <v>0</v>
       </c>
-      <c r="AG16" s="54">
+      <c r="AG16" s="8">
         <v>0</v>
       </c>
       <c r="AH16" s="54">
@@ -3106,8 +3165,11 @@
       <c r="AJ16" s="54">
         <v>0</v>
       </c>
+      <c r="AK16" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28"/>
       <c r="B17" s="29" t="s">
         <v>101</v>
@@ -3156,7 +3218,7 @@
         <f t="shared" si="0"/>
         <v>1101</v>
       </c>
-      <c r="R17" s="31">
+      <c r="R17" s="68">
         <v>0</v>
       </c>
       <c r="S17" s="31">
@@ -3166,10 +3228,10 @@
         <v>0</v>
       </c>
       <c r="U17" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V17" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W17" s="31">
         <v>0</v>
@@ -3189,19 +3251,19 @@
       <c r="AB17" s="31">
         <v>0</v>
       </c>
-      <c r="AC17" s="8">
+      <c r="AC17" s="31">
         <v>0</v>
       </c>
       <c r="AD17" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE17" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF17" s="8">
         <v>0</v>
       </c>
-      <c r="AG17" s="54">
+      <c r="AG17" s="8">
         <v>0</v>
       </c>
       <c r="AH17" s="54">
@@ -3213,8 +3275,11 @@
       <c r="AJ17" s="54">
         <v>0</v>
       </c>
+      <c r="AK17" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="28"/>
       <c r="B18" s="29" t="s">
         <v>99</v>
@@ -3263,7 +3328,7 @@
         <f t="shared" si="0"/>
         <v>1101</v>
       </c>
-      <c r="R18" s="21">
+      <c r="R18" s="69">
         <v>0</v>
       </c>
       <c r="S18" s="21">
@@ -3273,10 +3338,10 @@
         <v>0</v>
       </c>
       <c r="U18" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V18" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W18" s="21">
         <v>0</v>
@@ -3296,19 +3361,19 @@
       <c r="AB18" s="21">
         <v>0</v>
       </c>
-      <c r="AC18" s="8">
+      <c r="AC18" s="21">
         <v>0</v>
       </c>
       <c r="AD18" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE18" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF18" s="8">
         <v>0</v>
       </c>
-      <c r="AG18" s="54">
+      <c r="AG18" s="8">
         <v>0</v>
       </c>
       <c r="AH18" s="54">
@@ -3320,8 +3385,11 @@
       <c r="AJ18" s="54">
         <v>0</v>
       </c>
+      <c r="AK18" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="28"/>
       <c r="B19" s="29" t="s">
         <v>91</v>
@@ -3370,7 +3438,7 @@
         <f t="shared" si="0"/>
         <v>1110</v>
       </c>
-      <c r="R19" s="31">
+      <c r="R19" s="68">
         <v>0</v>
       </c>
       <c r="S19" s="31">
@@ -3380,10 +3448,10 @@
         <v>0</v>
       </c>
       <c r="U19" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V19" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W19" s="31">
         <v>0</v>
@@ -3403,7 +3471,7 @@
       <c r="AB19" s="31">
         <v>0</v>
       </c>
-      <c r="AC19" s="8">
+      <c r="AC19" s="31">
         <v>0</v>
       </c>
       <c r="AD19" s="8">
@@ -3415,7 +3483,7 @@
       <c r="AF19" s="8">
         <v>0</v>
       </c>
-      <c r="AG19" s="54">
+      <c r="AG19" s="8">
         <v>0</v>
       </c>
       <c r="AH19" s="54">
@@ -3427,8 +3495,11 @@
       <c r="AJ19" s="54">
         <v>0</v>
       </c>
+      <c r="AK19" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28"/>
       <c r="B20" s="29" t="s">
         <v>111</v>
@@ -3477,7 +3548,7 @@
         <f t="shared" si="0"/>
         <v>1111</v>
       </c>
-      <c r="R20" s="21">
+      <c r="R20" s="69">
         <v>0</v>
       </c>
       <c r="S20" s="21">
@@ -3487,10 +3558,10 @@
         <v>0</v>
       </c>
       <c r="U20" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V20" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20" s="21">
         <v>0</v>
@@ -3510,7 +3581,7 @@
       <c r="AB20" s="21">
         <v>0</v>
       </c>
-      <c r="AC20" s="8">
+      <c r="AC20" s="21">
         <v>0</v>
       </c>
       <c r="AD20" s="8">
@@ -3522,7 +3593,7 @@
       <c r="AF20" s="8">
         <v>0</v>
       </c>
-      <c r="AG20" s="54">
+      <c r="AG20" s="8">
         <v>0</v>
       </c>
       <c r="AH20" s="54">
@@ -3534,8 +3605,11 @@
       <c r="AJ20" s="54">
         <v>0</v>
       </c>
+      <c r="AK20" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="34"/>
       <c r="B21" s="35" t="s">
         <v>62</v>
@@ -3579,10 +3653,10 @@
       <c r="Q21" s="60" t="s">
         <v>212</v>
       </c>
-      <c r="R21" s="26">
-        <v>0</v>
-      </c>
-      <c r="S21" s="10">
+      <c r="R21" s="68">
+        <v>0</v>
+      </c>
+      <c r="S21" s="26">
         <v>0</v>
       </c>
       <c r="T21" s="10">
@@ -3591,8 +3665,8 @@
       <c r="U21" s="10">
         <v>0</v>
       </c>
-      <c r="V21" s="57" t="s">
-        <v>203</v>
+      <c r="V21" s="10">
+        <v>0</v>
       </c>
       <c r="W21" s="57" t="s">
         <v>203</v>
@@ -3612,7 +3686,7 @@
       <c r="AB21" s="57" t="s">
         <v>203</v>
       </c>
-      <c r="AC21" s="61" t="s">
+      <c r="AC21" s="57" t="s">
         <v>203</v>
       </c>
       <c r="AD21" s="61" t="s">
@@ -3633,11 +3707,14 @@
       <c r="AI21" s="61" t="s">
         <v>203</v>
       </c>
-      <c r="AJ21" s="54">
+      <c r="AJ21" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="AK21" s="54">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="28"/>
       <c r="B22" s="29" t="s">
         <v>97</v>
@@ -3686,7 +3763,7 @@
         <f>K22</f>
         <v>0</v>
       </c>
-      <c r="R22" s="38">
+      <c r="R22" s="69">
         <v>0</v>
       </c>
       <c r="S22" s="38">
@@ -3696,10 +3773,10 @@
         <v>0</v>
       </c>
       <c r="U22" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V22" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W22" s="38">
         <v>0</v>
@@ -3719,11 +3796,11 @@
       <c r="AB22" s="38">
         <v>0</v>
       </c>
-      <c r="AC22" s="41">
-        <v>1</v>
-      </c>
-      <c r="AD22" s="8">
-        <v>0</v>
+      <c r="AC22" s="38">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="41">
+        <v>1</v>
       </c>
       <c r="AE22" s="8">
         <v>0</v>
@@ -3731,7 +3808,7 @@
       <c r="AF22" s="8">
         <v>0</v>
       </c>
-      <c r="AG22" s="54">
+      <c r="AG22" s="8">
         <v>0</v>
       </c>
       <c r="AH22" s="54">
@@ -3743,8 +3820,11 @@
       <c r="AJ22" s="54">
         <v>0</v>
       </c>
+      <c r="AK22" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="28"/>
       <c r="B23" s="29" t="s">
         <v>95</v>
@@ -3793,7 +3873,7 @@
         <f>K23</f>
         <v>0</v>
       </c>
-      <c r="R23" s="10">
+      <c r="R23" s="68">
         <v>0</v>
       </c>
       <c r="S23" s="10">
@@ -3826,11 +3906,11 @@
       <c r="AB23" s="10">
         <v>0</v>
       </c>
-      <c r="AC23" s="8">
-        <v>1</v>
+      <c r="AC23" s="10">
+        <v>0</v>
       </c>
       <c r="AD23" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE23" s="8">
         <v>0</v>
@@ -3838,7 +3918,7 @@
       <c r="AF23" s="8">
         <v>0</v>
       </c>
-      <c r="AG23" s="54">
+      <c r="AG23" s="8">
         <v>0</v>
       </c>
       <c r="AH23" s="54">
@@ -3850,8 +3930,11 @@
       <c r="AJ23" s="54">
         <v>0</v>
       </c>
+      <c r="AK23" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="43"/>
       <c r="B24" s="44" t="s">
         <v>41</v>
@@ -3895,7 +3978,7 @@
       <c r="Q24" s="40">
         <v>100</v>
       </c>
-      <c r="R24" s="38">
+      <c r="R24" s="69">
         <v>0</v>
       </c>
       <c r="S24" s="38">
@@ -3905,22 +3988,22 @@
         <v>0</v>
       </c>
       <c r="U24" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V24" s="38">
         <v>1</v>
       </c>
       <c r="W24" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X24" s="38">
         <v>0</v>
       </c>
       <c r="Y24" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z24" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA24" s="38">
         <v>0</v>
@@ -3928,7 +4011,7 @@
       <c r="AB24" s="38">
         <v>0</v>
       </c>
-      <c r="AC24" s="8">
+      <c r="AC24" s="38">
         <v>0</v>
       </c>
       <c r="AD24" s="8">
@@ -3940,7 +4023,7 @@
       <c r="AF24" s="8">
         <v>0</v>
       </c>
-      <c r="AG24" s="54">
+      <c r="AG24" s="8">
         <v>0</v>
       </c>
       <c r="AH24" s="54">
@@ -3952,8 +4035,11 @@
       <c r="AJ24" s="54">
         <v>0</v>
       </c>
+      <c r="AK24" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="43"/>
       <c r="B25" s="44" t="s">
         <v>37</v>
@@ -3997,7 +4083,7 @@
       <c r="Q25" s="42">
         <v>100</v>
       </c>
-      <c r="R25" s="10">
+      <c r="R25" s="68">
         <v>0</v>
       </c>
       <c r="S25" s="10">
@@ -4013,24 +4099,24 @@
         <v>0</v>
       </c>
       <c r="W25" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X25" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y25" s="10">
         <v>0</v>
       </c>
       <c r="Z25" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA25" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB25" s="10">
         <v>0</v>
       </c>
-      <c r="AC25" s="8">
+      <c r="AC25" s="10">
         <v>0</v>
       </c>
       <c r="AD25" s="8">
@@ -4042,7 +4128,7 @@
       <c r="AF25" s="8">
         <v>0</v>
       </c>
-      <c r="AG25" s="54">
+      <c r="AG25" s="8">
         <v>0</v>
       </c>
       <c r="AH25" s="54">
@@ -4054,8 +4140,11 @@
       <c r="AJ25" s="54">
         <v>0</v>
       </c>
+      <c r="AK25" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="43"/>
       <c r="B26" s="44" t="s">
         <v>43</v>
@@ -4099,7 +4188,7 @@
       <c r="Q26" s="40">
         <v>100</v>
       </c>
-      <c r="R26" s="38">
+      <c r="R26" s="69">
         <v>0</v>
       </c>
       <c r="S26" s="38">
@@ -4109,10 +4198,10 @@
         <v>0</v>
       </c>
       <c r="U26" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V26" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W26" s="38">
         <v>0</v>
@@ -4127,12 +4216,12 @@
         <v>0</v>
       </c>
       <c r="AA26" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB26" s="38">
-        <v>0</v>
-      </c>
-      <c r="AC26" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="38">
         <v>0</v>
       </c>
       <c r="AD26" s="8">
@@ -4144,7 +4233,7 @@
       <c r="AF26" s="8">
         <v>0</v>
       </c>
-      <c r="AG26" s="54">
+      <c r="AG26" s="8">
         <v>0</v>
       </c>
       <c r="AH26" s="54">
@@ -4156,8 +4245,11 @@
       <c r="AJ26" s="54">
         <v>0</v>
       </c>
+      <c r="AK26" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="43"/>
       <c r="B27" s="44" t="s">
         <v>39</v>
@@ -4201,7 +4293,7 @@
       <c r="Q27" s="42">
         <v>100</v>
       </c>
-      <c r="R27" s="10">
+      <c r="R27" s="68">
         <v>0</v>
       </c>
       <c r="S27" s="10">
@@ -4220,10 +4312,10 @@
         <v>0</v>
       </c>
       <c r="X27" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y27" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z27" s="10">
         <v>0</v>
@@ -4232,10 +4324,10 @@
         <v>0</v>
       </c>
       <c r="AB27" s="10">
-        <v>1</v>
-      </c>
-      <c r="AC27" s="8">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AC27" s="10">
+        <v>1</v>
       </c>
       <c r="AD27" s="8">
         <v>0</v>
@@ -4246,7 +4338,7 @@
       <c r="AF27" s="8">
         <v>0</v>
       </c>
-      <c r="AG27" s="54">
+      <c r="AG27" s="8">
         <v>0</v>
       </c>
       <c r="AH27" s="54">
@@ -4258,8 +4350,11 @@
       <c r="AJ27" s="54">
         <v>0</v>
       </c>
+      <c r="AK27" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="34" t="s">
         <v>47</v>
       </c>
@@ -4290,26 +4385,68 @@
         <v>175</v>
       </c>
       <c r="L28" s="19"/>
-      <c r="M28" s="32"/>
-      <c r="N28" s="38"/>
-      <c r="O28" s="46"/>
-      <c r="P28" s="38"/>
+      <c r="M28" s="32">
+        <v>0</v>
+      </c>
+      <c r="N28" s="38">
+        <v>1</v>
+      </c>
+      <c r="O28" s="46">
+        <v>10</v>
+      </c>
+      <c r="P28" s="56" t="s">
+        <v>203</v>
+      </c>
       <c r="Q28" s="33" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
-      <c r="R28" s="38"/>
-      <c r="S28" s="38"/>
-      <c r="T28" s="38"/>
-      <c r="U28" s="38"/>
-      <c r="V28" s="38"/>
-      <c r="W28" s="38"/>
-      <c r="X28" s="38"/>
-      <c r="Y28" s="38"/>
-      <c r="Z28" s="38"/>
-      <c r="AA28" s="38"/>
-      <c r="AB28" s="38"/>
-      <c r="AG28" s="54">
+      <c r="R28" s="69">
+        <v>11</v>
+      </c>
+      <c r="S28" s="38">
+        <v>0</v>
+      </c>
+      <c r="T28" s="38">
+        <v>0</v>
+      </c>
+      <c r="U28" s="38">
+        <v>0</v>
+      </c>
+      <c r="V28" s="38">
+        <v>0</v>
+      </c>
+      <c r="W28" s="38">
+        <v>0</v>
+      </c>
+      <c r="X28" s="38">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="38">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="38">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="38">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="38">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="38">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="70">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="70">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="70">
+        <v>0</v>
+      </c>
+      <c r="AG28" s="70">
         <v>0</v>
       </c>
       <c r="AH28" s="54">
@@ -4321,8 +4458,11 @@
       <c r="AJ28" s="54">
         <v>0</v>
       </c>
+      <c r="AK28" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="34"/>
       <c r="B29" s="35" t="s">
         <v>58</v>
@@ -4351,11 +4491,68 @@
         <v>175</v>
       </c>
       <c r="L29" s="19"/>
+      <c r="M29" s="9">
+        <v>0</v>
+      </c>
+      <c r="N29" s="10">
+        <v>1</v>
+      </c>
+      <c r="O29" s="11">
+        <v>10</v>
+      </c>
+      <c r="P29" s="57" t="s">
+        <v>203</v>
+      </c>
       <c r="Q29" s="25" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
-      <c r="AG29" s="54">
+      <c r="R29" s="68">
+        <v>0</v>
+      </c>
+      <c r="S29" s="10">
+        <v>0</v>
+      </c>
+      <c r="T29" s="10">
+        <v>0</v>
+      </c>
+      <c r="U29" s="10">
+        <v>0</v>
+      </c>
+      <c r="V29" s="10">
+        <v>0</v>
+      </c>
+      <c r="W29" s="10">
+        <v>0</v>
+      </c>
+      <c r="X29" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="71">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="71">
+        <v>0</v>
+      </c>
+      <c r="AF29" s="71">
+        <v>0</v>
+      </c>
+      <c r="AG29" s="71">
         <v>0</v>
       </c>
       <c r="AH29" s="54">
@@ -4367,8 +4564,11 @@
       <c r="AJ29" s="54">
         <v>0</v>
       </c>
+      <c r="AK29" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="34"/>
       <c r="B30" s="35" t="s">
         <v>60</v>
@@ -4412,12 +4612,11 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="R30" s="50">
-        <f t="shared" ref="R30:AA30" si="2">R21</f>
+      <c r="R30" s="69">
         <v>0</v>
       </c>
       <c r="S30" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="S30:AB30" si="2">S21</f>
         <v>0</v>
       </c>
       <c r="T30" s="50">
@@ -4428,9 +4627,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="V30" s="50" t="str">
+      <c r="V30" s="50">
         <f t="shared" si="2"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="W30" s="50" t="str">
         <f t="shared" si="2"/>
@@ -4453,11 +4652,12 @@
         <v>X</v>
       </c>
       <c r="AB30" s="50" t="str">
-        <f>AB21</f>
+        <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="AC30" s="61" t="s">
-        <v>203</v>
+      <c r="AC30" s="50" t="str">
+        <f>AC21</f>
+        <v>X</v>
       </c>
       <c r="AD30" s="61" t="s">
         <v>203</v>
@@ -4477,11 +4677,14 @@
       <c r="AI30" s="61" t="s">
         <v>203</v>
       </c>
-      <c r="AJ30" s="54">
+      <c r="AJ30" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="AK30" s="54">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="34"/>
       <c r="B31" s="35" t="s">
         <v>64</v>
@@ -4523,7 +4726,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="R31" s="10">
+      <c r="R31" s="68">
         <v>0</v>
       </c>
       <c r="S31" s="10">
@@ -4533,10 +4736,10 @@
         <v>0</v>
       </c>
       <c r="U31" s="10">
-        <v>1</v>
-      </c>
-      <c r="V31" s="57" t="s">
-        <v>203</v>
+        <v>0</v>
+      </c>
+      <c r="V31" s="10">
+        <v>1</v>
       </c>
       <c r="W31" s="57" t="s">
         <v>203</v>
@@ -4556,10 +4759,10 @@
       <c r="AB31" s="57" t="s">
         <v>203</v>
       </c>
-      <c r="AC31" s="64" t="s">
+      <c r="AC31" s="57" t="s">
         <v>203</v>
       </c>
-      <c r="AD31" s="65" t="s">
+      <c r="AD31" s="64" t="s">
         <v>203</v>
       </c>
       <c r="AE31" s="65" t="s">
@@ -4577,11 +4780,14 @@
       <c r="AI31" s="65" t="s">
         <v>203</v>
       </c>
-      <c r="AJ31" s="54">
+      <c r="AJ31" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="AK31" s="54">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="35"/>
       <c r="B32" s="35" t="s">
         <v>50</v>
@@ -4610,26 +4816,68 @@
         <v>175</v>
       </c>
       <c r="L32" s="19"/>
-      <c r="M32" s="32"/>
-      <c r="N32" s="38"/>
-      <c r="O32" s="46"/>
-      <c r="P32" s="38"/>
+      <c r="M32" s="32">
+        <v>0</v>
+      </c>
+      <c r="N32" s="38">
+        <v>1</v>
+      </c>
+      <c r="O32" s="46">
+        <v>1</v>
+      </c>
+      <c r="P32" s="56" t="s">
+        <v>203</v>
+      </c>
       <c r="Q32" s="33" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
-      <c r="R32" s="38"/>
-      <c r="S32" s="38"/>
-      <c r="T32" s="38"/>
-      <c r="U32" s="38"/>
-      <c r="V32" s="38"/>
-      <c r="W32" s="38"/>
-      <c r="X32" s="38"/>
-      <c r="Y32" s="38"/>
-      <c r="Z32" s="38"/>
-      <c r="AA32" s="38"/>
-      <c r="AB32" s="38"/>
-      <c r="AG32" s="54">
+      <c r="R32" s="69">
+        <v>101</v>
+      </c>
+      <c r="S32" s="38">
+        <v>0</v>
+      </c>
+      <c r="T32" s="38">
+        <v>0</v>
+      </c>
+      <c r="U32" s="38">
+        <v>0</v>
+      </c>
+      <c r="V32" s="38">
+        <v>0</v>
+      </c>
+      <c r="W32" s="38">
+        <v>0</v>
+      </c>
+      <c r="X32" s="38">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="38">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="38">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="38">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="38">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="38">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="70">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="70">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="70">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="70">
         <v>0</v>
       </c>
       <c r="AH32" s="54">
@@ -4641,8 +4889,11 @@
       <c r="AJ32" s="54">
         <v>0</v>
       </c>
+      <c r="AK32" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="35"/>
       <c r="B33" s="35" t="s">
         <v>52</v>
@@ -4671,11 +4922,68 @@
         <v>175</v>
       </c>
       <c r="L33" s="19"/>
+      <c r="M33" s="9">
+        <v>0</v>
+      </c>
+      <c r="N33" s="10">
+        <v>1</v>
+      </c>
+      <c r="O33" s="11">
+        <v>1</v>
+      </c>
+      <c r="P33" s="57" t="s">
+        <v>203</v>
+      </c>
       <c r="Q33" s="25" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
-      <c r="AG33" s="54">
+      <c r="R33" s="68">
+        <v>100</v>
+      </c>
+      <c r="S33" s="10">
+        <v>0</v>
+      </c>
+      <c r="T33" s="10">
+        <v>0</v>
+      </c>
+      <c r="U33" s="10">
+        <v>0</v>
+      </c>
+      <c r="V33" s="10">
+        <v>0</v>
+      </c>
+      <c r="W33" s="10">
+        <v>0</v>
+      </c>
+      <c r="X33" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="71">
+        <v>0</v>
+      </c>
+      <c r="AE33" s="71">
+        <v>0</v>
+      </c>
+      <c r="AF33" s="71">
+        <v>0</v>
+      </c>
+      <c r="AG33" s="71">
         <v>0</v>
       </c>
       <c r="AH33" s="54">
@@ -4687,8 +4995,11 @@
       <c r="AJ33" s="54">
         <v>0</v>
       </c>
+      <c r="AK33" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="35"/>
       <c r="B34" s="35" t="s">
         <v>56</v>
@@ -4717,26 +5028,68 @@
         <v>175</v>
       </c>
       <c r="L34" s="19"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="38"/>
-      <c r="O34" s="46"/>
-      <c r="P34" s="38"/>
+      <c r="M34" s="32">
+        <v>0</v>
+      </c>
+      <c r="N34" s="38">
+        <v>1</v>
+      </c>
+      <c r="O34" s="46">
+        <v>10</v>
+      </c>
+      <c r="P34" s="56" t="s">
+        <v>203</v>
+      </c>
       <c r="Q34" s="33" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
-      <c r="R34" s="38"/>
-      <c r="S34" s="38"/>
-      <c r="T34" s="38"/>
-      <c r="U34" s="38"/>
-      <c r="V34" s="38"/>
-      <c r="W34" s="38"/>
-      <c r="X34" s="38"/>
-      <c r="Y34" s="38"/>
-      <c r="Z34" s="38"/>
-      <c r="AA34" s="38"/>
-      <c r="AB34" s="38"/>
-      <c r="AG34" s="54">
+      <c r="R34" s="69">
+        <v>1</v>
+      </c>
+      <c r="S34" s="38">
+        <v>0</v>
+      </c>
+      <c r="T34" s="38">
+        <v>0</v>
+      </c>
+      <c r="U34" s="38">
+        <v>0</v>
+      </c>
+      <c r="V34" s="38">
+        <v>0</v>
+      </c>
+      <c r="W34" s="38">
+        <v>0</v>
+      </c>
+      <c r="X34" s="38">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="38">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="38">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="38">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="38">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="38">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="70">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="70">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="70">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="70">
         <v>0</v>
       </c>
       <c r="AH34" s="54">
@@ -4748,8 +5101,11 @@
       <c r="AJ34" s="54">
         <v>0</v>
       </c>
+      <c r="AK34" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="35"/>
       <c r="B35" s="35" t="s">
         <v>54</v>
@@ -4778,11 +5134,68 @@
         <v>175</v>
       </c>
       <c r="L35" s="19"/>
+      <c r="M35" s="9">
+        <v>0</v>
+      </c>
+      <c r="N35" s="10">
+        <v>1</v>
+      </c>
+      <c r="O35" s="11">
+        <v>10</v>
+      </c>
+      <c r="P35" s="57" t="s">
+        <v>203</v>
+      </c>
       <c r="Q35" s="25" t="str">
         <f t="shared" si="0"/>
         <v>0001</v>
       </c>
-      <c r="AG35" s="54">
+      <c r="R35" s="68">
+        <v>10</v>
+      </c>
+      <c r="S35" s="10">
+        <v>0</v>
+      </c>
+      <c r="T35" s="10">
+        <v>0</v>
+      </c>
+      <c r="U35" s="10">
+        <v>0</v>
+      </c>
+      <c r="V35" s="10">
+        <v>0</v>
+      </c>
+      <c r="W35" s="10">
+        <v>0</v>
+      </c>
+      <c r="X35" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="71">
+        <v>0</v>
+      </c>
+      <c r="AE35" s="71">
+        <v>0</v>
+      </c>
+      <c r="AF35" s="71">
+        <v>0</v>
+      </c>
+      <c r="AG35" s="71">
         <v>0</v>
       </c>
       <c r="AH35" s="54">
@@ -4794,8 +5207,11 @@
       <c r="AJ35" s="54">
         <v>0</v>
       </c>
+      <c r="AK35" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="13" t="s">
         <v>10</v>
@@ -4840,7 +5256,7 @@
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R36" s="38">
+      <c r="R36" s="69">
         <v>0</v>
       </c>
       <c r="S36" s="38">
@@ -4850,10 +5266,10 @@
         <v>0</v>
       </c>
       <c r="U36" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V36" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W36" s="38">
         <v>0</v>
@@ -4873,7 +5289,7 @@
       <c r="AB36" s="38">
         <v>0</v>
       </c>
-      <c r="AC36" s="8">
+      <c r="AC36" s="38">
         <v>0</v>
       </c>
       <c r="AD36" s="8">
@@ -4885,7 +5301,7 @@
       <c r="AF36" s="8">
         <v>0</v>
       </c>
-      <c r="AG36" s="54">
+      <c r="AG36" s="8">
         <v>0</v>
       </c>
       <c r="AH36" s="54">
@@ -4897,8 +5313,11 @@
       <c r="AJ36" s="54">
         <v>0</v>
       </c>
+      <c r="AK36" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="13" t="s">
         <v>6</v>
@@ -4943,7 +5362,7 @@
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R37" s="10">
+      <c r="R37" s="68">
         <v>0</v>
       </c>
       <c r="S37" s="10">
@@ -4953,10 +5372,10 @@
         <v>0</v>
       </c>
       <c r="U37" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V37" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W37" s="10">
         <v>0</v>
@@ -4976,7 +5395,7 @@
       <c r="AB37" s="10">
         <v>0</v>
       </c>
-      <c r="AC37" s="8">
+      <c r="AC37" s="10">
         <v>0</v>
       </c>
       <c r="AD37" s="8">
@@ -4988,7 +5407,7 @@
       <c r="AF37" s="8">
         <v>0</v>
       </c>
-      <c r="AG37" s="54">
+      <c r="AG37" s="8">
         <v>0</v>
       </c>
       <c r="AH37" s="54">
@@ -5000,8 +5419,11 @@
       <c r="AJ37" s="54">
         <v>0</v>
       </c>
+      <c r="AK37" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="29"/>
       <c r="B38" s="29" t="s">
         <v>93</v>
@@ -5046,7 +5468,7 @@
         <f t="shared" si="0"/>
         <v>1110</v>
       </c>
-      <c r="R38" s="38">
+      <c r="R38" s="69">
         <v>0</v>
       </c>
       <c r="S38" s="38">
@@ -5056,10 +5478,10 @@
         <v>0</v>
       </c>
       <c r="U38" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V38" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W38" s="38">
         <v>0</v>
@@ -5079,7 +5501,7 @@
       <c r="AB38" s="38">
         <v>0</v>
       </c>
-      <c r="AC38" s="8">
+      <c r="AC38" s="38">
         <v>0</v>
       </c>
       <c r="AD38" s="8">
@@ -5091,7 +5513,7 @@
       <c r="AF38" s="8">
         <v>0</v>
       </c>
-      <c r="AG38" s="54">
+      <c r="AG38" s="8">
         <v>0</v>
       </c>
       <c r="AH38" s="54">
@@ -5103,8 +5525,11 @@
       <c r="AJ38" s="54">
         <v>0</v>
       </c>
+      <c r="AK38" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:36" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:37" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="29"/>
       <c r="B39" s="29" t="s">
         <v>109</v>
@@ -5149,7 +5574,7 @@
         <f t="shared" si="0"/>
         <v>1111</v>
       </c>
-      <c r="R39" s="10">
+      <c r="R39" s="68">
         <v>0</v>
       </c>
       <c r="S39" s="10">
@@ -5159,10 +5584,10 @@
         <v>0</v>
       </c>
       <c r="U39" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V39" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W39" s="10">
         <v>0</v>
@@ -5182,7 +5607,7 @@
       <c r="AB39" s="10">
         <v>0</v>
       </c>
-      <c r="AC39" s="8">
+      <c r="AC39" s="10">
         <v>0</v>
       </c>
       <c r="AD39" s="8">
@@ -5194,7 +5619,7 @@
       <c r="AF39" s="8">
         <v>0</v>
       </c>
-      <c r="AG39" s="54">
+      <c r="AG39" s="8">
         <v>0</v>
       </c>
       <c r="AH39" s="54">
@@ -5206,8 +5631,11 @@
       <c r="AJ39" s="54">
         <v>0</v>
       </c>
+      <c r="AK39" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="29"/>
       <c r="B40" s="29" t="s">
         <v>69</v>
@@ -5252,7 +5680,7 @@
         <f t="shared" si="0"/>
         <v>0110</v>
       </c>
-      <c r="R40" s="38">
+      <c r="R40" s="69">
         <v>0</v>
       </c>
       <c r="S40" s="38">
@@ -5262,10 +5690,10 @@
         <v>0</v>
       </c>
       <c r="U40" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V40" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W40" s="38">
         <v>0</v>
@@ -5288,7 +5716,7 @@
       <c r="AC40" s="38">
         <v>0</v>
       </c>
-      <c r="AD40" s="8">
+      <c r="AD40" s="38">
         <v>0</v>
       </c>
       <c r="AE40" s="8">
@@ -5297,7 +5725,7 @@
       <c r="AF40" s="8">
         <v>0</v>
       </c>
-      <c r="AG40" s="54">
+      <c r="AG40" s="8">
         <v>0</v>
       </c>
       <c r="AH40" s="54">
@@ -5309,8 +5737,11 @@
       <c r="AJ40" s="54">
         <v>0</v>
       </c>
+      <c r="AK40" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="29"/>
       <c r="B41" s="29" t="s">
         <v>77</v>
@@ -5355,7 +5786,7 @@
         <f t="shared" si="0"/>
         <v>0111</v>
       </c>
-      <c r="R41" s="10">
+      <c r="R41" s="68">
         <v>0</v>
       </c>
       <c r="S41" s="10">
@@ -5365,10 +5796,10 @@
         <v>0</v>
       </c>
       <c r="U41" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V41" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W41" s="10">
         <v>0</v>
@@ -5388,10 +5819,10 @@
       <c r="AB41" s="10">
         <v>0</v>
       </c>
-      <c r="AC41" s="48">
-        <v>0</v>
-      </c>
-      <c r="AD41" s="8">
+      <c r="AC41" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD41" s="48">
         <v>0</v>
       </c>
       <c r="AE41" s="8">
@@ -5400,7 +5831,7 @@
       <c r="AF41" s="8">
         <v>0</v>
       </c>
-      <c r="AG41" s="54">
+      <c r="AG41" s="8">
         <v>0</v>
       </c>
       <c r="AH41" s="54">
@@ -5412,8 +5843,11 @@
       <c r="AJ41" s="54">
         <v>0</v>
       </c>
+      <c r="AK41" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="29"/>
       <c r="B42" s="29" t="s">
         <v>79</v>
@@ -5458,7 +5892,7 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="R42" s="38">
+      <c r="R42" s="69">
         <v>0</v>
       </c>
       <c r="S42" s="38">
@@ -5468,10 +5902,10 @@
         <v>0</v>
       </c>
       <c r="U42" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V42" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W42" s="38">
         <v>0</v>
@@ -5491,10 +5925,10 @@
       <c r="AB42" s="38">
         <v>0</v>
       </c>
-      <c r="AC42" s="49">
-        <v>0</v>
-      </c>
-      <c r="AD42" s="8">
+      <c r="AC42" s="38">
+        <v>0</v>
+      </c>
+      <c r="AD42" s="49">
         <v>0</v>
       </c>
       <c r="AE42" s="8">
@@ -5503,7 +5937,7 @@
       <c r="AF42" s="8">
         <v>0</v>
       </c>
-      <c r="AG42" s="54">
+      <c r="AG42" s="8">
         <v>0</v>
       </c>
       <c r="AH42" s="54">
@@ -5515,8 +5949,11 @@
       <c r="AJ42" s="54">
         <v>0</v>
       </c>
+      <c r="AK42" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="44"/>
       <c r="B43" s="44" t="s">
         <v>45</v>
@@ -5560,7 +5997,7 @@
       <c r="Q43" s="52">
         <v>10</v>
       </c>
-      <c r="R43" s="10">
+      <c r="R43" s="68">
         <v>0</v>
       </c>
       <c r="S43" s="10">
@@ -5570,10 +6007,10 @@
         <v>0</v>
       </c>
       <c r="U43" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V43" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W43" s="10">
         <v>0</v>
@@ -5593,7 +6030,7 @@
       <c r="AB43" s="10">
         <v>0</v>
       </c>
-      <c r="AC43" s="53">
+      <c r="AC43" s="10">
         <v>0</v>
       </c>
       <c r="AD43" s="53">
@@ -5605,20 +6042,23 @@
       <c r="AF43" s="53">
         <v>0</v>
       </c>
-      <c r="AG43" s="54">
+      <c r="AG43" s="53">
         <v>0</v>
       </c>
       <c r="AH43" s="54">
         <v>0</v>
       </c>
       <c r="AI43" s="54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ43" s="54">
+        <v>1</v>
+      </c>
+      <c r="AK43" s="54">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13"/>
       <c r="B44" s="13" t="s">
         <v>14</v>
@@ -5667,7 +6107,7 @@
         <f t="shared" si="0"/>
         <v>0010</v>
       </c>
-      <c r="R44" s="38">
+      <c r="R44" s="69">
         <v>0</v>
       </c>
       <c r="S44" s="38">
@@ -5677,10 +6117,10 @@
         <v>0</v>
       </c>
       <c r="U44" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V44" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W44" s="38">
         <v>0</v>
@@ -5703,7 +6143,7 @@
       <c r="AC44" s="38">
         <v>0</v>
       </c>
-      <c r="AD44" s="8">
+      <c r="AD44" s="38">
         <v>0</v>
       </c>
       <c r="AE44" s="8">
@@ -5712,7 +6152,7 @@
       <c r="AF44" s="8">
         <v>0</v>
       </c>
-      <c r="AG44" s="54">
+      <c r="AG44" s="8">
         <v>0</v>
       </c>
       <c r="AH44" s="54">
@@ -5724,8 +6164,11 @@
       <c r="AJ44" s="54">
         <v>0</v>
       </c>
+      <c r="AK44" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13"/>
       <c r="B45" s="13" t="s">
         <v>20</v>
@@ -5774,7 +6217,7 @@
         <f t="shared" si="0"/>
         <v>0100</v>
       </c>
-      <c r="R45" s="10">
+      <c r="R45" s="68">
         <v>0</v>
       </c>
       <c r="S45" s="10">
@@ -5796,7 +6239,7 @@
         <v>0</v>
       </c>
       <c r="Y45" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z45" s="10">
         <v>1</v>
@@ -5807,10 +6250,10 @@
       <c r="AB45" s="10">
         <v>1</v>
       </c>
-      <c r="AC45" s="48">
-        <v>0</v>
-      </c>
-      <c r="AD45" s="8">
+      <c r="AC45" s="10">
+        <v>1</v>
+      </c>
+      <c r="AD45" s="48">
         <v>0</v>
       </c>
       <c r="AE45" s="8">
@@ -5819,7 +6262,7 @@
       <c r="AF45" s="8">
         <v>0</v>
       </c>
-      <c r="AG45" s="54">
+      <c r="AG45" s="8">
         <v>0</v>
       </c>
       <c r="AH45" s="54">
@@ -5831,8 +6274,11 @@
       <c r="AJ45" s="54">
         <v>0</v>
       </c>
+      <c r="AK45" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13"/>
       <c r="B46" s="13" t="s">
         <v>22</v>
@@ -5881,7 +6327,7 @@
         <f t="shared" si="0"/>
         <v>0101</v>
       </c>
-      <c r="R46" s="38">
+      <c r="R46" s="69">
         <v>0</v>
       </c>
       <c r="S46" s="38">
@@ -5903,7 +6349,7 @@
         <v>0</v>
       </c>
       <c r="Y46" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z46" s="38">
         <v>1</v>
@@ -5914,10 +6360,10 @@
       <c r="AB46" s="38">
         <v>1</v>
       </c>
-      <c r="AC46" s="49">
-        <v>0</v>
-      </c>
-      <c r="AD46" s="8">
+      <c r="AC46" s="38">
+        <v>1</v>
+      </c>
+      <c r="AD46" s="49">
         <v>0</v>
       </c>
       <c r="AE46" s="8">
@@ -5926,7 +6372,7 @@
       <c r="AF46" s="8">
         <v>0</v>
       </c>
-      <c r="AG46" s="54">
+      <c r="AG46" s="8">
         <v>0</v>
       </c>
       <c r="AH46" s="54">
@@ -5938,8 +6384,11 @@
       <c r="AJ46" s="54">
         <v>0</v>
       </c>
+      <c r="AK46" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="29"/>
       <c r="B47" s="29" t="s">
         <v>81</v>
@@ -5988,7 +6437,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="R47" s="10">
+      <c r="R47" s="68">
         <v>0</v>
       </c>
       <c r="S47" s="10">
@@ -5998,10 +6447,10 @@
         <v>0</v>
       </c>
       <c r="U47" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V47" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W47" s="10">
         <v>0</v>
@@ -6021,20 +6470,20 @@
       <c r="AB47" s="10">
         <v>0</v>
       </c>
-      <c r="AC47" s="49">
-        <v>0</v>
-      </c>
-      <c r="AD47" s="8">
+      <c r="AC47" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD47" s="49">
         <v>0</v>
       </c>
       <c r="AE47" s="8">
         <v>0</v>
       </c>
       <c r="AF47" s="8">
-        <v>1</v>
-      </c>
-      <c r="AG47" s="54">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AG47" s="8">
+        <v>1</v>
       </c>
       <c r="AH47" s="54">
         <v>0</v>
@@ -6045,8 +6494,11 @@
       <c r="AJ47" s="54">
         <v>0</v>
       </c>
+      <c r="AK47" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="29"/>
       <c r="B48" s="29" t="s">
         <v>107</v>
@@ -6093,7 +6545,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="R48" s="38">
+      <c r="R48" s="69">
         <v>0</v>
       </c>
       <c r="S48" s="38">
@@ -6103,10 +6555,10 @@
         <v>0</v>
       </c>
       <c r="U48" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V48" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W48" s="38">
         <v>0</v>
@@ -6126,20 +6578,20 @@
       <c r="AB48" s="38">
         <v>0</v>
       </c>
-      <c r="AC48" s="49">
-        <v>0</v>
-      </c>
-      <c r="AD48" s="8">
+      <c r="AC48" s="38">
+        <v>0</v>
+      </c>
+      <c r="AD48" s="49">
         <v>0</v>
       </c>
       <c r="AE48" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF48" s="8">
         <v>1</v>
       </c>
-      <c r="AG48" s="54">
-        <v>0</v>
+      <c r="AG48" s="8">
+        <v>1</v>
       </c>
       <c r="AH48" s="54">
         <v>0</v>
@@ -6150,8 +6602,11 @@
       <c r="AJ48" s="54">
         <v>0</v>
       </c>
+      <c r="AK48" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="44"/>
       <c r="B49" s="44" t="s">
         <v>33</v>
@@ -6196,11 +6651,11 @@
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R49" s="10">
+      <c r="R49" s="68">
         <v>0</v>
       </c>
       <c r="S49" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T49" s="10">
         <v>1</v>
@@ -6209,7 +6664,7 @@
         <v>1</v>
       </c>
       <c r="V49" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W49" s="10">
         <v>0</v>
@@ -6229,7 +6684,7 @@
       <c r="AB49" s="10">
         <v>0</v>
       </c>
-      <c r="AC49" s="53">
+      <c r="AC49" s="10">
         <v>0</v>
       </c>
       <c r="AD49" s="53">
@@ -6242,19 +6697,22 @@
         <v>0</v>
       </c>
       <c r="AG49" s="53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH49" s="53">
-        <v>0</v>
-      </c>
-      <c r="AI49" s="54">
+        <v>1</v>
+      </c>
+      <c r="AI49" s="53">
         <v>0</v>
       </c>
       <c r="AJ49" s="54">
         <v>0</v>
       </c>
+      <c r="AK49" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="44"/>
       <c r="B50" s="44" t="s">
         <v>31</v>
@@ -6299,11 +6757,11 @@
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R50" s="38">
+      <c r="R50" s="69">
         <v>0</v>
       </c>
       <c r="S50" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T50" s="38">
         <v>1</v>
@@ -6312,7 +6770,7 @@
         <v>1</v>
       </c>
       <c r="V50" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W50" s="38">
         <v>0</v>
@@ -6332,10 +6790,10 @@
       <c r="AB50" s="38">
         <v>0</v>
       </c>
-      <c r="AC50" s="53">
-        <v>0</v>
-      </c>
-      <c r="AD50" s="55">
+      <c r="AC50" s="38">
+        <v>0</v>
+      </c>
+      <c r="AD50" s="53">
         <v>0</v>
       </c>
       <c r="AE50" s="55">
@@ -6344,20 +6802,23 @@
       <c r="AF50" s="55">
         <v>0</v>
       </c>
-      <c r="AG50" s="54">
+      <c r="AG50" s="55">
         <v>0</v>
       </c>
       <c r="AH50" s="54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI50" s="54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ50" s="54">
         <v>0</v>
       </c>
+      <c r="AK50" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="44" t="s">
         <v>24</v>
       </c>
@@ -6404,11 +6865,11 @@
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R51" s="10">
+      <c r="R51" s="68">
         <v>0</v>
       </c>
       <c r="S51" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T51" s="10">
         <v>1</v>
@@ -6417,7 +6878,7 @@
         <v>1</v>
       </c>
       <c r="V51" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W51" s="10">
         <v>0</v>
@@ -6437,7 +6898,7 @@
       <c r="AB51" s="10">
         <v>0</v>
       </c>
-      <c r="AC51" s="53">
+      <c r="AC51" s="10">
         <v>0</v>
       </c>
       <c r="AD51" s="53">
@@ -6449,7 +6910,7 @@
       <c r="AF51" s="53">
         <v>0</v>
       </c>
-      <c r="AG51" s="54">
+      <c r="AG51" s="53">
         <v>0</v>
       </c>
       <c r="AH51" s="54">
@@ -6461,8 +6922,11 @@
       <c r="AJ51" s="54">
         <v>0</v>
       </c>
+      <c r="AK51" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="44"/>
       <c r="B52" s="44" t="s">
         <v>29</v>
@@ -6507,11 +6971,11 @@
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R52" s="38">
-        <v>1</v>
+      <c r="R52" s="69">
+        <v>0</v>
       </c>
       <c r="S52" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T52" s="38">
         <v>0</v>
@@ -6540,10 +7004,10 @@
       <c r="AB52" s="38">
         <v>0</v>
       </c>
-      <c r="AC52" s="53">
-        <v>0</v>
-      </c>
-      <c r="AD52" s="55">
+      <c r="AC52" s="38">
+        <v>0</v>
+      </c>
+      <c r="AD52" s="53">
         <v>0</v>
       </c>
       <c r="AE52" s="55">
@@ -6553,19 +7017,22 @@
         <v>0</v>
       </c>
       <c r="AG52" s="55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH52" s="55">
-        <v>0</v>
-      </c>
-      <c r="AI52" s="54">
+        <v>1</v>
+      </c>
+      <c r="AI52" s="55">
         <v>0</v>
       </c>
       <c r="AJ52" s="54">
         <v>0</v>
       </c>
+      <c r="AK52" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="44"/>
       <c r="B53" s="44" t="s">
         <v>35</v>
@@ -6610,11 +7077,11 @@
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R53" s="10">
-        <v>1</v>
+      <c r="R53" s="68">
+        <v>0</v>
       </c>
       <c r="S53" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T53" s="10">
         <v>0</v>
@@ -6643,7 +7110,7 @@
       <c r="AB53" s="10">
         <v>0</v>
       </c>
-      <c r="AC53" s="53">
+      <c r="AC53" s="10">
         <v>0</v>
       </c>
       <c r="AD53" s="53">
@@ -6659,16 +7126,19 @@
         <v>0</v>
       </c>
       <c r="AH53" s="53">
-        <v>1</v>
-      </c>
-      <c r="AI53" s="54">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AI53" s="53">
+        <v>1</v>
       </c>
       <c r="AJ53" s="54">
         <v>0</v>
       </c>
+      <c r="AK53" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="44"/>
       <c r="B54" s="44" t="s">
         <v>27</v>
@@ -6713,11 +7183,11 @@
         <f t="shared" si="0"/>
         <v>0000</v>
       </c>
-      <c r="R54" s="38">
-        <v>1</v>
+      <c r="R54" s="69">
+        <v>0</v>
       </c>
       <c r="S54" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T54" s="38">
         <v>0</v>
@@ -6746,10 +7216,10 @@
       <c r="AB54" s="38">
         <v>0</v>
       </c>
-      <c r="AC54" s="53">
-        <v>0</v>
-      </c>
-      <c r="AD54" s="55">
+      <c r="AC54" s="38">
+        <v>0</v>
+      </c>
+      <c r="AD54" s="53">
         <v>0</v>
       </c>
       <c r="AE54" s="55">
@@ -6764,14 +7234,17 @@
       <c r="AH54" s="55">
         <v>0</v>
       </c>
-      <c r="AI54" s="54">
+      <c r="AI54" s="55">
         <v>0</v>
       </c>
       <c r="AJ54" s="54">
         <v>0</v>
       </c>
+      <c r="AK54" s="54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="D55" s="51"/>
       <c r="E55" s="51"/>
       <c r="F55" s="51"/>

</xml_diff>